<commit_message>
Submit the "Is a solar future inevitable version"
This is the model version used for the Nature Communications paper "Is a solar future inevitable".
</commit_message>
<xml_diff>
--- a/Inputs/_MasterFiles/FTT_variables.xlsx
+++ b/Inputs/_MasterFiles/FTT_variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\E3ME\FTT_Stand_Alone\Inputs\_MasterFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6AAC6B1-6F73-4CBC-BFCC-308507F8D1EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B6D1F64-B99B-4AD8-9104-76A345471C80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7500" yWindow="-16395" windowWidth="29190" windowHeight="15990" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FTT-P" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'FTT-P'!$A$1:$G$19</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'FTT-Tr'!$A$1:$G$1</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="284">
   <si>
     <t>Variable name</t>
   </si>
@@ -894,18 +894,6 @@
   </si>
   <si>
     <t>tl_2018</t>
-  </si>
-  <si>
-    <t>ZCEZ</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>Costs (Column 64)</t>
-  </si>
-  <si>
-    <t>FTT-Fr T-Scaling</t>
   </si>
 </sst>
 </file>
@@ -1254,7 +1242,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3270,10 +3258,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85BB7FF7-82D6-482E-815B-F3751454FF7D}">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3320,7 +3308,7 @@
         <v>189</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>35330000</v>
@@ -3349,7 +3337,7 @@
         <v>192</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>35320000</v>
@@ -3378,7 +3366,7 @@
         <v>223</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4">
         <v>35060000</v>
@@ -3407,7 +3395,7 @@
         <v>198</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <v>35070000</v>
@@ -3436,7 +3424,7 @@
         <v>201</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6">
         <v>35140000</v>
@@ -3465,7 +3453,7 @@
         <v>222</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7">
         <v>35040000</v>
@@ -3494,7 +3482,7 @@
         <v>224</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8">
         <v>35050000</v>
@@ -3523,7 +3511,7 @@
         <v>225</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9">
         <v>35020000</v>
@@ -3552,7 +3540,7 @@
         <v>226</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10">
         <v>35030000</v>
@@ -3581,7 +3569,7 @@
         <v>227</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11">
         <v>35150000</v>
@@ -3610,7 +3598,7 @@
         <v>228</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12">
         <v>35130000</v>
@@ -3639,7 +3627,7 @@
         <v>218</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13">
         <v>35140000</v>
@@ -3668,7 +3656,7 @@
         <v>232</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14">
         <v>35210000</v>
@@ -3694,7 +3682,7 @@
         <v>234</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15">
         <v>35220000</v>
@@ -3778,7 +3766,7 @@
         <v>245</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18" s="3">
         <v>35340000</v>
@@ -3807,7 +3795,7 @@
         <v>251</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19" s="3">
         <v>35350000</v>
@@ -3836,7 +3824,7 @@
         <v>253</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20">
         <v>35190000</v>
@@ -3865,7 +3853,7 @@
         <v>257</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21">
         <v>35200000</v>
@@ -3894,7 +3882,7 @@
         <v>261</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" s="3">
         <v>35360000</v>
@@ -3923,7 +3911,7 @@
         <v>267</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23" s="3">
         <v>35370000</v>
@@ -3952,7 +3940,7 @@
         <v>273</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C24" s="3">
         <v>35380000</v>
@@ -4010,7 +3998,7 @@
         <v>279</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C26" s="3">
         <v>35390000</v>
@@ -4032,35 +4020,6 @@
       </c>
       <c r="I26" t="s">
         <v>278</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
-        <v>284</v>
-      </c>
-      <c r="B27">
-        <v>0</v>
-      </c>
-      <c r="C27" s="3">
-        <v>35410000</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="E27" t="s">
-        <v>56</v>
-      </c>
-      <c r="F27">
-        <v>0</v>
-      </c>
-      <c r="G27">
-        <v>0</v>
-      </c>
-      <c r="H27" t="s">
-        <v>285</v>
-      </c>
-      <c r="I27" t="s">
-        <v>286</v>
       </c>
     </row>
   </sheetData>
@@ -4072,7 +4031,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA629D80-511C-42AD-ACB3-22237E3BD282}">
   <dimension ref="A1:B69"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
       <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Transpose where RTI not first
Automatically transpose so that RTI comes as the row in 2D variables, to ensure the conversion is correct.
</commit_message>
<xml_diff>
--- a/Inputs/_MasterFiles/FTT_variables.xlsx
+++ b/Inputs/_MasterFiles/FTT_variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\E3ME\FTT_Stand_Alone\Inputs\_MasterFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/f_j_m_m_nijsse_exeter_ac_uk/Documents/Documents/GitHub/FTT_StandAlone/Inputs/_MasterFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6AAC6B1-6F73-4CBC-BFCC-308507F8D1EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FTT-P" sheetId="1" r:id="rId1"/>
@@ -965,10 +965,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
@@ -1257,16 +1256,16 @@
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.59765625" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="12.86328125" customWidth="1"/>
-    <col min="7" max="7" width="14.3984375" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1289,7 +1288,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1312,7 +1311,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>60</v>
       </c>
@@ -1335,7 +1334,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>64</v>
       </c>
@@ -1358,7 +1357,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>65</v>
       </c>
@@ -1381,7 +1380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>76</v>
       </c>
@@ -1404,7 +1403,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>87</v>
       </c>
@@ -1427,7 +1426,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>57</v>
       </c>
@@ -1450,7 +1449,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>81</v>
       </c>
@@ -1473,7 +1472,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>72</v>
       </c>
@@ -1496,7 +1495,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>74</v>
       </c>
@@ -1519,7 +1518,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>70</v>
       </c>
@@ -1542,7 +1541,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>84</v>
       </c>
@@ -1565,7 +1564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>91</v>
       </c>
@@ -1588,7 +1587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>93</v>
       </c>
@@ -1611,7 +1610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>83</v>
       </c>
@@ -1634,7 +1633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>85</v>
       </c>
@@ -1657,7 +1656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>68</v>
       </c>
@@ -1680,7 +1679,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>78</v>
       </c>
@@ -1718,18 +1717,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E04294AC-DBC1-4E51-84ED-2EC5066B9024}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.59765625" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1752,7 +1751,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1775,7 +1774,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1798,7 +1797,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1821,7 +1820,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1844,7 +1843,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1867,7 +1866,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1890,7 +1889,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1913,7 +1912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -1936,7 +1935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1959,7 +1958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -1982,7 +1981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -2005,7 +2004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -2028,7 +2027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -2051,7 +2050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -2074,7 +2073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -2097,7 +2096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -2120,7 +2119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -2143,7 +2142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -2166,7 +2165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -2189,7 +2188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>37</v>
       </c>
@@ -2212,7 +2211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -2235,7 +2234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>54</v>
       </c>
@@ -2271,13 +2270,13 @@
       <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.3984375" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2300,7 +2299,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>99</v>
       </c>
@@ -2323,7 +2322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>102</v>
       </c>
@@ -2346,7 +2345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>103</v>
       </c>
@@ -2369,7 +2368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>104</v>
       </c>
@@ -2392,7 +2391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>105</v>
       </c>
@@ -2415,7 +2414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>106</v>
       </c>
@@ -2438,7 +2437,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>107</v>
       </c>
@@ -2461,7 +2460,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>108</v>
       </c>
@@ -2484,7 +2483,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>109</v>
       </c>
@@ -2507,7 +2506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>110</v>
       </c>
@@ -2530,7 +2529,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>111</v>
       </c>
@@ -2553,7 +2552,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>112</v>
       </c>
@@ -2576,7 +2575,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>113</v>
       </c>
@@ -2599,7 +2598,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>114</v>
       </c>
@@ -2622,7 +2621,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>115</v>
       </c>
@@ -2645,7 +2644,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>116</v>
       </c>
@@ -2681,14 +2680,14 @@
       <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.59765625" customWidth="1"/>
-    <col min="5" max="5" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.5703125" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2711,7 +2710,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>134</v>
       </c>
@@ -2734,7 +2733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>158</v>
       </c>
@@ -2757,7 +2756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>135</v>
       </c>
@@ -2780,7 +2779,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>136</v>
       </c>
@@ -2803,7 +2802,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>137</v>
       </c>
@@ -2826,7 +2825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>138</v>
       </c>
@@ -2849,7 +2848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>139</v>
       </c>
@@ -2872,7 +2871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>140</v>
       </c>
@@ -2895,7 +2894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>141</v>
       </c>
@@ -2918,7 +2917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>142</v>
       </c>
@@ -2941,7 +2940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>143</v>
       </c>
@@ -2964,7 +2963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>144</v>
       </c>
@@ -2987,7 +2986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>145</v>
       </c>
@@ -3010,7 +3009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>146</v>
       </c>
@@ -3033,7 +3032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>147</v>
       </c>
@@ -3056,7 +3055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>148</v>
       </c>
@@ -3079,7 +3078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>149</v>
       </c>
@@ -3102,7 +3101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>150</v>
       </c>
@@ -3125,7 +3124,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>151</v>
       </c>
@@ -3148,7 +3147,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>152</v>
       </c>
@@ -3171,7 +3170,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>153</v>
       </c>
@@ -3194,7 +3193,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>154</v>
       </c>
@@ -3217,7 +3216,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>155</v>
       </c>
@@ -3240,7 +3239,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>156</v>
       </c>
@@ -3272,21 +3271,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85BB7FF7-82D6-482E-815B-F3751454FF7D}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.06640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.46484375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.53125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.06640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3315,7 +3314,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>189</v>
       </c>
@@ -3344,7 +3343,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>192</v>
       </c>
@@ -3373,7 +3372,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>223</v>
       </c>
@@ -3395,14 +3394,14 @@
       <c r="G4" t="s">
         <v>56</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" t="s">
         <v>220</v>
       </c>
       <c r="I4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>198</v>
       </c>
@@ -3424,14 +3423,14 @@
       <c r="G5">
         <v>0</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" t="s">
         <v>236</v>
       </c>
       <c r="I5" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>201</v>
       </c>
@@ -3460,7 +3459,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>222</v>
       </c>
@@ -3489,7 +3488,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>224</v>
       </c>
@@ -3518,7 +3517,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>225</v>
       </c>
@@ -3547,7 +3546,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>226</v>
       </c>
@@ -3576,7 +3575,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>227</v>
       </c>
@@ -3605,7 +3604,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>228</v>
       </c>
@@ -3634,7 +3633,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>218</v>
       </c>
@@ -3663,7 +3662,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>232</v>
       </c>
@@ -3689,7 +3688,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>234</v>
       </c>
@@ -3715,7 +3714,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>241</v>
       </c>
@@ -3744,7 +3743,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>242</v>
       </c>
@@ -3773,14 +3772,14 @@
         <v>238</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>245</v>
       </c>
       <c r="B18">
         <v>0</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="2">
         <v>35340000</v>
       </c>
       <c r="D18" t="s">
@@ -3802,14 +3801,14 @@
         <v>249</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>251</v>
       </c>
       <c r="B19">
         <v>0</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="2">
         <v>35350000</v>
       </c>
       <c r="D19" t="s">
@@ -3831,7 +3830,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>253</v>
       </c>
@@ -3860,7 +3859,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>257</v>
       </c>
@@ -3889,14 +3888,14 @@
         <v>259</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>261</v>
       </c>
       <c r="B22">
         <v>0</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="2">
         <v>35360000</v>
       </c>
       <c r="D22" t="s">
@@ -3905,7 +3904,7 @@
       <c r="E22" t="s">
         <v>56</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="F22" s="3" t="s">
         <v>280</v>
       </c>
       <c r="G22">
@@ -3918,14 +3917,14 @@
         <v>262</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>267</v>
       </c>
       <c r="B23">
         <v>0</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="2">
         <v>35370000</v>
       </c>
       <c r="D23" t="s">
@@ -3947,14 +3946,14 @@
         <v>266</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>273</v>
       </c>
       <c r="B24">
         <v>0</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="2">
         <v>35380000</v>
       </c>
       <c r="D24" t="s">
@@ -3976,7 +3975,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>269</v>
       </c>
@@ -3992,7 +3991,7 @@
       <c r="E25" t="s">
         <v>195</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F25" t="s">
         <v>41</v>
       </c>
       <c r="G25">
@@ -4005,26 +4004,26 @@
         <v>275</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A26" s="4" t="s">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
         <v>279</v>
       </c>
       <c r="B26">
         <v>0</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="2">
         <v>35390000</v>
       </c>
       <c r="D26" t="s">
         <v>276</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="F26" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="G26" s="4" t="s">
+      <c r="G26" s="3" t="s">
         <v>56</v>
       </c>
       <c r="H26" t="s">
@@ -4034,17 +4033,17 @@
         <v>278</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>284</v>
       </c>
       <c r="B27">
         <v>0</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27" s="2">
         <v>35410000</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="2" t="s">
         <v>287</v>
       </c>
       <c r="E27" t="s">
@@ -4076,9 +4075,9 @@
       <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4086,7 +4085,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -4094,7 +4093,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -4102,7 +4101,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -4110,7 +4109,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -4118,7 +4117,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -4126,7 +4125,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>54</v>
       </c>
@@ -4134,7 +4133,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -4142,7 +4141,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -4150,7 +4149,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -4158,7 +4157,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -4166,7 +4165,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -4174,7 +4173,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -4182,7 +4181,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -4190,7 +4189,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -4198,7 +4197,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>65</v>
       </c>
@@ -4206,7 +4205,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>76</v>
       </c>
@@ -4214,7 +4213,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>81</v>
       </c>
@@ -4222,7 +4221,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>72</v>
       </c>
@@ -4230,7 +4229,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>74</v>
       </c>
@@ -4238,7 +4237,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>70</v>
       </c>
@@ -4246,7 +4245,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>68</v>
       </c>
@@ -4254,7 +4253,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>78</v>
       </c>
@@ -4262,7 +4261,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>106</v>
       </c>
@@ -4270,7 +4269,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>107</v>
       </c>
@@ -4278,7 +4277,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>108</v>
       </c>
@@ -4286,7 +4285,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>109</v>
       </c>
@@ -4294,7 +4293,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>110</v>
       </c>
@@ -4302,7 +4301,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>111</v>
       </c>
@@ -4310,7 +4309,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>112</v>
       </c>
@@ -4318,7 +4317,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>113</v>
       </c>
@@ -4326,7 +4325,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>114</v>
       </c>
@@ -4334,7 +4333,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>115</v>
       </c>
@@ -4342,7 +4341,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>133</v>
       </c>
@@ -4350,7 +4349,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>134</v>
       </c>
@@ -4358,7 +4357,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>158</v>
       </c>
@@ -4366,7 +4365,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>135</v>
       </c>
@@ -4374,7 +4373,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>150</v>
       </c>
@@ -4382,7 +4381,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>151</v>
       </c>
@@ -4390,7 +4389,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>152</v>
       </c>
@@ -4398,7 +4397,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>153</v>
       </c>
@@ -4406,7 +4405,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>154</v>
       </c>
@@ -4414,7 +4413,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>155</v>
       </c>
@@ -4422,7 +4421,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>156</v>
       </c>
@@ -4430,7 +4429,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>189</v>
       </c>
@@ -4438,7 +4437,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>192</v>
       </c>
@@ -4446,7 +4445,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>223</v>
       </c>
@@ -4454,7 +4453,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>198</v>
       </c>
@@ -4462,7 +4461,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>201</v>
       </c>
@@ -4470,7 +4469,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>222</v>
       </c>
@@ -4478,7 +4477,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>224</v>
       </c>
@@ -4486,7 +4485,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>225</v>
       </c>
@@ -4494,7 +4493,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>226</v>
       </c>
@@ -4502,7 +4501,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>227</v>
       </c>
@@ -4510,7 +4509,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>228</v>
       </c>
@@ -4518,7 +4517,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>218</v>
       </c>
@@ -4526,7 +4525,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>251</v>
       </c>
@@ -4534,7 +4533,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>253</v>
       </c>
@@ -4542,7 +4541,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>257</v>
       </c>
@@ -4550,7 +4549,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>273</v>
       </c>
@@ -4558,8 +4557,8 @@
         <v>97</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A69" s="4"/>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Update FTT-Tr classification sizes
Changed classification sizes of C3TI and VTTI. Removed TSFD (not used). Removed old input files for FTT-Tr. Added new U.db1 file with the correct dimensions for transport.
</commit_message>
<xml_diff>
--- a/Inputs/_MasterFiles/FTT_variables.xlsx
+++ b/Inputs/_MasterFiles/FTT_variables.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/f_j_m_m_nijsse_exeter_ac_uk/Documents/Documents/GitHub/FTT_StandAlone/Inputs/_MasterFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/cl852_exeter_ac_uk/Documents/Documents/GitHub/FTT_StandAlone/Inputs/_MasterFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6AAC6B1-6F73-4CBC-BFCC-308507F8D1EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{B6AAC6B1-6F73-4CBC-BFCC-308507F8D1EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6720B74-0E82-430C-BE0F-4DF10A26EE9E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FTT-P" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="286">
   <si>
     <t>Variable name</t>
   </si>
@@ -143,9 +143,6 @@
     <t>TESF</t>
   </si>
   <si>
-    <t>TSFD</t>
-  </si>
-  <si>
     <t>TESH</t>
   </si>
   <si>
@@ -174,9 +171,6 @@
   </si>
   <si>
     <t>FTT-Tr Private veh survival functions over 23y (th-veh)</t>
-  </si>
-  <si>
-    <t>FTT-Tr Private veh survival functions time derivative over 23y (th-veh)</t>
   </si>
   <si>
     <t>FTT-Tr Private veh sales history over 23y (th-veh)</t>
@@ -1256,21 +1250,21 @@
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" customWidth="1"/>
+    <col min="4" max="4" width="19.54296875" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.81640625" customWidth="1"/>
+    <col min="7" max="7" width="14.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1288,7 +1282,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1299,21 +1293,21 @@
         <v>31010000</v>
       </c>
       <c r="D2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>58</v>
-      </c>
-      <c r="F2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>60</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1322,21 +1316,21 @@
         <v>31020000</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F3" t="s">
         <v>24</v>
       </c>
       <c r="G3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1345,21 +1339,21 @@
         <v>31030000</v>
       </c>
       <c r="D4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F4" t="s">
         <v>24</v>
       </c>
       <c r="G4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1368,10 +1362,10 @@
         <v>31040000</v>
       </c>
       <c r="D5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -1380,9 +1374,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1391,21 +1385,21 @@
         <v>31050000</v>
       </c>
       <c r="D6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F6" t="s">
         <v>24</v>
       </c>
       <c r="G6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -1414,21 +1408,21 @@
         <v>31060000</v>
       </c>
       <c r="D7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -1437,21 +1431,21 @@
         <v>31070000</v>
       </c>
       <c r="D8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1460,21 +1454,21 @@
         <v>31090000</v>
       </c>
       <c r="D9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F9" t="s">
         <v>24</v>
       </c>
       <c r="G9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1483,21 +1477,21 @@
         <v>31100000</v>
       </c>
       <c r="D10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F10" t="s">
         <v>24</v>
       </c>
       <c r="G10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1506,21 +1500,21 @@
         <v>31110000</v>
       </c>
       <c r="D11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F11" t="s">
         <v>24</v>
       </c>
       <c r="G11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1529,21 +1523,21 @@
         <v>31120000</v>
       </c>
       <c r="D12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F12" t="s">
         <v>24</v>
       </c>
       <c r="G12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -1552,21 +1546,21 @@
         <v>31130000</v>
       </c>
       <c r="D13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -1575,21 +1569,21 @@
         <v>31140000</v>
       </c>
       <c r="D14" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F14" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G14">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -1598,21 +1592,21 @@
         <v>31150000</v>
       </c>
       <c r="D15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F15" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G15">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1621,21 +1615,21 @@
         <v>31180000</v>
       </c>
       <c r="D16" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G16">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -1644,21 +1638,21 @@
         <v>31190000</v>
       </c>
       <c r="D17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G17">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -1667,21 +1661,21 @@
         <v>31200000</v>
       </c>
       <c r="D18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E18" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F18" t="s">
         <v>24</v>
       </c>
       <c r="G18" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -1690,16 +1684,16 @@
         <v>31210000</v>
       </c>
       <c r="D19" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E19" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F19" t="s">
         <v>24</v>
       </c>
       <c r="G19" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1715,25 +1709,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E04294AC-DBC1-4E51-84ED-2EC5066B9024}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.5703125" customWidth="1"/>
+    <col min="2" max="2" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1751,7 +1745,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1771,10 +1765,10 @@
         <v>23</v>
       </c>
       <c r="G2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1794,10 +1788,10 @@
         <v>24</v>
       </c>
       <c r="G3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1817,10 +1811,10 @@
         <v>24</v>
       </c>
       <c r="G4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1840,10 +1834,10 @@
         <v>24</v>
       </c>
       <c r="G5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1863,10 +1857,10 @@
         <v>24</v>
       </c>
       <c r="G6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1886,10 +1880,10 @@
         <v>24</v>
       </c>
       <c r="G7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1900,10 +1894,10 @@
         <v>32130000</v>
       </c>
       <c r="D8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F8" t="s">
         <v>24</v>
@@ -1912,7 +1906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -1923,10 +1917,10 @@
         <v>32140000</v>
       </c>
       <c r="D9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F9" t="s">
         <v>24</v>
@@ -1935,7 +1929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1946,10 +1940,10 @@
         <v>32150000</v>
       </c>
       <c r="D10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F10" t="s">
         <v>24</v>
@@ -1958,7 +1952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -1969,7 +1963,7 @@
         <v>32160000</v>
       </c>
       <c r="D11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E11" t="s">
         <v>22</v>
@@ -1981,7 +1975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -1992,7 +1986,7 @@
         <v>32170000</v>
       </c>
       <c r="D12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E12" t="s">
         <v>22</v>
@@ -2004,7 +1998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -2015,7 +2009,7 @@
         <v>32180000</v>
       </c>
       <c r="D13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E13" t="s">
         <v>22</v>
@@ -2027,76 +2021,76 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>32</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14">
         <v>32190000</v>
       </c>
       <c r="D14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G14">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>33</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15">
-        <v>32200000</v>
+        <v>32210000</v>
       </c>
       <c r="D15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G15">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>34</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16">
-        <v>32210000</v>
+        <v>32220000</v>
       </c>
       <c r="D16" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G16">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -2104,105 +2098,105 @@
         <v>1</v>
       </c>
       <c r="C17">
-        <v>32220000</v>
+        <v>32230000</v>
       </c>
       <c r="D17" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E17" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" t="s">
         <v>40</v>
       </c>
-      <c r="F17" t="s">
-        <v>56</v>
-      </c>
       <c r="G17">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>32300000</v>
+      </c>
+      <c r="D18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>32310000</v>
+      </c>
+      <c r="D19" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" t="s">
+        <v>54</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>36</v>
       </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18">
-        <v>32230000</v>
-      </c>
-      <c r="D18" t="s">
-        <v>42</v>
-      </c>
-      <c r="E18" t="s">
-        <v>22</v>
-      </c>
-      <c r="F18" t="s">
-        <v>41</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19">
-        <v>32300000</v>
-      </c>
-      <c r="D19" t="s">
-        <v>46</v>
-      </c>
-      <c r="E19" t="s">
-        <v>56</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>19</v>
-      </c>
       <c r="B20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20">
-        <v>32310000</v>
+        <v>32320000</v>
       </c>
       <c r="D20" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E20" t="s">
-        <v>56</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
+        <v>54</v>
+      </c>
+      <c r="F20" t="s">
+        <v>24</v>
       </c>
       <c r="G20">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21">
-        <v>32320000</v>
+        <v>32330000</v>
       </c>
       <c r="D21" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="E21" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F21" t="s">
         <v>24</v>
@@ -2211,49 +2205,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C22">
-        <v>32330000</v>
+        <v>32340000</v>
       </c>
       <c r="D22" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="E22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F22" t="s">
         <v>24</v>
       </c>
       <c r="G22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>54</v>
-      </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="C23">
-        <v>32340000</v>
-      </c>
-      <c r="D23" t="s">
-        <v>55</v>
-      </c>
-      <c r="E23" t="s">
-        <v>56</v>
-      </c>
-      <c r="F23" t="s">
-        <v>24</v>
-      </c>
-      <c r="G23">
         <v>0</v>
       </c>
     </row>
@@ -2270,18 +2241,18 @@
       <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.42578125" customWidth="1"/>
+    <col min="2" max="2" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -2299,9 +2270,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2310,21 +2281,21 @@
         <v>33130000</v>
       </c>
       <c r="D2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>100</v>
-      </c>
-      <c r="E2" t="s">
-        <v>101</v>
-      </c>
-      <c r="F2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>102</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -2333,21 +2304,21 @@
         <v>33180000</v>
       </c>
       <c r="D3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -2356,21 +2327,21 @@
         <v>33020000</v>
       </c>
       <c r="D4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2379,21 +2350,21 @@
         <v>33030000</v>
       </c>
       <c r="D5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -2402,10 +2373,10 @@
         <v>33050000</v>
       </c>
       <c r="D6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -2414,9 +2385,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -2425,21 +2396,21 @@
         <v>33120000</v>
       </c>
       <c r="D7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F7" t="s">
         <v>24</v>
       </c>
       <c r="G7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -2448,21 +2419,21 @@
         <v>33140000</v>
       </c>
       <c r="D8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F8" t="s">
         <v>24</v>
       </c>
       <c r="G8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -2471,21 +2442,21 @@
         <v>33040000</v>
       </c>
       <c r="D9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F9" t="s">
         <v>24</v>
       </c>
       <c r="G9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -2494,10 +2465,10 @@
         <v>33170000</v>
       </c>
       <c r="D10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F10" t="s">
         <v>24</v>
@@ -2506,9 +2477,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -2517,21 +2488,21 @@
         <v>33060000</v>
       </c>
       <c r="D11" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F11" t="s">
         <v>24</v>
       </c>
       <c r="G11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -2540,21 +2511,21 @@
         <v>33070000</v>
       </c>
       <c r="D12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F12" t="s">
         <v>24</v>
       </c>
       <c r="G12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -2563,21 +2534,21 @@
         <v>33080000</v>
       </c>
       <c r="D13" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E13" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F13" t="s">
         <v>24</v>
       </c>
       <c r="G13" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -2586,21 +2557,21 @@
         <v>33090000</v>
       </c>
       <c r="D14" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E14" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F14" t="s">
         <v>24</v>
       </c>
       <c r="G14" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -2609,21 +2580,21 @@
         <v>33100000</v>
       </c>
       <c r="D15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F15" t="s">
         <v>24</v>
       </c>
       <c r="G15" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -2632,21 +2603,21 @@
         <v>33110000</v>
       </c>
       <c r="D16" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E16" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F16" t="s">
         <v>24</v>
       </c>
       <c r="G16" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -2655,16 +2626,16 @@
         <v>33010000</v>
       </c>
       <c r="D17" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E17" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F17" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -2680,19 +2651,19 @@
       <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.5703125" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.54296875" customWidth="1"/>
+    <col min="5" max="5" width="9.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -2710,9 +2681,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2721,10 +2692,10 @@
         <v>34230000</v>
       </c>
       <c r="D2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F2" t="s">
         <v>24</v>
@@ -2733,9 +2704,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -2744,10 +2715,10 @@
         <v>34290000</v>
       </c>
       <c r="D3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F3" t="s">
         <v>24</v>
@@ -2756,9 +2727,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -2767,21 +2738,21 @@
         <v>34240000</v>
       </c>
       <c r="D4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F4" t="s">
         <v>24</v>
       </c>
       <c r="G4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2790,21 +2761,21 @@
         <v>34010000</v>
       </c>
       <c r="D5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E5" t="s">
+        <v>181</v>
+      </c>
+      <c r="F5" t="s">
         <v>183</v>
       </c>
-      <c r="F5" t="s">
-        <v>185</v>
-      </c>
       <c r="G5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -2813,21 +2784,21 @@
         <v>34050000</v>
       </c>
       <c r="D6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -2836,21 +2807,21 @@
         <v>34020000</v>
       </c>
       <c r="D7" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E7" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F7" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -2859,21 +2830,21 @@
         <v>34320000</v>
       </c>
       <c r="D8" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -2882,21 +2853,21 @@
         <v>34030000</v>
       </c>
       <c r="D9" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E9" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F9" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -2905,21 +2876,21 @@
         <v>34040000</v>
       </c>
       <c r="D10" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E10" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -2928,21 +2899,21 @@
         <v>34110000</v>
       </c>
       <c r="D11" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F11" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -2951,21 +2922,21 @@
         <v>34120000</v>
       </c>
       <c r="D12" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F12" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G12">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -2974,21 +2945,21 @@
         <v>34130000</v>
       </c>
       <c r="D13" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F13" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -2997,21 +2968,21 @@
         <v>34140000</v>
       </c>
       <c r="D14" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F14" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G14">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -3020,21 +2991,21 @@
         <v>34070000</v>
       </c>
       <c r="D15" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E15" t="s">
+        <v>182</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>186</v>
-      </c>
       <c r="G15">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -3043,21 +3014,21 @@
         <v>34080000</v>
       </c>
       <c r="D16" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E16" t="s">
+        <v>182</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>186</v>
-      </c>
       <c r="G16">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -3066,10 +3037,10 @@
         <v>34100000</v>
       </c>
       <c r="D17" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E17" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -3078,9 +3049,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -3089,10 +3060,10 @@
         <v>34090000</v>
       </c>
       <c r="D18" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E18" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -3101,9 +3072,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -3112,21 +3083,21 @@
         <v>34160000</v>
       </c>
       <c r="D19" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E19" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F19" t="s">
         <v>24</v>
       </c>
       <c r="G19" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -3135,21 +3106,21 @@
         <v>34170000</v>
       </c>
       <c r="D20" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E20" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F20" t="s">
         <v>24</v>
       </c>
       <c r="G20" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -3158,21 +3129,21 @@
         <v>34180000</v>
       </c>
       <c r="D21" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E21" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F21" t="s">
         <v>24</v>
       </c>
       <c r="G21" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -3181,21 +3152,21 @@
         <v>34190000</v>
       </c>
       <c r="D22" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E22" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F22" t="s">
         <v>24</v>
       </c>
       <c r="G22" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -3204,21 +3175,21 @@
         <v>34220000</v>
       </c>
       <c r="D23" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E23" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F23" t="s">
         <v>24</v>
       </c>
       <c r="G23" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -3227,21 +3198,21 @@
         <v>34200000</v>
       </c>
       <c r="D24" t="s">
+        <v>179</v>
+      </c>
+      <c r="E24" t="s">
         <v>181</v>
       </c>
-      <c r="E24" t="s">
-        <v>183</v>
-      </c>
       <c r="F24" t="s">
         <v>24</v>
       </c>
       <c r="G24" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -3250,16 +3221,16 @@
         <v>34210000</v>
       </c>
       <c r="D25" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E25" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F25" t="s">
         <v>24</v>
       </c>
       <c r="G25" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -3275,22 +3246,22 @@
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.54296875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -3308,15 +3279,15 @@
         <v>25</v>
       </c>
       <c r="H1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -3325,10 +3296,10 @@
         <v>35330000</v>
       </c>
       <c r="D2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F2" t="s">
         <v>24</v>
@@ -3337,15 +3308,15 @@
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="I2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -3354,10 +3325,10 @@
         <v>35320000</v>
       </c>
       <c r="D3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F3" t="s">
         <v>24</v>
@@ -3366,15 +3337,15 @@
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="I3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -3383,27 +3354,27 @@
         <v>35060000</v>
       </c>
       <c r="D4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F4" t="s">
         <v>24</v>
       </c>
       <c r="G4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="I4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -3412,10 +3383,10 @@
         <v>35070000</v>
       </c>
       <c r="D5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F5" t="s">
         <v>24</v>
@@ -3424,15 +3395,15 @@
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="I5" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -3441,10 +3412,10 @@
         <v>35140000</v>
       </c>
       <c r="D6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F6" t="s">
         <v>24</v>
@@ -3453,15 +3424,15 @@
         <v>0</v>
       </c>
       <c r="H6" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="I6" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -3470,27 +3441,27 @@
         <v>35040000</v>
       </c>
       <c r="D7" t="s">
+        <v>227</v>
+      </c>
+      <c r="E7" t="s">
+        <v>193</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" t="s">
+        <v>54</v>
+      </c>
+      <c r="H7" t="s">
         <v>229</v>
       </c>
-      <c r="E7" t="s">
-        <v>195</v>
-      </c>
-      <c r="F7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" t="s">
-        <v>56</v>
-      </c>
-      <c r="H7" t="s">
-        <v>231</v>
-      </c>
       <c r="I7" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -3499,27 +3470,27 @@
         <v>35050000</v>
       </c>
       <c r="D8" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F8" t="s">
         <v>24</v>
       </c>
       <c r="G8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H8" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I8" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -3528,27 +3499,27 @@
         <v>35020000</v>
       </c>
       <c r="D9" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E9" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F9" t="s">
         <v>24</v>
       </c>
       <c r="G9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H9" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="I9" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -3557,27 +3528,27 @@
         <v>35030000</v>
       </c>
       <c r="D10" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E10" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F10" t="s">
         <v>24</v>
       </c>
       <c r="G10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H10" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="I10" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -3586,10 +3557,10 @@
         <v>35150000</v>
       </c>
       <c r="D11" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F11" t="s">
         <v>24</v>
@@ -3598,15 +3569,15 @@
         <v>0</v>
       </c>
       <c r="H11" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="I11" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -3615,10 +3586,10 @@
         <v>35130000</v>
       </c>
       <c r="D12" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F12" t="s">
         <v>24</v>
@@ -3630,12 +3601,12 @@
         <v>26</v>
       </c>
       <c r="I12" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -3644,10 +3615,10 @@
         <v>35140000</v>
       </c>
       <c r="D13" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F13" t="s">
         <v>24</v>
@@ -3656,15 +3627,15 @@
         <v>0</v>
       </c>
       <c r="H13" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="I13" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -3673,13 +3644,13 @@
         <v>35210000</v>
       </c>
       <c r="D14" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E14" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F14" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -3688,9 +3659,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -3699,13 +3670,13 @@
         <v>35220000</v>
       </c>
       <c r="D15" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E15" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F15" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -3714,9 +3685,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -3725,27 +3696,27 @@
         <v>35160000</v>
       </c>
       <c r="D16" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E16" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F16" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G16">
         <v>0</v>
       </c>
       <c r="H16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="I16" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -3754,27 +3725,27 @@
         <v>35170000</v>
       </c>
       <c r="D17" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E17" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F17" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G17">
         <v>0</v>
       </c>
       <c r="H17" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="I17" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -3783,10 +3754,10 @@
         <v>35340000</v>
       </c>
       <c r="D18" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E18" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -3795,15 +3766,15 @@
         <v>0</v>
       </c>
       <c r="H18" t="s">
+        <v>245</v>
+      </c>
+      <c r="I18" t="s">
         <v>247</v>
       </c>
-      <c r="I18" t="s">
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>249</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>251</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -3812,10 +3783,10 @@
         <v>35350000</v>
       </c>
       <c r="D19" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E19" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F19" t="s">
         <v>24</v>
@@ -3824,15 +3795,15 @@
         <v>0</v>
       </c>
       <c r="H19" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="I19" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -3841,27 +3812,27 @@
         <v>35190000</v>
       </c>
       <c r="D20" t="s">
+        <v>252</v>
+      </c>
+      <c r="E20" t="s">
+        <v>54</v>
+      </c>
+      <c r="F20" t="s">
+        <v>24</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20" t="s">
+        <v>253</v>
+      </c>
+      <c r="I20" t="s">
         <v>254</v>
       </c>
-      <c r="E20" t="s">
-        <v>56</v>
-      </c>
-      <c r="F20" t="s">
-        <v>24</v>
-      </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20" t="s">
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>255</v>
-      </c>
-      <c r="I20" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>257</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -3870,10 +3841,10 @@
         <v>35200000</v>
       </c>
       <c r="D21" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E21" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F21" t="s">
         <v>24</v>
@@ -3882,15 +3853,15 @@
         <v>0</v>
       </c>
       <c r="H21" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="I21" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>259</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>261</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -3899,27 +3870,27 @@
         <v>35360000</v>
       </c>
       <c r="D22" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="G22">
         <v>0</v>
       </c>
       <c r="H22" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="I22" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -3928,10 +3899,10 @@
         <v>35370000</v>
       </c>
       <c r="D23" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E23" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -3940,15 +3911,15 @@
         <v>0</v>
       </c>
       <c r="H23" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="I23" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -3957,27 +3928,27 @@
         <v>35380000</v>
       </c>
       <c r="D24" t="s">
+        <v>268</v>
+      </c>
+      <c r="E24" t="s">
+        <v>54</v>
+      </c>
+      <c r="F24" t="s">
+        <v>24</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24" t="s">
+        <v>269</v>
+      </c>
+      <c r="I24" t="s">
         <v>270</v>
       </c>
-      <c r="E24" t="s">
-        <v>56</v>
-      </c>
-      <c r="F24" t="s">
-        <v>24</v>
-      </c>
-      <c r="G24">
-        <v>0</v>
-      </c>
-      <c r="H24" t="s">
-        <v>271</v>
-      </c>
-      <c r="I24" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -3986,27 +3957,27 @@
         <v>35230000</v>
       </c>
       <c r="D25" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E25" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G25">
         <v>0</v>
       </c>
       <c r="H25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I25" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -4015,27 +3986,27 @@
         <v>35390000</v>
       </c>
       <c r="D26" t="s">
+        <v>274</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H26" t="s">
+        <v>275</v>
+      </c>
+      <c r="I26" t="s">
         <v>276</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="H26" t="s">
-        <v>277</v>
-      </c>
-      <c r="I26" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -4044,10 +4015,10 @@
         <v>35410000</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F27">
         <v>0</v>
@@ -4056,10 +4027,10 @@
         <v>0</v>
       </c>
       <c r="H27" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="I27" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
   </sheetData>
@@ -4075,489 +4046,489 @@
       <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B14" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B15" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B16" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>76</v>
       </c>
-      <c r="B17" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>81</v>
-      </c>
-      <c r="B18" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>72</v>
-      </c>
-      <c r="B19" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>74</v>
-      </c>
-      <c r="B20" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>70</v>
-      </c>
-      <c r="B21" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>68</v>
-      </c>
-      <c r="B22" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>78</v>
-      </c>
       <c r="B23" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
+        <v>104</v>
+      </c>
+      <c r="B24" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>105</v>
+      </c>
+      <c r="B25" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>106</v>
       </c>
-      <c r="B24" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="B26" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>107</v>
       </c>
-      <c r="B25" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="B27" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>108</v>
       </c>
-      <c r="B26" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="B28" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>109</v>
       </c>
-      <c r="B27" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="B29" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
         <v>110</v>
       </c>
-      <c r="B28" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="B30" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>111</v>
       </c>
-      <c r="B29" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="B31" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
         <v>112</v>
       </c>
-      <c r="B30" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="B32" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
         <v>113</v>
       </c>
-      <c r="B31" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>114</v>
-      </c>
-      <c r="B32" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>115</v>
-      </c>
       <c r="B33" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
+        <v>131</v>
+      </c>
+      <c r="B34" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>132</v>
+      </c>
+      <c r="B35" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>156</v>
+      </c>
+      <c r="B36" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
         <v>133</v>
       </c>
-      <c r="B34" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>134</v>
-      </c>
-      <c r="B35" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>158</v>
-      </c>
-      <c r="B36" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>135</v>
-      </c>
       <c r="B37" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
+        <v>148</v>
+      </c>
+      <c r="B38" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>149</v>
+      </c>
+      <c r="B39" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
         <v>150</v>
       </c>
-      <c r="B38" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="B40" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
         <v>151</v>
       </c>
-      <c r="B39" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="B41" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
         <v>152</v>
       </c>
-      <c r="B40" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="B42" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
         <v>153</v>
       </c>
-      <c r="B41" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="B43" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
         <v>154</v>
       </c>
-      <c r="B42" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>155</v>
-      </c>
-      <c r="B43" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>156</v>
-      </c>
       <c r="B44" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B45" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B46" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
+        <v>221</v>
+      </c>
+      <c r="B47" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>196</v>
+      </c>
+      <c r="B48" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>199</v>
+      </c>
+      <c r="B49" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>220</v>
+      </c>
+      <c r="B50" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>222</v>
+      </c>
+      <c r="B51" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
         <v>223</v>
       </c>
-      <c r="B47" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>198</v>
-      </c>
-      <c r="B48" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>201</v>
-      </c>
-      <c r="B49" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>222</v>
-      </c>
-      <c r="B50" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="B52" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
         <v>224</v>
       </c>
-      <c r="B51" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="B53" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
         <v>225</v>
       </c>
-      <c r="B52" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="B54" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
         <v>226</v>
       </c>
-      <c r="B53" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>227</v>
-      </c>
-      <c r="B54" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>228</v>
-      </c>
       <c r="B55" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B56" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
+        <v>249</v>
+      </c>
+      <c r="B57" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
         <v>251</v>
       </c>
-      <c r="B57" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>253</v>
-      </c>
       <c r="B58" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B59" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B60" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A69" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Data update and starting EV cost
Updated to 2022 data (same as FORTRAN model) and added calculation for starting EV cost without battery (TEVC in this version). This matches exactly values from the FORTRAN model.
</commit_message>
<xml_diff>
--- a/Inputs/_MasterFiles/FTT_variables.xlsx
+++ b/Inputs/_MasterFiles/FTT_variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/cl852_exeter_ac_uk/Documents/Documents/GitHub/FTT_StandAlone/Inputs/_MasterFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{B6AAC6B1-6F73-4CBC-BFCC-308507F8D1EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6720B74-0E82-430C-BE0F-4DF10A26EE9E}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="13_ncr:1_{B6AAC6B1-6F73-4CBC-BFCC-308507F8D1EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4925BCBE-2068-4D64-B4C2-8F0F11A3AF43}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1711,8 +1711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E04294AC-DBC1-4E51-84ED-2EC5066B9024}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2003,7 +2003,7 @@
         <v>31</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13">
         <v>32180000</v>

</xml_diff>

<commit_message>
Add battery learning, fix gamma values
Big update to add new learning treatment for batteries. Now, majority of learning for EVs/PHEVs happens on the battery rather than the total cost of the car.

Fixed a small bug in the masterfiles to csv script. Before, the FTT-Tr gamma values were not being exported.

Changed the U databank as the old one was causing an error in the FORTRAN model (wouldn't have made a difference here but best to have the same file anyway).

FTT-Tr model output now very close to FORTRAN version. I suspect any differences are due to Euler Forward vs. RK4.
</commit_message>
<xml_diff>
--- a/Inputs/_MasterFiles/FTT_variables.xlsx
+++ b/Inputs/_MasterFiles/FTT_variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/cl852_exeter_ac_uk/Documents/Documents/GitHub/FTT_StandAlone/Inputs/_MasterFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="13_ncr:1_{B6AAC6B1-6F73-4CBC-BFCC-308507F8D1EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4925BCBE-2068-4D64-B4C2-8F0F11A3AF43}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="13_ncr:1_{B6AAC6B1-6F73-4CBC-BFCC-308507F8D1EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E572DB04-5F09-4BAF-BE63-0D05288AE52C}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1711,8 +1711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E04294AC-DBC1-4E51-84ED-2EC5066B9024}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1773,7 +1773,7 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>32020000</v>
@@ -1796,7 +1796,7 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>32030000</v>
@@ -1819,7 +1819,7 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5">
         <v>32040000</v>
@@ -1842,7 +1842,7 @@
         <v>12</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6">
         <v>32050000</v>
@@ -1865,7 +1865,7 @@
         <v>14</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7">
         <v>32060000</v>
@@ -1888,7 +1888,7 @@
         <v>26</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8">
         <v>32130000</v>
@@ -1911,7 +1911,7 @@
         <v>27</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9">
         <v>32140000</v>
@@ -1934,7 +1934,7 @@
         <v>28</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10">
         <v>32150000</v>
@@ -1957,7 +1957,7 @@
         <v>29</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11">
         <v>32160000</v>
@@ -1980,7 +1980,7 @@
         <v>30</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12">
         <v>32170000</v>
@@ -2095,7 +2095,7 @@
         <v>35</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17">
         <v>32230000</v>

</xml_diff>

<commit_message>
automate the change to csv files
Ensuring that variables like TEWW and GAMMA are correctly changed. The latter still poses a problem with the gamma functionality, which updates the csv files directly.
</commit_message>
<xml_diff>
--- a/Inputs/_MasterFiles/FTT_variables.xlsx
+++ b/Inputs/_MasterFiles/FTT_variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/cl852_exeter_ac_uk/Documents/Documents/GitHub/FTT_StandAlone/Inputs/_MasterFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/f_j_m_m_nijsse_exeter_ac_uk/Documents/Documents/GitHub/FTT_StandAlone_laptop/FTT_StandAlone/Inputs/_MasterFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="13_ncr:1_{B6AAC6B1-6F73-4CBC-BFCC-308507F8D1EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E572DB04-5F09-4BAF-BE63-0D05288AE52C}"/>
+  <xr:revisionPtr revIDLastSave="294" documentId="13_ncr:1_{B6AAC6B1-6F73-4CBC-BFCC-308507F8D1EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC775577-5634-4C66-940B-B6E76A5CD3E1}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FTT-P" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="295">
   <si>
     <t>Variable name</t>
   </si>
@@ -284,9 +284,6 @@
     <t>MEWR</t>
   </si>
   <si>
-    <t>FTT-Power</t>
-  </si>
-  <si>
     <t>MEWB</t>
   </si>
   <si>
@@ -900,6 +897,36 @@
   </si>
   <si>
     <t>FTT-Fr T-Scaling</t>
+  </si>
+  <si>
+    <t>tl_2012</t>
+  </si>
+  <si>
+    <t>TGAM</t>
+  </si>
+  <si>
+    <t>tl_2014</t>
+  </si>
+  <si>
+    <t>Conversion?</t>
+  </si>
+  <si>
+    <t>GAMMA</t>
+  </si>
+  <si>
+    <t>HGAM</t>
+  </si>
+  <si>
+    <t>Scenario</t>
+  </si>
+  <si>
+    <t>S0</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>FTT-Power regulations</t>
   </si>
 </sst>
 </file>
@@ -1244,27 +1271,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.54296875" customWidth="1"/>
+    <col min="4" max="4" width="35" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="12.81640625" customWidth="1"/>
-    <col min="7" max="7" width="14.453125" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1281,8 +1308,14 @@
       <c r="G1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H1" t="s">
+        <v>288</v>
+      </c>
+      <c r="I1" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1304,8 +1337,14 @@
       <c r="G2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>58</v>
       </c>
@@ -1327,8 +1366,14 @@
       <c r="G3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>62</v>
       </c>
@@ -1350,8 +1395,14 @@
       <c r="G4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>63</v>
       </c>
@@ -1373,8 +1424,14 @@
       <c r="G5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>74</v>
       </c>
@@ -1396,10 +1453,16 @@
       <c r="G6" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -1408,7 +1471,7 @@
         <v>31060000</v>
       </c>
       <c r="D7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E7" t="s">
         <v>56</v>
@@ -1419,8 +1482,14 @@
       <c r="G7" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -1442,8 +1511,14 @@
       <c r="G8" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>79</v>
       </c>
@@ -1454,7 +1529,7 @@
         <v>31090000</v>
       </c>
       <c r="D9" t="s">
-        <v>80</v>
+        <v>294</v>
       </c>
       <c r="E9" t="s">
         <v>56</v>
@@ -1465,8 +1540,14 @@
       <c r="G9" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>70</v>
       </c>
@@ -1488,8 +1569,14 @@
       <c r="G10" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>72</v>
       </c>
@@ -1511,8 +1598,14 @@
       <c r="G11" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -1534,10 +1627,16 @@
       <c r="G12" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -1546,7 +1645,7 @@
         <v>31130000</v>
       </c>
       <c r="D13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E13" t="s">
         <v>56</v>
@@ -1557,10 +1656,16 @@
       <c r="G13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -1569,21 +1674,27 @@
         <v>31140000</v>
       </c>
       <c r="D14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E14" t="s">
         <v>56</v>
       </c>
       <c r="F14" t="s">
+        <v>89</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>90</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>91</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -1592,21 +1703,27 @@
         <v>31150000</v>
       </c>
       <c r="D15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E15" t="s">
         <v>56</v>
       </c>
       <c r="F15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1615,7 +1732,7 @@
         <v>31180000</v>
       </c>
       <c r="D16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E16" t="s">
         <v>56</v>
@@ -1626,10 +1743,16 @@
       <c r="G16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -1638,7 +1761,7 @@
         <v>31190000</v>
       </c>
       <c r="D17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E17" t="s">
         <v>56</v>
@@ -1649,8 +1772,14 @@
       <c r="G17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>66</v>
       </c>
@@ -1672,8 +1801,14 @@
       <c r="G18" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>76</v>
       </c>
@@ -1694,6 +1829,12 @@
       </c>
       <c r="G19" t="s">
         <v>54</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19" t="s">
+        <v>293</v>
       </c>
     </row>
   </sheetData>
@@ -1709,25 +1850,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E04294AC-DBC1-4E51-84ED-2EC5066B9024}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.54296875" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1744,8 +1885,14 @@
       <c r="G1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H1" t="s">
+        <v>288</v>
+      </c>
+      <c r="I1" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1767,13 +1914,19 @@
       <c r="G2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H2" t="s">
+        <v>289</v>
+      </c>
+      <c r="I2" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>32020000</v>
@@ -1790,13 +1943,19 @@
       <c r="G3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4">
         <v>32030000</v>
@@ -1813,13 +1972,19 @@
       <c r="G4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <v>32040000</v>
@@ -1836,13 +2001,19 @@
       <c r="G5" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6">
         <v>32050000</v>
@@ -1859,13 +2030,19 @@
       <c r="G6" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7">
         <v>32060000</v>
@@ -1882,13 +2059,19 @@
       <c r="G7" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8">
         <v>32130000</v>
@@ -1905,13 +2088,19 @@
       <c r="G8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>27</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9">
         <v>32140000</v>
@@ -1928,13 +2117,19 @@
       <c r="G9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10">
         <v>32150000</v>
@@ -1951,13 +2146,19 @@
       <c r="G10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11">
         <v>32160000</v>
@@ -1974,13 +2175,19 @@
       <c r="G11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>30</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12">
         <v>32170000</v>
@@ -1997,13 +2204,19 @@
       <c r="G12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>31</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13">
         <v>32180000</v>
@@ -2020,13 +2233,19 @@
       <c r="G13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H13" t="s">
+        <v>24</v>
+      </c>
+      <c r="I13" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>32</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14">
         <v>32190000</v>
@@ -2043,13 +2262,19 @@
       <c r="G14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>33</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15">
         <v>32210000</v>
@@ -2066,13 +2291,19 @@
       <c r="G15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>34</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16">
         <v>32220000</v>
@@ -2089,13 +2320,19 @@
       <c r="G16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>35</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17">
         <v>32230000</v>
@@ -2112,13 +2349,19 @@
       <c r="G17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18">
         <v>32300000</v>
@@ -2135,13 +2378,19 @@
       <c r="G18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19">
         <v>32310000</v>
@@ -2158,13 +2407,19 @@
       <c r="G19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>36</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20">
         <v>32320000</v>
@@ -2181,13 +2436,19 @@
       <c r="G20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>16</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21">
         <v>32330000</v>
@@ -2204,13 +2465,19 @@
       <c r="G21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>52</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22">
         <v>32340000</v>
@@ -2226,6 +2493,12 @@
       </c>
       <c r="G22">
         <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22" t="s">
+        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -2235,24 +2508,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{893746F0-70F0-4C21-8E46-9B5DBA6E54BB}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.453125" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -2269,10 +2542,16 @@
       <c r="G1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H1" t="s">
+        <v>288</v>
+      </c>
+      <c r="I1" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2281,10 +2560,10 @@
         <v>33130000</v>
       </c>
       <c r="D2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E2" t="s">
         <v>98</v>
-      </c>
-      <c r="E2" t="s">
-        <v>99</v>
       </c>
       <c r="F2" t="s">
         <v>40</v>
@@ -2292,10 +2571,16 @@
       <c r="G2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -2304,7 +2589,7 @@
         <v>33180000</v>
       </c>
       <c r="D3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E3" t="s">
         <v>40</v>
@@ -2315,10 +2600,16 @@
       <c r="G3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -2327,21 +2618,27 @@
         <v>33020000</v>
       </c>
       <c r="D4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2350,21 +2647,27 @@
         <v>33030000</v>
       </c>
       <c r="D5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -2373,10 +2676,10 @@
         <v>33050000</v>
       </c>
       <c r="D6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -2384,10 +2687,16 @@
       <c r="G6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -2396,10 +2705,10 @@
         <v>33120000</v>
       </c>
       <c r="D7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F7" t="s">
         <v>24</v>
@@ -2407,10 +2716,16 @@
       <c r="G7" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -2419,7 +2734,7 @@
         <v>33140000</v>
       </c>
       <c r="D8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E8" t="s">
         <v>40</v>
@@ -2430,10 +2745,16 @@
       <c r="G8" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -2442,10 +2763,10 @@
         <v>33040000</v>
       </c>
       <c r="D9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F9" t="s">
         <v>24</v>
@@ -2453,10 +2774,16 @@
       <c r="G9" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -2465,7 +2792,7 @@
         <v>33170000</v>
       </c>
       <c r="D10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E10" t="s">
         <v>54</v>
@@ -2476,10 +2803,16 @@
       <c r="G10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -2488,10 +2821,10 @@
         <v>33060000</v>
       </c>
       <c r="D11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F11" t="s">
         <v>24</v>
@@ -2499,10 +2832,16 @@
       <c r="G11" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -2511,10 +2850,10 @@
         <v>33070000</v>
       </c>
       <c r="D12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F12" t="s">
         <v>24</v>
@@ -2522,10 +2861,16 @@
       <c r="G12" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -2534,10 +2879,10 @@
         <v>33080000</v>
       </c>
       <c r="D13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F13" t="s">
         <v>24</v>
@@ -2545,10 +2890,16 @@
       <c r="G13" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -2557,10 +2908,10 @@
         <v>33090000</v>
       </c>
       <c r="D14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F14" t="s">
         <v>24</v>
@@ -2568,10 +2919,16 @@
       <c r="G14" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -2580,10 +2937,10 @@
         <v>33100000</v>
       </c>
       <c r="D15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F15" t="s">
         <v>24</v>
@@ -2591,10 +2948,16 @@
       <c r="G15" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -2603,10 +2966,10 @@
         <v>33110000</v>
       </c>
       <c r="D16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F16" t="s">
         <v>24</v>
@@ -2614,10 +2977,16 @@
       <c r="G16" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -2626,16 +2995,22 @@
         <v>33010000</v>
       </c>
       <c r="D17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G17" t="s">
         <v>54</v>
+      </c>
+      <c r="H17" t="s">
+        <v>289</v>
+      </c>
+      <c r="I17" t="s">
+        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -2645,25 +3020,25 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F76D307B-9060-4C33-AF9D-2A846C2CA587}">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.54296875" customWidth="1"/>
-    <col min="5" max="5" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.5703125" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -2680,10 +3055,16 @@
       <c r="G1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H1" t="s">
+        <v>288</v>
+      </c>
+      <c r="I1" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2692,7 +3073,7 @@
         <v>34230000</v>
       </c>
       <c r="D2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E2" t="s">
         <v>54</v>
@@ -2703,10 +3084,16 @@
       <c r="G2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -2715,7 +3102,7 @@
         <v>34290000</v>
       </c>
       <c r="D3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E3" t="s">
         <v>54</v>
@@ -2726,10 +3113,16 @@
       <c r="G3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -2738,10 +3131,10 @@
         <v>34240000</v>
       </c>
       <c r="D4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F4" t="s">
         <v>24</v>
@@ -2749,10 +3142,16 @@
       <c r="G4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2761,21 +3160,27 @@
         <v>34010000</v>
       </c>
       <c r="D5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G5" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -2784,10 +3189,10 @@
         <v>34050000</v>
       </c>
       <c r="D6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F6" t="s">
         <v>54</v>
@@ -2795,10 +3200,16 @@
       <c r="G6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -2807,21 +3218,27 @@
         <v>34020000</v>
       </c>
       <c r="D7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -2830,21 +3247,27 @@
         <v>34320000</v>
       </c>
       <c r="D8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -2853,21 +3276,27 @@
         <v>34030000</v>
       </c>
       <c r="D9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -2876,21 +3305,27 @@
         <v>34040000</v>
       </c>
       <c r="D10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -2899,21 +3334,27 @@
         <v>34110000</v>
       </c>
       <c r="D11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E11" t="s">
         <v>54</v>
       </c>
       <c r="F11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -2922,21 +3363,27 @@
         <v>34120000</v>
       </c>
       <c r="D12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E12" t="s">
         <v>54</v>
       </c>
       <c r="F12" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -2945,21 +3392,27 @@
         <v>34130000</v>
       </c>
       <c r="D13" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E13" t="s">
         <v>54</v>
       </c>
       <c r="F13" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -2968,21 +3421,27 @@
         <v>34140000</v>
       </c>
       <c r="D14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E14" t="s">
         <v>54</v>
       </c>
       <c r="F14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -2991,21 +3450,27 @@
         <v>34070000</v>
       </c>
       <c r="D15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -3014,21 +3479,27 @@
         <v>34080000</v>
       </c>
       <c r="D16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -3037,10 +3508,10 @@
         <v>34100000</v>
       </c>
       <c r="D17" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -3048,10 +3519,16 @@
       <c r="G17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -3060,10 +3537,10 @@
         <v>34090000</v>
       </c>
       <c r="D18" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -3071,10 +3548,16 @@
       <c r="G18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -3083,10 +3566,10 @@
         <v>34160000</v>
       </c>
       <c r="D19" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E19" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F19" t="s">
         <v>24</v>
@@ -3094,10 +3577,16 @@
       <c r="G19" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -3106,10 +3595,10 @@
         <v>34170000</v>
       </c>
       <c r="D20" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E20" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F20" t="s">
         <v>24</v>
@@ -3117,10 +3606,16 @@
       <c r="G20" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -3129,10 +3624,10 @@
         <v>34180000</v>
       </c>
       <c r="D21" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E21" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F21" t="s">
         <v>24</v>
@@ -3140,10 +3635,16 @@
       <c r="G21" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -3152,10 +3653,10 @@
         <v>34190000</v>
       </c>
       <c r="D22" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E22" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F22" t="s">
         <v>24</v>
@@ -3163,10 +3664,16 @@
       <c r="G22" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -3175,10 +3682,10 @@
         <v>34220000</v>
       </c>
       <c r="D23" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E23" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F23" t="s">
         <v>24</v>
@@ -3186,10 +3693,16 @@
       <c r="G23" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -3198,10 +3711,10 @@
         <v>34200000</v>
       </c>
       <c r="D24" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E24" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F24" t="s">
         <v>24</v>
@@ -3209,10 +3722,16 @@
       <c r="G24" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -3221,16 +3740,22 @@
         <v>34210000</v>
       </c>
       <c r="D25" t="s">
+        <v>179</v>
+      </c>
+      <c r="E25" t="s">
         <v>180</v>
       </c>
-      <c r="E25" t="s">
-        <v>181</v>
-      </c>
       <c r="F25" t="s">
         <v>24</v>
       </c>
       <c r="G25" t="s">
         <v>54</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25" t="s">
+        <v>293</v>
       </c>
     </row>
   </sheetData>
@@ -3240,28 +3765,28 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85BB7FF7-82D6-482E-815B-F3751454FF7D}">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -3279,24 +3804,30 @@
         <v>25</v>
       </c>
       <c r="H1" t="s">
+        <v>187</v>
+      </c>
+      <c r="I1" t="s">
         <v>188</v>
       </c>
-      <c r="I1" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J1" t="s">
+        <v>288</v>
+      </c>
+      <c r="K1" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>35330000</v>
       </c>
       <c r="D2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E2" t="s">
         <v>54</v>
@@ -3308,24 +3839,30 @@
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>35320000</v>
       </c>
       <c r="D3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E3" t="s">
         <v>54</v>
@@ -3337,27 +3874,33 @@
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4">
         <v>35060000</v>
       </c>
       <c r="D4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F4" t="s">
         <v>24</v>
@@ -3366,24 +3909,30 @@
         <v>54</v>
       </c>
       <c r="H4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <v>35070000</v>
       </c>
       <c r="D5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E5" t="s">
         <v>54</v>
@@ -3395,56 +3944,68 @@
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="I5" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+        <v>195</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6">
         <v>35140000</v>
       </c>
       <c r="D6" t="s">
+        <v>213</v>
+      </c>
+      <c r="E6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
         <v>214</v>
       </c>
-      <c r="E6" t="s">
-        <v>54</v>
-      </c>
-      <c r="F6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6" t="s">
-        <v>215</v>
-      </c>
       <c r="I6" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+        <v>197</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7">
         <v>35040000</v>
       </c>
       <c r="D7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F7" t="s">
         <v>24</v>
@@ -3453,56 +4014,68 @@
         <v>54</v>
       </c>
       <c r="H7" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I7" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8">
         <v>35050000</v>
       </c>
       <c r="D8" t="s">
+        <v>204</v>
+      </c>
+      <c r="E8" t="s">
+        <v>192</v>
+      </c>
+      <c r="F8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" t="s">
+        <v>54</v>
+      </c>
+      <c r="H8" t="s">
+        <v>202</v>
+      </c>
+      <c r="I8" t="s">
         <v>205</v>
       </c>
-      <c r="E8" t="s">
-        <v>193</v>
-      </c>
-      <c r="F8" t="s">
-        <v>24</v>
-      </c>
-      <c r="G8" t="s">
-        <v>54</v>
-      </c>
-      <c r="H8" t="s">
-        <v>203</v>
-      </c>
-      <c r="I8" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9">
         <v>35020000</v>
       </c>
       <c r="D9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F9" t="s">
         <v>24</v>
@@ -3511,27 +4084,33 @@
         <v>54</v>
       </c>
       <c r="H9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I9" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+        <v>206</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10">
         <v>35030000</v>
       </c>
       <c r="D10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F10" t="s">
         <v>24</v>
@@ -3540,53 +4119,65 @@
         <v>54</v>
       </c>
       <c r="H10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I10" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+        <v>207</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11">
         <v>35150000</v>
       </c>
       <c r="D11" t="s">
+        <v>211</v>
+      </c>
+      <c r="E11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11" t="s">
         <v>212</v>
       </c>
-      <c r="E11" t="s">
-        <v>54</v>
-      </c>
-      <c r="F11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11" t="s">
-        <v>213</v>
-      </c>
       <c r="I11" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+        <v>208</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12">
         <v>35130000</v>
       </c>
       <c r="D12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E12" t="s">
         <v>54</v>
@@ -3601,56 +4192,68 @@
         <v>26</v>
       </c>
       <c r="I12" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+        <v>209</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13">
         <v>35140000</v>
       </c>
       <c r="D13" t="s">
+        <v>213</v>
+      </c>
+      <c r="E13" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13" t="s">
         <v>214</v>
       </c>
-      <c r="E13" t="s">
-        <v>54</v>
-      </c>
-      <c r="F13" t="s">
-        <v>24</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13" t="s">
-        <v>215</v>
-      </c>
       <c r="I13" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+        <v>210</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14">
         <v>35210000</v>
       </c>
       <c r="D14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -3658,25 +4261,31 @@
       <c r="I14" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15">
         <v>35220000</v>
       </c>
       <c r="D15" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E15" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F15" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -3684,10 +4293,16 @@
       <c r="I15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -3696,27 +4311,33 @@
         <v>35160000</v>
       </c>
       <c r="D16" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E16" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F16" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G16">
         <v>0</v>
       </c>
       <c r="H16" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I16" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+        <v>236</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -3725,181 +4346,217 @@
         <v>35170000</v>
       </c>
       <c r="D17" t="s">
+        <v>234</v>
+      </c>
+      <c r="E17" t="s">
+        <v>192</v>
+      </c>
+      <c r="F17" t="s">
+        <v>192</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17" t="s">
+        <v>237</v>
+      </c>
+      <c r="I17" t="s">
         <v>235</v>
       </c>
-      <c r="E17" t="s">
-        <v>193</v>
-      </c>
-      <c r="F17" t="s">
-        <v>193</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17" t="s">
-        <v>238</v>
-      </c>
-      <c r="I17" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18" s="2">
         <v>35340000</v>
       </c>
       <c r="D18" t="s">
+        <v>243</v>
+      </c>
+      <c r="E18" t="s">
+        <v>192</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18" t="s">
         <v>244</v>
       </c>
-      <c r="E18" t="s">
-        <v>193</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18" t="s">
-        <v>245</v>
-      </c>
       <c r="I18" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+        <v>246</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19" s="2">
         <v>35350000</v>
       </c>
       <c r="D19" t="s">
+        <v>249</v>
+      </c>
+      <c r="E19" t="s">
+        <v>54</v>
+      </c>
+      <c r="F19" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19" t="s">
+        <v>247</v>
+      </c>
+      <c r="I19" t="s">
+        <v>245</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>250</v>
       </c>
-      <c r="E19" t="s">
-        <v>54</v>
-      </c>
-      <c r="F19" t="s">
-        <v>24</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19" t="s">
-        <v>248</v>
-      </c>
-      <c r="I19" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>251</v>
-      </c>
       <c r="B20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20">
         <v>35190000</v>
       </c>
       <c r="D20" t="s">
+        <v>251</v>
+      </c>
+      <c r="E20" t="s">
+        <v>54</v>
+      </c>
+      <c r="F20" t="s">
+        <v>24</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20" t="s">
         <v>252</v>
       </c>
-      <c r="E20" t="s">
-        <v>54</v>
-      </c>
-      <c r="F20" t="s">
-        <v>24</v>
-      </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
         <v>253</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>255</v>
-      </c>
       <c r="B21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21">
         <v>35200000</v>
       </c>
       <c r="D21" t="s">
+        <v>257</v>
+      </c>
+      <c r="E21" t="s">
+        <v>54</v>
+      </c>
+      <c r="F21" t="s">
+        <v>24</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21" t="s">
+        <v>255</v>
+      </c>
+      <c r="I21" t="s">
+        <v>256</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>258</v>
       </c>
-      <c r="E21" t="s">
-        <v>54</v>
-      </c>
-      <c r="F21" t="s">
-        <v>24</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21" t="s">
-        <v>256</v>
-      </c>
-      <c r="I21" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>259</v>
-      </c>
       <c r="B22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" s="2">
         <v>35360000</v>
       </c>
       <c r="D22" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E22" t="s">
         <v>54</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G22">
         <v>0</v>
       </c>
       <c r="H22" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="I22" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+        <v>259</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23" s="2">
         <v>35370000</v>
       </c>
       <c r="D23" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E23" t="s">
         <v>54</v>
@@ -3911,44 +4568,56 @@
         <v>0</v>
       </c>
       <c r="H23" t="s">
+        <v>262</v>
+      </c>
+      <c r="I23" t="s">
         <v>263</v>
       </c>
-      <c r="I23" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C24" s="2">
         <v>35380000</v>
       </c>
       <c r="D24" t="s">
+        <v>267</v>
+      </c>
+      <c r="E24" t="s">
+        <v>54</v>
+      </c>
+      <c r="F24" t="s">
+        <v>24</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24" t="s">
         <v>268</v>
       </c>
-      <c r="E24" t="s">
-        <v>54</v>
-      </c>
-      <c r="F24" t="s">
-        <v>24</v>
-      </c>
-      <c r="G24">
-        <v>0</v>
-      </c>
-      <c r="H24" t="s">
+      <c r="I24" t="s">
         <v>269</v>
       </c>
-      <c r="I24" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -3957,10 +4626,10 @@
         <v>35230000</v>
       </c>
       <c r="D25" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E25" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F25" t="s">
         <v>40</v>
@@ -3972,50 +4641,62 @@
         <v>35</v>
       </c>
       <c r="I25" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+        <v>272</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C26" s="2">
         <v>35390000</v>
       </c>
       <c r="D26" t="s">
+        <v>273</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H26" t="s">
         <v>274</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="H26" t="s">
+      <c r="I26" t="s">
         <v>275</v>
       </c>
-      <c r="I26" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J26" t="s">
+        <v>289</v>
+      </c>
+      <c r="K26" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C27" s="2">
         <v>35410000</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E27" t="s">
         <v>54</v>
@@ -4027,10 +4708,16 @@
         <v>0</v>
       </c>
       <c r="H27" t="s">
+        <v>282</v>
+      </c>
+      <c r="I27" t="s">
         <v>283</v>
       </c>
-      <c r="I27" t="s">
-        <v>284</v>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27" t="s">
+        <v>293</v>
       </c>
     </row>
   </sheetData>
@@ -4042,493 +4729,517 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA629D80-511C-42AD-ACB3-22237E3BD282}">
   <dimension ref="A1:B69"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>58</v>
       </c>
       <c r="B14" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>62</v>
       </c>
       <c r="B15" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>63</v>
       </c>
       <c r="B16" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>74</v>
       </c>
       <c r="B17" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>79</v>
       </c>
       <c r="B18" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>70</v>
       </c>
       <c r="B19" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>72</v>
       </c>
       <c r="B20" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>68</v>
       </c>
       <c r="B21" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>66</v>
       </c>
       <c r="B22" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>76</v>
       </c>
       <c r="B23" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>103</v>
+      </c>
+      <c r="B24" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>104</v>
       </c>
-      <c r="B24" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+      <c r="B25" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>105</v>
       </c>
-      <c r="B25" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+      <c r="B26" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>106</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>107</v>
       </c>
-      <c r="B27" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+      <c r="B28" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>108</v>
       </c>
-      <c r="B28" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+      <c r="B29" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>109</v>
       </c>
-      <c r="B29" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+      <c r="B30" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>110</v>
       </c>
-      <c r="B30" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+      <c r="B31" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>111</v>
       </c>
-      <c r="B31" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
+      <c r="B32" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>112</v>
       </c>
-      <c r="B32" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>113</v>
-      </c>
       <c r="B33" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>130</v>
+      </c>
+      <c r="B34" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>131</v>
       </c>
-      <c r="B34" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
+      <c r="B35" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>155</v>
+      </c>
+      <c r="B36" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>132</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B37" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>147</v>
+      </c>
+      <c r="B38" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>156</v>
-      </c>
-      <c r="B36" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>148</v>
+      </c>
+      <c r="B39" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>149</v>
+      </c>
+      <c r="B40" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>150</v>
+      </c>
+      <c r="B41" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>151</v>
+      </c>
+      <c r="B42" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>152</v>
+      </c>
+      <c r="B43" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>153</v>
+      </c>
+      <c r="B44" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>133</v>
-      </c>
-      <c r="B37" t="s">
+      <c r="B45" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>189</v>
+      </c>
+      <c r="B46" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>220</v>
+      </c>
+      <c r="B47" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>148</v>
-      </c>
-      <c r="B38" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>149</v>
-      </c>
-      <c r="B39" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>150</v>
-      </c>
-      <c r="B40" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>151</v>
-      </c>
-      <c r="B41" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>152</v>
-      </c>
-      <c r="B42" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>153</v>
-      </c>
-      <c r="B43" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>154</v>
-      </c>
-      <c r="B44" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>187</v>
-      </c>
-      <c r="B45" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>195</v>
+      </c>
+      <c r="B48" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>198</v>
+      </c>
+      <c r="B49" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>190</v>
-      </c>
-      <c r="B46" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>219</v>
+      </c>
+      <c r="B50" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>221</v>
       </c>
-      <c r="B47" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>196</v>
-      </c>
-      <c r="B48" t="s">
+      <c r="B51" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>199</v>
-      </c>
-      <c r="B49" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>220</v>
-      </c>
-      <c r="B50" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>222</v>
       </c>
-      <c r="B51" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
+      <c r="B52" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>223</v>
       </c>
-      <c r="B52" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
+      <c r="B53" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>224</v>
       </c>
-      <c r="B53" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
+      <c r="B54" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>225</v>
       </c>
-      <c r="B54" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
-        <v>226</v>
-      </c>
       <c r="B55" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B56" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B57" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B58" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B59" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B60" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>31</v>
+      </c>
+      <c r="B61" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>286</v>
+      </c>
+      <c r="B62" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>290</v>
+      </c>
+      <c r="B63" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix for FTT-Fr csv generation
Fixing an issue with ZGAM not existing and a few other dimension problems with FTT-Fr
</commit_message>
<xml_diff>
--- a/Inputs/_MasterFiles/FTT_variables.xlsx
+++ b/Inputs/_MasterFiles/FTT_variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/f_j_m_m_nijsse_exeter_ac_uk/Documents/Documents/GitHub/FTT_StandAlone_laptop/FTT_StandAlone/Inputs/_MasterFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/cl852_exeter_ac_uk/Documents/Documents/GitHub/FTT_StandAlone/Inputs/_MasterFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="294" documentId="13_ncr:1_{B6AAC6B1-6F73-4CBC-BFCC-308507F8D1EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC775577-5634-4C66-940B-B6E76A5CD3E1}"/>
+  <xr:revisionPtr revIDLastSave="320" documentId="13_ncr:1_{B6AAC6B1-6F73-4CBC-BFCC-308507F8D1EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5FC304AD-5583-4324-A9F9-0480E273D876}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FTT-P" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="297">
   <si>
     <t>Variable name</t>
   </si>
@@ -927,6 +927,12 @@
   </si>
   <si>
     <t>FTT-Power regulations</t>
+  </si>
+  <si>
+    <t>ZGAM</t>
+  </si>
+  <si>
+    <t>tl_2019</t>
   </si>
 </sst>
 </file>
@@ -1277,16 +1283,16 @@
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.81640625" customWidth="1"/>
+    <col min="7" max="7" width="14.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1315,7 +1321,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1344,7 +1350,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>58</v>
       </c>
@@ -1373,7 +1379,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>62</v>
       </c>
@@ -1402,7 +1408,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>63</v>
       </c>
@@ -1431,7 +1437,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>74</v>
       </c>
@@ -1460,7 +1466,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>84</v>
       </c>
@@ -1489,7 +1495,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -1518,7 +1524,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>79</v>
       </c>
@@ -1547,7 +1553,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>70</v>
       </c>
@@ -1576,7 +1582,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>72</v>
       </c>
@@ -1605,7 +1611,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -1634,7 +1640,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>81</v>
       </c>
@@ -1663,7 +1669,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>88</v>
       </c>
@@ -1692,7 +1698,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>90</v>
       </c>
@@ -1721,7 +1727,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>80</v>
       </c>
@@ -1750,7 +1756,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>82</v>
       </c>
@@ -1779,7 +1785,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>66</v>
       </c>
@@ -1808,7 +1814,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>76</v>
       </c>
@@ -1852,18 +1858,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E04294AC-DBC1-4E51-84ED-2EC5066B9024}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.5703125" customWidth="1"/>
+    <col min="2" max="2" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1892,7 +1898,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1921,7 +1927,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1950,7 +1956,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1979,7 +1985,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2008,7 +2014,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -2037,7 +2043,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -2066,7 +2072,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -2095,7 +2101,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -2124,7 +2130,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -2153,7 +2159,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -2182,7 +2188,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -2211,7 +2217,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -2240,7 +2246,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -2269,7 +2275,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -2298,7 +2304,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -2327,7 +2333,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -2356,7 +2362,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -2385,7 +2391,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -2414,7 +2420,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -2443,7 +2449,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -2472,7 +2478,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>52</v>
       </c>
@@ -2514,13 +2520,13 @@
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.42578125" customWidth="1"/>
+    <col min="2" max="2" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2549,7 +2555,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>96</v>
       </c>
@@ -2578,7 +2584,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>99</v>
       </c>
@@ -2607,7 +2613,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>100</v>
       </c>
@@ -2636,7 +2642,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>101</v>
       </c>
@@ -2665,7 +2671,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>102</v>
       </c>
@@ -2694,7 +2700,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>103</v>
       </c>
@@ -2723,7 +2729,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>104</v>
       </c>
@@ -2752,7 +2758,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>105</v>
       </c>
@@ -2781,7 +2787,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>106</v>
       </c>
@@ -2810,7 +2816,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>107</v>
       </c>
@@ -2839,7 +2845,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>108</v>
       </c>
@@ -2868,7 +2874,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>109</v>
       </c>
@@ -2897,7 +2903,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>110</v>
       </c>
@@ -2926,7 +2932,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>111</v>
       </c>
@@ -2955,7 +2961,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>112</v>
       </c>
@@ -2984,7 +2990,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>113</v>
       </c>
@@ -3026,14 +3032,14 @@
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="50.5703125" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.54296875" customWidth="1"/>
+    <col min="5" max="5" width="9.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3062,7 +3068,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>131</v>
       </c>
@@ -3091,7 +3097,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>155</v>
       </c>
@@ -3120,7 +3126,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>132</v>
       </c>
@@ -3149,7 +3155,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>133</v>
       </c>
@@ -3178,7 +3184,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>134</v>
       </c>
@@ -3207,7 +3213,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>135</v>
       </c>
@@ -3236,7 +3242,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>136</v>
       </c>
@@ -3265,7 +3271,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>137</v>
       </c>
@@ -3294,7 +3300,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>138</v>
       </c>
@@ -3323,7 +3329,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>139</v>
       </c>
@@ -3352,7 +3358,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>140</v>
       </c>
@@ -3381,7 +3387,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>141</v>
       </c>
@@ -3410,7 +3416,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>142</v>
       </c>
@@ -3439,7 +3445,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>143</v>
       </c>
@@ -3468,7 +3474,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>144</v>
       </c>
@@ -3497,7 +3503,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>145</v>
       </c>
@@ -3526,7 +3532,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>146</v>
       </c>
@@ -3555,7 +3561,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>147</v>
       </c>
@@ -3584,7 +3590,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>148</v>
       </c>
@@ -3613,7 +3619,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>149</v>
       </c>
@@ -3642,7 +3648,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>150</v>
       </c>
@@ -3671,7 +3677,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>151</v>
       </c>
@@ -3700,7 +3706,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>152</v>
       </c>
@@ -3729,7 +3735,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>153</v>
       </c>
@@ -3767,21 +3773,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85BB7FF7-82D6-482E-815B-F3751454FF7D}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.54296875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3816,7 +3822,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>186</v>
       </c>
@@ -3851,7 +3857,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>189</v>
       </c>
@@ -3886,7 +3892,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>220</v>
       </c>
@@ -3921,7 +3927,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>195</v>
       </c>
@@ -3956,7 +3962,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>198</v>
       </c>
@@ -3991,7 +3997,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>219</v>
       </c>
@@ -4026,7 +4032,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>221</v>
       </c>
@@ -4061,7 +4067,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>222</v>
       </c>
@@ -4096,7 +4102,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>223</v>
       </c>
@@ -4131,7 +4137,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>224</v>
       </c>
@@ -4166,7 +4172,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>225</v>
       </c>
@@ -4201,7 +4207,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>215</v>
       </c>
@@ -4236,7 +4242,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>229</v>
       </c>
@@ -4268,7 +4274,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>231</v>
       </c>
@@ -4300,7 +4306,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>238</v>
       </c>
@@ -4335,7 +4341,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>239</v>
       </c>
@@ -4370,7 +4376,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>242</v>
       </c>
@@ -4405,7 +4411,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>248</v>
       </c>
@@ -4440,7 +4446,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>250</v>
       </c>
@@ -4475,7 +4481,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>254</v>
       </c>
@@ -4510,7 +4516,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>258</v>
       </c>
@@ -4545,7 +4551,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>264</v>
       </c>
@@ -4580,7 +4586,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>270</v>
       </c>
@@ -4615,7 +4621,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>266</v>
       </c>
@@ -4650,7 +4656,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>276</v>
       </c>
@@ -4685,7 +4691,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>281</v>
       </c>
@@ -4713,8 +4719,8 @@
       <c r="I27" t="s">
         <v>283</v>
       </c>
-      <c r="J27">
-        <v>0</v>
+      <c r="J27" t="s">
+        <v>24</v>
       </c>
       <c r="K27" t="s">
         <v>293</v>
@@ -4727,15 +4733,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA629D80-511C-42AD-ACB3-22237E3BD282}">
-  <dimension ref="A1:B69"/>
+  <dimension ref="A1:B70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66:B66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4743,7 +4749,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -4751,7 +4757,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -4759,7 +4765,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -4767,7 +4773,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -4775,7 +4781,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -4783,7 +4789,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -4791,7 +4797,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -4799,7 +4805,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -4807,7 +4813,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -4815,7 +4821,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -4823,7 +4829,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -4831,7 +4837,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -4839,7 +4845,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>58</v>
       </c>
@@ -4847,7 +4853,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>62</v>
       </c>
@@ -4855,7 +4861,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>63</v>
       </c>
@@ -4863,7 +4869,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>74</v>
       </c>
@@ -4871,7 +4877,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>79</v>
       </c>
@@ -4879,7 +4885,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>70</v>
       </c>
@@ -4887,7 +4893,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>72</v>
       </c>
@@ -4895,7 +4901,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>68</v>
       </c>
@@ -4903,7 +4909,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>66</v>
       </c>
@@ -4911,7 +4917,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>76</v>
       </c>
@@ -4919,7 +4925,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>103</v>
       </c>
@@ -4927,7 +4933,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>104</v>
       </c>
@@ -4935,7 +4941,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>105</v>
       </c>
@@ -4943,7 +4949,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>106</v>
       </c>
@@ -4951,7 +4957,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>107</v>
       </c>
@@ -4959,7 +4965,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>108</v>
       </c>
@@ -4967,7 +4973,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>109</v>
       </c>
@@ -4975,7 +4981,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>110</v>
       </c>
@@ -4983,7 +4989,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>111</v>
       </c>
@@ -4991,7 +4997,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>112</v>
       </c>
@@ -4999,7 +5005,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>130</v>
       </c>
@@ -5007,7 +5013,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>131</v>
       </c>
@@ -5015,7 +5021,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>155</v>
       </c>
@@ -5023,7 +5029,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>132</v>
       </c>
@@ -5031,7 +5037,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>147</v>
       </c>
@@ -5039,7 +5045,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>148</v>
       </c>
@@ -5047,7 +5053,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>149</v>
       </c>
@@ -5055,7 +5061,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>150</v>
       </c>
@@ -5063,7 +5069,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>151</v>
       </c>
@@ -5071,7 +5077,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>152</v>
       </c>
@@ -5079,7 +5085,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>153</v>
       </c>
@@ -5087,7 +5093,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>186</v>
       </c>
@@ -5095,7 +5101,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>189</v>
       </c>
@@ -5103,7 +5109,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>220</v>
       </c>
@@ -5111,7 +5117,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>195</v>
       </c>
@@ -5119,7 +5125,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>198</v>
       </c>
@@ -5127,7 +5133,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>219</v>
       </c>
@@ -5135,7 +5141,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>221</v>
       </c>
@@ -5143,7 +5149,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>222</v>
       </c>
@@ -5151,7 +5157,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>223</v>
       </c>
@@ -5159,7 +5165,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>224</v>
       </c>
@@ -5167,7 +5173,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>225</v>
       </c>
@@ -5175,7 +5181,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>215</v>
       </c>
@@ -5183,7 +5189,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>248</v>
       </c>
@@ -5191,7 +5197,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>250</v>
       </c>
@@ -5199,7 +5205,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>254</v>
       </c>
@@ -5207,7 +5213,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>270</v>
       </c>
@@ -5215,7 +5221,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>31</v>
       </c>
@@ -5223,7 +5229,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>286</v>
       </c>
@@ -5231,7 +5237,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>290</v>
       </c>
@@ -5239,8 +5245,24 @@
         <v>287</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="3"/>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>295</v>
+      </c>
+      <c r="B64" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>281</v>
+      </c>
+      <c r="B65" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A70" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Change HEWF to S0 only
HEWF should not change between scenarios. Therefore, it has been changed to just output for the S0 scenario.
</commit_message>
<xml_diff>
--- a/Inputs/_MasterFiles/FTT_variables.xlsx
+++ b/Inputs/_MasterFiles/FTT_variables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/cl852_exeter_ac_uk/Documents/Documents/GitHub/FTT_StandAlone/Inputs/_MasterFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{96C6DCC7-F135-4F9F-BBD1-97530C10B60C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44E33A8A-4BEB-4D28-B5D1-EE55F2A2093E}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{96C6DCC7-F135-4F9F-BBD1-97530C10B60C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{771B7194-D847-4D0A-A393-E2F94739CDC5}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FTT-P" sheetId="1" r:id="rId1"/>
@@ -1279,7 +1279,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -1858,8 +1858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E04294AC-DBC1-4E51-84ED-2EC5066B9024}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2516,8 +2516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{893746F0-70F0-4C21-8E46-9B5DBA6E54BB}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:I6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2784,7 +2784,7 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -2813,7 +2813,7 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -4735,7 +4735,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA629D80-511C-42AD-ACB3-22237E3BD282}">
   <dimension ref="A1:B66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+    <sheetView topLeftCell="A55" workbookViewId="0">
       <selection activeCell="H71" sqref="H71"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Changes to freight fuel tax
Fuel tax was not working properly before in FTT-Fr. Renamed fuel tax variable to 'RZFT'. Units now $/MJ rather than $/litre. I think FTT-Tr units maybe be wrong on this.

Added categories for taxable fuel categories in the source code. Added variables to see purchase cost and fuel cost inclusive of subsidy/tax in the front end.
</commit_message>
<xml_diff>
--- a/Inputs/_MasterFiles/FTT_variables.xlsx
+++ b/Inputs/_MasterFiles/FTT_variables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/cl852_exeter_ac_uk/Documents/Documents/GitHub/FTT_StandAlone/Inputs/_MasterFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{96C6DCC7-F135-4F9F-BBD1-97530C10B60C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4BFEED6-38BC-496D-A115-2ACEDB4D7D32}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{96C6DCC7-F135-4F9F-BBD1-97530C10B60C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{633FC2CE-8022-472C-9BE9-1C2649AABB15}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FTT-P" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="287">
   <si>
     <t>Variable name</t>
   </si>
@@ -638,9 +638,6 @@
     <t>RTFT0</t>
   </si>
   <si>
-    <t>RTFZ0</t>
-  </si>
-  <si>
     <t>FTT-Fr Registration carbon tax in $/(gCO2/km)</t>
   </si>
   <si>
@@ -674,9 +671,6 @@
     <t>RTCO0</t>
   </si>
   <si>
-    <t>RTFT1</t>
-  </si>
-  <si>
     <t>FTT-Fr Biofuel blending mandate</t>
   </si>
   <si>
@@ -689,9 +683,6 @@
     <t>FT</t>
   </si>
   <si>
-    <t>RTFZ1</t>
-  </si>
-  <si>
     <t>VT</t>
   </si>
   <si>
@@ -909,6 +900,9 @@
   </si>
   <si>
     <t>tl_2019</t>
+  </si>
+  <si>
+    <t>RZFT</t>
   </si>
 </sst>
 </file>
@@ -1277,10 +1271,10 @@
         <v>25</v>
       </c>
       <c r="H1" t="s">
+        <v>277</v>
+      </c>
+      <c r="I1" t="s">
         <v>280</v>
-      </c>
-      <c r="I1" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
@@ -1309,7 +1303,7 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -1338,7 +1332,7 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -1367,7 +1361,7 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -1396,7 +1390,7 @@
         <v>24</v>
       </c>
       <c r="I5" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -1425,7 +1419,7 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
@@ -1454,7 +1448,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -1483,7 +1477,7 @@
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -1497,7 +1491,7 @@
         <v>31090000</v>
       </c>
       <c r="D9" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="E9" t="s">
         <v>56</v>
@@ -1512,7 +1506,7 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -1541,7 +1535,7 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -1570,7 +1564,7 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
@@ -1599,7 +1593,7 @@
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
@@ -1628,7 +1622,7 @@
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
@@ -1657,7 +1651,7 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
@@ -1686,7 +1680,7 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
@@ -1715,7 +1709,7 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
@@ -1744,7 +1738,7 @@
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
@@ -1773,7 +1767,7 @@
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
@@ -1802,7 +1796,7 @@
         <v>0</v>
       </c>
       <c r="I19" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -1854,10 +1848,10 @@
         <v>25</v>
       </c>
       <c r="H1" t="s">
+        <v>277</v>
+      </c>
+      <c r="I1" t="s">
         <v>280</v>
-      </c>
-      <c r="I1" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
@@ -1883,10 +1877,10 @@
         <v>54</v>
       </c>
       <c r="H2" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="I2" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -1915,7 +1909,7 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -1944,7 +1938,7 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -1973,7 +1967,7 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -2002,7 +1996,7 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
@@ -2031,7 +2025,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -2060,7 +2054,7 @@
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -2089,7 +2083,7 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -2118,7 +2112,7 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -2147,7 +2141,7 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
@@ -2176,7 +2170,7 @@
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
@@ -2205,7 +2199,7 @@
         <v>24</v>
       </c>
       <c r="I13" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
@@ -2234,7 +2228,7 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
@@ -2263,7 +2257,7 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
@@ -2292,7 +2286,7 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
@@ -2321,7 +2315,7 @@
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
@@ -2350,7 +2344,7 @@
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
@@ -2379,7 +2373,7 @@
         <v>0</v>
       </c>
       <c r="I19" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
@@ -2408,7 +2402,7 @@
         <v>0</v>
       </c>
       <c r="I20" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
@@ -2437,7 +2431,7 @@
         <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
@@ -2466,7 +2460,7 @@
         <v>0</v>
       </c>
       <c r="I22" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -2511,10 +2505,10 @@
         <v>25</v>
       </c>
       <c r="H1" t="s">
+        <v>277</v>
+      </c>
+      <c r="I1" t="s">
         <v>280</v>
-      </c>
-      <c r="I1" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
@@ -2543,7 +2537,7 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -2572,7 +2566,7 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -2601,7 +2595,7 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -2630,7 +2624,7 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -2659,7 +2653,7 @@
         <v>24</v>
       </c>
       <c r="I6" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
@@ -2688,7 +2682,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -2717,7 +2711,7 @@
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -2746,7 +2740,7 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -2775,7 +2769,7 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -2804,7 +2798,7 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
@@ -2833,7 +2827,7 @@
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
@@ -2862,7 +2856,7 @@
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
@@ -2891,7 +2885,7 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
@@ -2920,7 +2914,7 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
@@ -2949,7 +2943,7 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
@@ -2975,10 +2969,10 @@
         <v>54</v>
       </c>
       <c r="H17" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="I17" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -3024,10 +3018,10 @@
         <v>25</v>
       </c>
       <c r="H1" t="s">
+        <v>277</v>
+      </c>
+      <c r="I1" t="s">
         <v>280</v>
-      </c>
-      <c r="I1" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
@@ -3056,7 +3050,7 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -3085,7 +3079,7 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -3114,7 +3108,7 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -3143,7 +3137,7 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -3172,7 +3166,7 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
@@ -3201,7 +3195,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -3230,7 +3224,7 @@
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -3259,7 +3253,7 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -3288,7 +3282,7 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -3317,7 +3311,7 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
@@ -3346,7 +3340,7 @@
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
@@ -3375,7 +3369,7 @@
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
@@ -3404,7 +3398,7 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
@@ -3433,7 +3427,7 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
@@ -3462,7 +3456,7 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
@@ -3491,7 +3485,7 @@
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
@@ -3520,7 +3514,7 @@
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
@@ -3549,7 +3543,7 @@
         <v>0</v>
       </c>
       <c r="I19" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
@@ -3578,7 +3572,7 @@
         <v>0</v>
       </c>
       <c r="I20" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
@@ -3607,7 +3601,7 @@
         <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
@@ -3636,7 +3630,7 @@
         <v>0</v>
       </c>
       <c r="I22" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
@@ -3665,7 +3659,7 @@
         <v>0</v>
       </c>
       <c r="I23" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
@@ -3694,7 +3688,7 @@
         <v>0</v>
       </c>
       <c r="I24" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
@@ -3723,7 +3717,7 @@
         <v>0</v>
       </c>
       <c r="I25" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -3733,10 +3727,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85BB7FF7-82D6-482E-815B-F3751454FF7D}">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3778,10 +3772,10 @@
         <v>188</v>
       </c>
       <c r="J1" t="s">
+        <v>277</v>
+      </c>
+      <c r="K1" t="s">
         <v>280</v>
-      </c>
-      <c r="K1" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
@@ -3816,7 +3810,7 @@
         <v>0</v>
       </c>
       <c r="K2" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
@@ -3851,12 +3845,12 @@
         <v>0</v>
       </c>
       <c r="K3" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3877,7 +3871,7 @@
         <v>54</v>
       </c>
       <c r="H4" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="I4" t="s">
         <v>14</v>
@@ -3886,7 +3880,7 @@
         <v>0</v>
       </c>
       <c r="K4" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
@@ -3900,7 +3894,7 @@
         <v>35070000</v>
       </c>
       <c r="D5" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E5" t="s">
         <v>54</v>
@@ -3912,7 +3906,7 @@
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="I5" t="s">
         <v>195</v>
@@ -3921,12 +3915,12 @@
         <v>0</v>
       </c>
       <c r="K5" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>198</v>
+        <v>286</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3935,7 +3929,7 @@
         <v>35140000</v>
       </c>
       <c r="D6" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E6" t="s">
         <v>54</v>
@@ -3947,7 +3941,7 @@
         <v>0</v>
       </c>
       <c r="H6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I6" t="s">
         <v>197</v>
@@ -3956,12 +3950,12 @@
         <v>0</v>
       </c>
       <c r="K6" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3970,7 +3964,7 @@
         <v>35040000</v>
       </c>
       <c r="D7" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E7" t="s">
         <v>192</v>
@@ -3982,21 +3976,21 @@
         <v>54</v>
       </c>
       <c r="H7" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="I7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J7">
         <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -4005,7 +3999,7 @@
         <v>35050000</v>
       </c>
       <c r="D8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E8" t="s">
         <v>192</v>
@@ -4017,21 +4011,21 @@
         <v>54</v>
       </c>
       <c r="H8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J8">
         <v>0</v>
       </c>
       <c r="K8" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -4040,7 +4034,7 @@
         <v>35020000</v>
       </c>
       <c r="D9" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="E9" t="s">
         <v>192</v>
@@ -4052,21 +4046,21 @@
         <v>54</v>
       </c>
       <c r="H9" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="I9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J9">
         <v>0</v>
       </c>
       <c r="K9" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -4075,7 +4069,7 @@
         <v>35030000</v>
       </c>
       <c r="D10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E10" t="s">
         <v>192</v>
@@ -4087,21 +4081,21 @@
         <v>54</v>
       </c>
       <c r="H10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J10">
         <v>0</v>
       </c>
       <c r="K10" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -4110,7 +4104,7 @@
         <v>35150000</v>
       </c>
       <c r="D11" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E11" t="s">
         <v>54</v>
@@ -4122,21 +4116,21 @@
         <v>0</v>
       </c>
       <c r="H11" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="I11" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J11">
         <v>0</v>
       </c>
       <c r="K11" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -4145,7 +4139,7 @@
         <v>35130000</v>
       </c>
       <c r="D12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E12" t="s">
         <v>54</v>
@@ -4160,62 +4154,62 @@
         <v>26</v>
       </c>
       <c r="I12" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="J12">
         <v>0</v>
       </c>
       <c r="K12" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>215</v>
+        <v>231</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13">
-        <v>35140000</v>
+        <v>35160000</v>
       </c>
       <c r="D13" t="s">
-        <v>213</v>
+        <v>234</v>
       </c>
       <c r="E13" t="s">
-        <v>54</v>
+        <v>192</v>
       </c>
       <c r="F13" t="s">
-        <v>24</v>
+        <v>192</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
       <c r="H13" t="s">
-        <v>214</v>
+        <v>233</v>
       </c>
       <c r="I13" t="s">
-        <v>210</v>
+        <v>229</v>
       </c>
       <c r="J13">
         <v>0</v>
       </c>
       <c r="K13" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14">
-        <v>35160000</v>
+        <v>35170000</v>
       </c>
       <c r="D14" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="E14" t="s">
         <v>192</v>
@@ -4227,100 +4221,100 @@
         <v>0</v>
       </c>
       <c r="H14" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="I14" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="J14">
         <v>0</v>
       </c>
       <c r="K14" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>237</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>35350000</v>
+      </c>
+      <c r="D15" t="s">
+        <v>238</v>
+      </c>
+      <c r="E15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15" t="s">
+        <v>236</v>
+      </c>
+      <c r="I15" t="s">
         <v>235</v>
       </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15">
-        <v>35170000</v>
-      </c>
-      <c r="D15" t="s">
-        <v>230</v>
-      </c>
-      <c r="E15" t="s">
-        <v>192</v>
-      </c>
-      <c r="F15" t="s">
-        <v>192</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15" t="s">
-        <v>233</v>
-      </c>
-      <c r="I15" t="s">
-        <v>231</v>
-      </c>
       <c r="J15">
         <v>0</v>
       </c>
       <c r="K15" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>239</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>35190000</v>
+      </c>
+      <c r="D16" t="s">
         <v>240</v>
       </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16">
-        <v>35350000</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" t="s">
+        <v>24</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16" t="s">
         <v>241</v>
       </c>
-      <c r="E16" t="s">
-        <v>54</v>
-      </c>
-      <c r="F16" t="s">
-        <v>24</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="H16" t="s">
-        <v>239</v>
-      </c>
       <c r="I16" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="J16">
         <v>0</v>
       </c>
       <c r="K16" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17">
-        <v>35190000</v>
+        <v>35200000</v>
       </c>
       <c r="D17" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="E17" t="s">
         <v>54</v>
@@ -4341,33 +4335,33 @@
         <v>0</v>
       </c>
       <c r="K17" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18">
-        <v>35200000</v>
+        <v>35360000</v>
       </c>
       <c r="D18" t="s">
+        <v>250</v>
+      </c>
+      <c r="E18" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" t="s">
+        <v>266</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18" t="s">
         <v>249</v>
-      </c>
-      <c r="E18" t="s">
-        <v>54</v>
-      </c>
-      <c r="F18" t="s">
-        <v>24</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18" t="s">
-        <v>247</v>
       </c>
       <c r="I18" t="s">
         <v>248</v>
@@ -4376,103 +4370,103 @@
         <v>0</v>
       </c>
       <c r="K18" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19">
-        <v>35360000</v>
+        <v>35370000</v>
       </c>
       <c r="D19" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="E19" t="s">
         <v>54</v>
       </c>
-      <c r="F19" t="s">
-        <v>269</v>
+      <c r="F19">
+        <v>0</v>
       </c>
       <c r="G19">
         <v>0</v>
       </c>
       <c r="H19" t="s">
+        <v>251</v>
+      </c>
+      <c r="I19" t="s">
         <v>252</v>
       </c>
-      <c r="I19" t="s">
-        <v>251</v>
-      </c>
       <c r="J19">
         <v>0</v>
       </c>
       <c r="K19" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
+        <v>259</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>35380000</v>
+      </c>
+      <c r="D20" t="s">
         <v>256</v>
       </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20">
-        <v>35370000</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
+        <v>54</v>
+      </c>
+      <c r="F20" t="s">
+        <v>24</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20" t="s">
         <v>257</v>
       </c>
-      <c r="E20" t="s">
-        <v>54</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20" t="s">
-        <v>254</v>
-      </c>
       <c r="I20" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="J20">
         <v>0</v>
       </c>
       <c r="K20" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21">
-        <v>35380000</v>
+        <v>35230000</v>
       </c>
       <c r="D21" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E21" t="s">
-        <v>54</v>
+        <v>192</v>
       </c>
       <c r="F21" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="G21">
         <v>0</v>
       </c>
       <c r="H21" t="s">
-        <v>260</v>
+        <v>35</v>
       </c>
       <c r="I21" t="s">
         <v>261</v>
@@ -4481,112 +4475,77 @@
         <v>0</v>
       </c>
       <c r="K21" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>258</v>
+        <v>265</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22">
-        <v>35230000</v>
+        <v>35390000</v>
       </c>
       <c r="D22" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E22" t="s">
         <v>192</v>
       </c>
       <c r="F22" t="s">
-        <v>40</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
+        <v>267</v>
+      </c>
+      <c r="G22" t="s">
+        <v>54</v>
       </c>
       <c r="H22" t="s">
-        <v>35</v>
+        <v>263</v>
       </c>
       <c r="I22" t="s">
         <v>264</v>
       </c>
-      <c r="J22">
-        <v>0</v>
+      <c r="J22" t="s">
+        <v>278</v>
       </c>
       <c r="K22" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23">
-        <v>35390000</v>
+        <v>35410000</v>
       </c>
       <c r="D23" t="s">
-        <v>265</v>
+        <v>273</v>
       </c>
       <c r="E23" t="s">
-        <v>192</v>
-      </c>
-      <c r="F23" t="s">
-        <v>270</v>
-      </c>
-      <c r="G23" t="s">
-        <v>54</v>
+        <v>54</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
       </c>
       <c r="H23" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="I23" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="J23" t="s">
-        <v>281</v>
+        <v>24</v>
       </c>
       <c r="K23" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>273</v>
-      </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="C24">
-        <v>35410000</v>
-      </c>
-      <c r="D24" t="s">
-        <v>276</v>
-      </c>
-      <c r="E24" t="s">
-        <v>54</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-      <c r="G24">
-        <v>0</v>
-      </c>
-      <c r="H24" t="s">
-        <v>274</v>
-      </c>
-      <c r="I24" t="s">
-        <v>275</v>
-      </c>
-      <c r="J24" t="s">
-        <v>24</v>
-      </c>
-      <c r="K24" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -4596,10 +4555,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA629D80-511C-42AD-ACB3-22237E3BD282}">
-  <dimension ref="A1:B66"/>
+  <dimension ref="A1:B65"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="H71" sqref="H71"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4961,7 +4920,7 @@
         <v>186</v>
       </c>
       <c r="B45" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
@@ -4969,12 +4928,12 @@
         <v>189</v>
       </c>
       <c r="B46" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B47" t="s">
         <v>95</v>
@@ -4985,76 +4944,76 @@
         <v>195</v>
       </c>
       <c r="B48" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>198</v>
+        <v>286</v>
       </c>
       <c r="B49" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B50" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B51" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B52" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B53" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B54" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B55" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>215</v>
+        <v>237</v>
       </c>
       <c r="B56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B57" t="s">
         <v>94</v>
@@ -5062,7 +5021,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B58" t="s">
         <v>94</v>
@@ -5070,7 +5029,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>246</v>
+        <v>259</v>
       </c>
       <c r="B59" t="s">
         <v>94</v>
@@ -5078,58 +5037,50 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>262</v>
+        <v>31</v>
       </c>
       <c r="B60" t="s">
-        <v>94</v>
+        <v>274</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>31</v>
+        <v>275</v>
       </c>
       <c r="B61" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B62" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B63" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>287</v>
+        <v>270</v>
       </c>
       <c r="B64" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>273</v>
+        <v>102</v>
       </c>
       <c r="B65" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A66" t="s">
-        <v>102</v>
-      </c>
-      <c r="B66" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RTFS variable added and working
</commit_message>
<xml_diff>
--- a/Inputs/_MasterFiles/FTT_variables.xlsx
+++ b/Inputs/_MasterFiles/FTT_variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/cl852_exeter_ac_uk/Documents/Documents/GitHub/FTT_StandAlone/Inputs/_MasterFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb614170\FTT_StandAlone\Inputs\_MasterFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{96C6DCC7-F135-4F9F-BBD1-97530C10B60C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{771B7194-D847-4D0A-A393-E2F94739CDC5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA0FE0CA-7E66-4B51-BF93-1EE2C1AB2D7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FTT-P" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="299">
   <si>
     <t>Variable name</t>
   </si>
@@ -933,6 +933,12 @@
   </si>
   <si>
     <t>tl_2019</t>
+  </si>
+  <si>
+    <t>RTFS</t>
+  </si>
+  <si>
+    <t>FTT-Tr Fossil Fuel Subsidy Phase Out</t>
   </si>
 </sst>
 </file>
@@ -1856,10 +1862,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E04294AC-DBC1-4E51-84ED-2EC5066B9024}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2507,6 +2513,35 @@
         <v>292</v>
       </c>
     </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>297</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>32350000</v>
+      </c>
+      <c r="D23" t="s">
+        <v>298</v>
+      </c>
+      <c r="E23" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" t="s">
+        <v>24</v>
+      </c>
+      <c r="G23" t="s">
+        <v>54</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23" t="s">
+        <v>292</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2516,7 +2551,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{893746F0-70F0-4C21-8E46-9B5DBA6E54BB}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
@@ -4733,10 +4768,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA629D80-511C-42AD-ACB3-22237E3BD282}">
-  <dimension ref="A1:B66"/>
+  <dimension ref="A1:B67"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="H71" sqref="H71"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5269,6 +5304,14 @@
         <v>287</v>
       </c>
     </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>297</v>
+      </c>
+      <c r="B67" t="s">
+        <v>95</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixing input file errors + tidy FTT_S_main
Some changes to the dimensions of variables in variablelisting.csv to ensure files are read in. Minor changes to formatting of FTT_S_main. No errors in reading variables. Code runs for FTT-Steel. Output not checked.
</commit_message>
<xml_diff>
--- a/Inputs/_MasterFiles/FTT_variables.xlsx
+++ b/Inputs/_MasterFiles/FTT_variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/cl852_exeter_ac_uk/Documents/Documents/GitHub/FTT_StandAlone/Inputs/_MasterFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{96C6DCC7-F135-4F9F-BBD1-97530C10B60C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{771B7194-D847-4D0A-A393-E2F94739CDC5}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="13_ncr:1_{96C6DCC7-F135-4F9F-BBD1-97530C10B60C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D352B917-055F-4966-AAA9-33ACE560BE59}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FTT-P" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="298">
   <si>
     <t>Variable name</t>
   </si>
@@ -933,6 +933,9 @@
   </si>
   <si>
     <t>tl_2019</t>
+  </si>
+  <si>
+    <t>tl_2010</t>
   </si>
 </sst>
 </file>
@@ -1858,8 +1861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E04294AC-DBC1-4E51-84ED-2EC5066B9024}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2516,7 +2519,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{893746F0-70F0-4C21-8E46-9B5DBA6E54BB}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
@@ -3029,7 +3032,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3525,8 +3528,8 @@
       <c r="G17">
         <v>0</v>
       </c>
-      <c r="H17">
-        <v>0</v>
+      <c r="H17" t="s">
+        <v>24</v>
       </c>
       <c r="I17" t="s">
         <v>292</v>
@@ -3554,8 +3557,8 @@
       <c r="G18">
         <v>0</v>
       </c>
-      <c r="H18">
-        <v>0</v>
+      <c r="H18" t="s">
+        <v>24</v>
       </c>
       <c r="I18" t="s">
         <v>292</v>
@@ -3773,8 +3776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85BB7FF7-82D6-482E-815B-F3751454FF7D}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4733,10 +4736,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA629D80-511C-42AD-ACB3-22237E3BD282}">
-  <dimension ref="A1:B66"/>
+  <dimension ref="A1:B68"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="H71" sqref="H71"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5269,6 +5272,22 @@
         <v>287</v>
       </c>
     </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>146</v>
+      </c>
+      <c r="B67" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>145</v>
+      </c>
+      <c r="B68" t="s">
+        <v>297</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Get gamma values as separate csv file
</commit_message>
<xml_diff>
--- a/Inputs/_MasterFiles/FTT_variables.xlsx
+++ b/Inputs/_MasterFiles/FTT_variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/cl852_exeter_ac_uk/Documents/Documents/GitHub/FTT_StandAlone/Inputs/_MasterFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/f_j_m_m_nijsse_exeter_ac_uk/Documents/Documents/GitHub/FTT_StandAlone_laptop_repos/FTT_StandAlone/Inputs/_MasterFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{96C6DCC7-F135-4F9F-BBD1-97530C10B60C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{771B7194-D847-4D0A-A393-E2F94739CDC5}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{96C6DCC7-F135-4F9F-BBD1-97530C10B60C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CBFF8A9F-2F92-4DFD-840D-86D8450A3184}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FTT-P" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="299">
   <si>
     <t>Variable name</t>
   </si>
@@ -933,6 +933,12 @@
   </si>
   <si>
     <t>tl_2019</t>
+  </si>
+  <si>
+    <t>SGAM</t>
+  </si>
+  <si>
+    <t>tl_2011</t>
   </si>
 </sst>
 </file>
@@ -1012,6 +1018,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1283,16 +1293,16 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="12.81640625" customWidth="1"/>
-    <col min="7" max="7" width="14.453125" customWidth="1"/>
+    <col min="6" max="6" width="12.77734375" customWidth="1"/>
+    <col min="7" max="7" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1321,7 +1331,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1350,7 +1360,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>58</v>
       </c>
@@ -1379,7 +1389,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>62</v>
       </c>
@@ -1408,7 +1418,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>63</v>
       </c>
@@ -1437,7 +1447,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>74</v>
       </c>
@@ -1466,7 +1476,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>84</v>
       </c>
@@ -1495,7 +1505,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -1524,7 +1534,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>79</v>
       </c>
@@ -1553,7 +1563,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>70</v>
       </c>
@@ -1582,7 +1592,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>72</v>
       </c>
@@ -1611,7 +1621,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -1640,7 +1650,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>81</v>
       </c>
@@ -1669,7 +1679,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>88</v>
       </c>
@@ -1698,7 +1708,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>90</v>
       </c>
@@ -1727,7 +1737,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>80</v>
       </c>
@@ -1756,7 +1766,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>82</v>
       </c>
@@ -1785,7 +1795,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>66</v>
       </c>
@@ -1814,7 +1824,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>76</v>
       </c>
@@ -1858,18 +1868,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E04294AC-DBC1-4E51-84ED-2EC5066B9024}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.54296875" customWidth="1"/>
+    <col min="2" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1898,7 +1908,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1927,7 +1937,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1956,7 +1966,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1985,7 +1995,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2014,7 +2024,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -2043,7 +2053,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -2072,7 +2082,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -2101,7 +2111,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -2130,7 +2140,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -2159,7 +2169,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -2188,7 +2198,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -2217,7 +2227,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -2246,7 +2256,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -2275,7 +2285,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -2304,7 +2314,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -2333,7 +2343,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -2362,7 +2372,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -2391,7 +2401,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -2420,7 +2430,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -2449,7 +2459,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -2478,7 +2488,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>52</v>
       </c>
@@ -2516,17 +2526,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{893746F0-70F0-4C21-8E46-9B5DBA6E54BB}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.453125" customWidth="1"/>
+    <col min="2" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2555,7 +2565,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>96</v>
       </c>
@@ -2584,7 +2594,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>99</v>
       </c>
@@ -2613,7 +2623,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>100</v>
       </c>
@@ -2642,7 +2652,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>101</v>
       </c>
@@ -2671,7 +2681,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>102</v>
       </c>
@@ -2700,7 +2710,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>103</v>
       </c>
@@ -2729,7 +2739,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>104</v>
       </c>
@@ -2758,7 +2768,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>105</v>
       </c>
@@ -2787,7 +2797,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>106</v>
       </c>
@@ -2816,7 +2826,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>107</v>
       </c>
@@ -2845,7 +2855,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>108</v>
       </c>
@@ -2874,7 +2884,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>109</v>
       </c>
@@ -2903,7 +2913,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>110</v>
       </c>
@@ -2932,7 +2942,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>111</v>
       </c>
@@ -2961,7 +2971,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>112</v>
       </c>
@@ -2990,7 +3000,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>113</v>
       </c>
@@ -3029,17 +3039,17 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="50.54296875" customWidth="1"/>
-    <col min="5" max="5" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.5546875" customWidth="1"/>
+    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3068,7 +3078,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>131</v>
       </c>
@@ -3097,7 +3107,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>155</v>
       </c>
@@ -3126,7 +3136,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>132</v>
       </c>
@@ -3155,7 +3165,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>133</v>
       </c>
@@ -3177,14 +3187,14 @@
       <c r="G5" t="s">
         <v>54</v>
       </c>
-      <c r="H5">
-        <v>0</v>
+      <c r="H5" t="s">
+        <v>289</v>
       </c>
       <c r="I5" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>134</v>
       </c>
@@ -3213,7 +3223,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>135</v>
       </c>
@@ -3242,7 +3252,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>136</v>
       </c>
@@ -3271,7 +3281,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>137</v>
       </c>
@@ -3300,7 +3310,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>138</v>
       </c>
@@ -3329,7 +3339,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>139</v>
       </c>
@@ -3358,7 +3368,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>140</v>
       </c>
@@ -3387,7 +3397,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>141</v>
       </c>
@@ -3416,7 +3426,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>142</v>
       </c>
@@ -3445,7 +3455,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>143</v>
       </c>
@@ -3474,7 +3484,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>144</v>
       </c>
@@ -3503,7 +3513,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>145</v>
       </c>
@@ -3532,7 +3542,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>146</v>
       </c>
@@ -3561,7 +3571,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>147</v>
       </c>
@@ -3590,7 +3600,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>148</v>
       </c>
@@ -3619,7 +3629,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>149</v>
       </c>
@@ -3648,7 +3658,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>150</v>
       </c>
@@ -3677,7 +3687,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>151</v>
       </c>
@@ -3706,7 +3716,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>152</v>
       </c>
@@ -3735,7 +3745,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>153</v>
       </c>
@@ -3777,17 +3787,17 @@
       <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3822,7 +3832,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>186</v>
       </c>
@@ -3857,7 +3867,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>189</v>
       </c>
@@ -3892,7 +3902,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>220</v>
       </c>
@@ -3927,7 +3937,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>195</v>
       </c>
@@ -3962,7 +3972,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>198</v>
       </c>
@@ -3997,7 +4007,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>219</v>
       </c>
@@ -4032,7 +4042,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>221</v>
       </c>
@@ -4067,7 +4077,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>222</v>
       </c>
@@ -4102,7 +4112,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>223</v>
       </c>
@@ -4137,7 +4147,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>224</v>
       </c>
@@ -4172,7 +4182,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>225</v>
       </c>
@@ -4207,7 +4217,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>215</v>
       </c>
@@ -4242,7 +4252,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>229</v>
       </c>
@@ -4274,7 +4284,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>231</v>
       </c>
@@ -4306,7 +4316,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>238</v>
       </c>
@@ -4341,7 +4351,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>239</v>
       </c>
@@ -4376,7 +4386,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>242</v>
       </c>
@@ -4411,7 +4421,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>248</v>
       </c>
@@ -4446,7 +4456,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>250</v>
       </c>
@@ -4481,7 +4491,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>254</v>
       </c>
@@ -4516,7 +4526,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>258</v>
       </c>
@@ -4551,7 +4561,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>264</v>
       </c>
@@ -4586,7 +4596,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>270</v>
       </c>
@@ -4621,7 +4631,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>266</v>
       </c>
@@ -4656,7 +4666,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>276</v>
       </c>
@@ -4691,7 +4701,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>281</v>
       </c>
@@ -4733,15 +4743,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA629D80-511C-42AD-ACB3-22237E3BD282}">
-  <dimension ref="A1:B66"/>
+  <dimension ref="A1:B67"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="H71" sqref="H71"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4749,7 +4759,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -4757,7 +4767,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -4765,7 +4775,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -4773,7 +4783,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -4781,7 +4791,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -4789,7 +4799,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -4797,7 +4807,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -4805,7 +4815,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -4813,7 +4823,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -4821,7 +4831,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -4829,7 +4839,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -4837,7 +4847,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -4845,7 +4855,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>58</v>
       </c>
@@ -4853,7 +4863,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>62</v>
       </c>
@@ -4861,7 +4871,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>63</v>
       </c>
@@ -4869,7 +4879,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>74</v>
       </c>
@@ -4877,7 +4887,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>79</v>
       </c>
@@ -4885,7 +4895,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>70</v>
       </c>
@@ -4893,7 +4903,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>72</v>
       </c>
@@ -4901,7 +4911,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>68</v>
       </c>
@@ -4909,7 +4919,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>66</v>
       </c>
@@ -4917,7 +4927,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>76</v>
       </c>
@@ -4925,7 +4935,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>103</v>
       </c>
@@ -4933,7 +4943,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>104</v>
       </c>
@@ -4941,7 +4951,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>105</v>
       </c>
@@ -4949,7 +4959,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>106</v>
       </c>
@@ -4957,7 +4967,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>107</v>
       </c>
@@ -4965,7 +4975,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>108</v>
       </c>
@@ -4973,7 +4983,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>109</v>
       </c>
@@ -4981,7 +4991,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>110</v>
       </c>
@@ -4989,7 +4999,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>111</v>
       </c>
@@ -4997,7 +5007,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>112</v>
       </c>
@@ -5005,7 +5015,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>130</v>
       </c>
@@ -5013,7 +5023,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>131</v>
       </c>
@@ -5021,7 +5031,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>155</v>
       </c>
@@ -5029,7 +5039,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>132</v>
       </c>
@@ -5037,7 +5047,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>147</v>
       </c>
@@ -5045,7 +5055,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>148</v>
       </c>
@@ -5053,7 +5063,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>149</v>
       </c>
@@ -5061,7 +5071,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>150</v>
       </c>
@@ -5069,7 +5079,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>151</v>
       </c>
@@ -5077,7 +5087,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>152</v>
       </c>
@@ -5085,7 +5095,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>153</v>
       </c>
@@ -5093,7 +5103,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>186</v>
       </c>
@@ -5101,7 +5111,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>189</v>
       </c>
@@ -5109,7 +5119,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>220</v>
       </c>
@@ -5117,7 +5127,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>195</v>
       </c>
@@ -5125,7 +5135,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>198</v>
       </c>
@@ -5133,7 +5143,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>219</v>
       </c>
@@ -5141,7 +5151,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>221</v>
       </c>
@@ -5149,7 +5159,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>222</v>
       </c>
@@ -5157,7 +5167,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>223</v>
       </c>
@@ -5165,7 +5175,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>224</v>
       </c>
@@ -5173,7 +5183,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>225</v>
       </c>
@@ -5181,7 +5191,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>215</v>
       </c>
@@ -5189,7 +5199,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>248</v>
       </c>
@@ -5197,7 +5207,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>250</v>
       </c>
@@ -5205,7 +5215,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>254</v>
       </c>
@@ -5213,7 +5223,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>270</v>
       </c>
@@ -5221,7 +5231,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>31</v>
       </c>
@@ -5229,7 +5239,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>286</v>
       </c>
@@ -5237,7 +5247,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>290</v>
       </c>
@@ -5245,7 +5255,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>295</v>
       </c>
@@ -5253,7 +5263,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>281</v>
       </c>
@@ -5261,12 +5271,20 @@
         <v>296</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>102</v>
       </c>
       <c r="B66" t="s">
         <v>287</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>297</v>
+      </c>
+      <c r="B67" t="s">
+        <v>298</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed a few bugs which lets CHI run
Needed to add sheet to FTT_Variables.xlsx to overcome issues.

A few bugs in IH code.
</commit_message>
<xml_diff>
--- a/Inputs/_MasterFiles/FTT_variables.xlsx
+++ b/Inputs/_MasterFiles/FTT_variables.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/cl852_exeter_ac_uk/Documents/Documents/GitHub/FTT_StandAlone/Inputs/_MasterFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rosiehayward/Documents/GitHub/FTT_StandAlone/Inputs/_MasterFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{96C6DCC7-F135-4F9F-BBD1-97530C10B60C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{771B7194-D847-4D0A-A393-E2F94739CDC5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D610159C-F6DB-1F42-9315-7BC9E96A5F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2040" yWindow="1440" windowWidth="22940" windowHeight="12480" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FTT-P" sheetId="1" r:id="rId1"/>
     <sheet name="FTT-Tr" sheetId="2" r:id="rId2"/>
     <sheet name="FTT-H" sheetId="3" r:id="rId3"/>
-    <sheet name="FTT-S" sheetId="4" r:id="rId4"/>
-    <sheet name="FTT-Fr" sheetId="7" r:id="rId5"/>
-    <sheet name="Time_Horizons" sheetId="6" r:id="rId6"/>
+    <sheet name="FTT-IH-CHI" sheetId="8" r:id="rId4"/>
+    <sheet name="FTT-S" sheetId="4" r:id="rId5"/>
+    <sheet name="FTT-Fr" sheetId="7" r:id="rId6"/>
+    <sheet name="Time_Horizons" sheetId="6" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'FTT-P'!$A$1:$G$19</definedName>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="344">
   <si>
     <t>Variable name</t>
   </si>
@@ -933,6 +934,147 @@
   </si>
   <si>
     <t>tl_2019</t>
+  </si>
+  <si>
+    <t>IUD1</t>
+  </si>
+  <si>
+    <t>ISC1</t>
+  </si>
+  <si>
+    <t>IWW1</t>
+  </si>
+  <si>
+    <t>IWI1</t>
+  </si>
+  <si>
+    <t>IWK1</t>
+  </si>
+  <si>
+    <t>IWA1</t>
+  </si>
+  <si>
+    <t>BIC1</t>
+  </si>
+  <si>
+    <t>IWS1</t>
+  </si>
+  <si>
+    <t>IWB1</t>
+  </si>
+  <si>
+    <t>IFD1</t>
+  </si>
+  <si>
+    <t>ILC1</t>
+  </si>
+  <si>
+    <t>ILG1</t>
+  </si>
+  <si>
+    <t>ILD1</t>
+  </si>
+  <si>
+    <t>IWE1</t>
+  </si>
+  <si>
+    <t>IHW1</t>
+  </si>
+  <si>
+    <t>IAM1</t>
+  </si>
+  <si>
+    <t>IRG1</t>
+  </si>
+  <si>
+    <t>ISB1</t>
+  </si>
+  <si>
+    <t>IXS1</t>
+  </si>
+  <si>
+    <t>IHF1</t>
+  </si>
+  <si>
+    <t>IJT1</t>
+  </si>
+  <si>
+    <t>IFT1</t>
+  </si>
+  <si>
+    <t>FTT-IH-CHI useful energy demand (GWh)</t>
+  </si>
+  <si>
+    <t>FTT-IH-CHI market share caps</t>
+  </si>
+  <si>
+    <t>FTT-IH-CHI cumulative capacities (EU28)</t>
+  </si>
+  <si>
+    <t>FTT-IH-CHI yearly capacity additions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FTT-IH-CHI yearly capacity </t>
+  </si>
+  <si>
+    <t>FTT-IH-CHI substitution matrix</t>
+  </si>
+  <si>
+    <t>FTT-IH-CHI cost matrix</t>
+  </si>
+  <si>
+    <t>FTT-IH-CHI market shares</t>
+  </si>
+  <si>
+    <t>FTT-IH-CHI learning spillover matrix</t>
+  </si>
+  <si>
+    <t>FTT-IH-CHI final energy demand</t>
+  </si>
+  <si>
+    <t>FTT-IH-CHI The real bare LC without taxes</t>
+  </si>
+  <si>
+    <t>FTT-IH-CHI LC as seen by consumer</t>
+  </si>
+  <si>
+    <t>FTT-IH-CHI LC standard deviation</t>
+  </si>
+  <si>
+    <t>FTT-IH-CHI Emissions</t>
+  </si>
+  <si>
+    <t>FTT-IH-CHI Global average emissions per UED (kt of CO2/GWh)</t>
+  </si>
+  <si>
+    <t>FTT-IH-CHI gamma values</t>
+  </si>
+  <si>
+    <t>FTT-IH-CHI regulations (based on capacity)</t>
+  </si>
+  <si>
+    <t>FTT-IH-CHI subsidies (percentage of investment cost)</t>
+  </si>
+  <si>
+    <t>FTT-IH-CHI exogenous share changes</t>
+  </si>
+  <si>
+    <t>FTT-IH-CHI final fuel demand for industrial heat (ktoe)</t>
+  </si>
+  <si>
+    <t>FTT-IH-CHI Tech to fuel conversion matrix (fuel x technology)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FTT-IH-CHI Fuel tax (2010 Euros/MWh) </t>
+  </si>
+  <si>
+    <t>ITTI</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>CTTI</t>
   </si>
 </sst>
 </file>
@@ -1279,20 +1421,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="12.81640625" customWidth="1"/>
-    <col min="7" max="7" width="14.453125" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" customWidth="1"/>
+    <col min="7" max="7" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1321,7 +1463,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1350,7 +1492,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>58</v>
       </c>
@@ -1379,7 +1521,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>62</v>
       </c>
@@ -1408,7 +1550,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>63</v>
       </c>
@@ -1437,7 +1579,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>74</v>
       </c>
@@ -1466,7 +1608,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>84</v>
       </c>
@@ -1495,7 +1637,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -1524,7 +1666,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>79</v>
       </c>
@@ -1553,7 +1695,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>70</v>
       </c>
@@ -1582,7 +1724,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>72</v>
       </c>
@@ -1611,7 +1753,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -1640,7 +1782,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>81</v>
       </c>
@@ -1669,7 +1811,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>88</v>
       </c>
@@ -1698,7 +1840,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>90</v>
       </c>
@@ -1727,7 +1869,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>80</v>
       </c>
@@ -1756,7 +1898,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>82</v>
       </c>
@@ -1785,7 +1927,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>66</v>
       </c>
@@ -1814,7 +1956,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>76</v>
       </c>
@@ -1862,14 +2004,14 @@
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.54296875" customWidth="1"/>
+    <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1898,7 +2040,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1927,7 +2069,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1956,7 +2098,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1985,7 +2127,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2014,7 +2156,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -2043,7 +2185,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -2072,7 +2214,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -2101,7 +2243,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -2130,7 +2272,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -2159,7 +2301,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -2188,7 +2330,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -2217,7 +2359,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -2246,7 +2388,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -2275,7 +2417,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -2304,7 +2446,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -2333,7 +2475,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -2362,7 +2504,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -2391,7 +2533,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -2420,7 +2562,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -2449,7 +2591,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -2478,7 +2620,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>52</v>
       </c>
@@ -2516,17 +2658,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{893746F0-70F0-4C21-8E46-9B5DBA6E54BB}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.453125" customWidth="1"/>
+    <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2555,7 +2697,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>96</v>
       </c>
@@ -2584,7 +2726,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>99</v>
       </c>
@@ -2613,7 +2755,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>100</v>
       </c>
@@ -2642,7 +2784,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>101</v>
       </c>
@@ -2671,7 +2813,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>102</v>
       </c>
@@ -2700,7 +2842,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>103</v>
       </c>
@@ -2729,7 +2871,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>104</v>
       </c>
@@ -2758,7 +2900,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>105</v>
       </c>
@@ -2787,7 +2929,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>106</v>
       </c>
@@ -2816,7 +2958,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>107</v>
       </c>
@@ -2845,7 +2987,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>108</v>
       </c>
@@ -2874,7 +3016,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>109</v>
       </c>
@@ -2903,7 +3045,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>110</v>
       </c>
@@ -2932,7 +3074,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>111</v>
       </c>
@@ -2961,7 +3103,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>112</v>
       </c>
@@ -2990,7 +3132,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>113</v>
       </c>
@@ -3025,6 +3167,689 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F80E1CF-C03F-6E48-9D79-9BE92647AD7E}">
+  <dimension ref="A1:I23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
+        <v>288</v>
+      </c>
+      <c r="I1" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>319</v>
+      </c>
+      <c r="E2" t="s">
+        <v>341</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>298</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>320</v>
+      </c>
+      <c r="E3" t="s">
+        <v>341</v>
+      </c>
+      <c r="F3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>299</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>321</v>
+      </c>
+      <c r="E4" t="s">
+        <v>341</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>300</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>322</v>
+      </c>
+      <c r="E5" t="s">
+        <v>341</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>301</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>323</v>
+      </c>
+      <c r="E6" t="s">
+        <v>341</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>302</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>324</v>
+      </c>
+      <c r="E7" t="s">
+        <v>341</v>
+      </c>
+      <c r="F7" t="s">
+        <v>341</v>
+      </c>
+      <c r="G7" t="s">
+        <v>342</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>303</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>325</v>
+      </c>
+      <c r="E8" t="s">
+        <v>341</v>
+      </c>
+      <c r="F8" t="s">
+        <v>343</v>
+      </c>
+      <c r="G8" t="s">
+        <v>54</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>304</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>326</v>
+      </c>
+      <c r="E9" t="s">
+        <v>341</v>
+      </c>
+      <c r="F9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>305</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>327</v>
+      </c>
+      <c r="E10" t="s">
+        <v>341</v>
+      </c>
+      <c r="F10" t="s">
+        <v>341</v>
+      </c>
+      <c r="G10" t="s">
+        <v>342</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>306</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>328</v>
+      </c>
+      <c r="E11" t="s">
+        <v>341</v>
+      </c>
+      <c r="F11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" t="s">
+        <v>54</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>307</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>329</v>
+      </c>
+      <c r="E12" t="s">
+        <v>341</v>
+      </c>
+      <c r="F12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" t="s">
+        <v>54</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>308</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13" t="s">
+        <v>330</v>
+      </c>
+      <c r="E13" t="s">
+        <v>341</v>
+      </c>
+      <c r="F13" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" t="s">
+        <v>54</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>309</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14" t="s">
+        <v>331</v>
+      </c>
+      <c r="E14" t="s">
+        <v>341</v>
+      </c>
+      <c r="F14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" t="s">
+        <v>54</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>310</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15" t="s">
+        <v>332</v>
+      </c>
+      <c r="E15" t="s">
+        <v>341</v>
+      </c>
+      <c r="F15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" t="s">
+        <v>54</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>311</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>333</v>
+      </c>
+      <c r="E16" t="s">
+        <v>341</v>
+      </c>
+      <c r="F16" t="s">
+        <v>24</v>
+      </c>
+      <c r="G16" t="s">
+        <v>342</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>312</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17" t="s">
+        <v>334</v>
+      </c>
+      <c r="E17" t="s">
+        <v>341</v>
+      </c>
+      <c r="F17" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17" t="s">
+        <v>54</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>313</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18" t="s">
+        <v>335</v>
+      </c>
+      <c r="E18" t="s">
+        <v>341</v>
+      </c>
+      <c r="F18" t="s">
+        <v>24</v>
+      </c>
+      <c r="G18" t="s">
+        <v>54</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>314</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19" t="s">
+        <v>336</v>
+      </c>
+      <c r="E19" t="s">
+        <v>341</v>
+      </c>
+      <c r="F19" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19" t="s">
+        <v>54</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>315</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20" t="s">
+        <v>337</v>
+      </c>
+      <c r="E20" t="s">
+        <v>341</v>
+      </c>
+      <c r="F20" t="s">
+        <v>24</v>
+      </c>
+      <c r="G20" t="s">
+        <v>54</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>316</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21" t="s">
+        <v>338</v>
+      </c>
+      <c r="E21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21" t="s">
+        <v>24</v>
+      </c>
+      <c r="G21" t="s">
+        <v>54</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>317</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22" t="s">
+        <v>339</v>
+      </c>
+      <c r="E22" t="s">
+        <v>40</v>
+      </c>
+      <c r="F22" t="s">
+        <v>341</v>
+      </c>
+      <c r="G22" t="s">
+        <v>342</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>318</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23" t="s">
+        <v>340</v>
+      </c>
+      <c r="E23" t="s">
+        <v>341</v>
+      </c>
+      <c r="F23" t="s">
+        <v>24</v>
+      </c>
+      <c r="G23" t="s">
+        <v>54</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F76D307B-9060-4C33-AF9D-2A846C2CA587}">
   <dimension ref="A1:I25"/>
   <sheetViews>
@@ -3032,14 +3857,14 @@
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="50.54296875" customWidth="1"/>
-    <col min="5" max="5" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.5" customWidth="1"/>
+    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3068,7 +3893,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>131</v>
       </c>
@@ -3097,7 +3922,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>155</v>
       </c>
@@ -3126,7 +3951,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>132</v>
       </c>
@@ -3155,7 +3980,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>133</v>
       </c>
@@ -3184,7 +4009,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>134</v>
       </c>
@@ -3213,7 +4038,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>135</v>
       </c>
@@ -3242,7 +4067,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>136</v>
       </c>
@@ -3271,7 +4096,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>137</v>
       </c>
@@ -3300,7 +4125,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>138</v>
       </c>
@@ -3329,7 +4154,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>139</v>
       </c>
@@ -3358,7 +4183,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>140</v>
       </c>
@@ -3387,7 +4212,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>141</v>
       </c>
@@ -3416,7 +4241,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>142</v>
       </c>
@@ -3445,7 +4270,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>143</v>
       </c>
@@ -3474,7 +4299,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>144</v>
       </c>
@@ -3503,7 +4328,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>145</v>
       </c>
@@ -3532,7 +4357,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>146</v>
       </c>
@@ -3561,7 +4386,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>147</v>
       </c>
@@ -3590,7 +4415,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>148</v>
       </c>
@@ -3619,7 +4444,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>149</v>
       </c>
@@ -3648,7 +4473,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>150</v>
       </c>
@@ -3677,7 +4502,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>151</v>
       </c>
@@ -3706,7 +4531,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>152</v>
       </c>
@@ -3735,7 +4560,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>153</v>
       </c>
@@ -3769,7 +4594,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85BB7FF7-82D6-482E-815B-F3751454FF7D}">
   <dimension ref="A1:K27"/>
   <sheetViews>
@@ -3777,17 +4602,17 @@
       <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3822,7 +4647,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>186</v>
       </c>
@@ -3857,7 +4682,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>189</v>
       </c>
@@ -3892,7 +4717,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>220</v>
       </c>
@@ -3927,7 +4752,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>195</v>
       </c>
@@ -3962,7 +4787,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>198</v>
       </c>
@@ -3997,7 +4822,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>219</v>
       </c>
@@ -4032,7 +4857,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>221</v>
       </c>
@@ -4067,7 +4892,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>222</v>
       </c>
@@ -4102,7 +4927,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>223</v>
       </c>
@@ -4137,7 +4962,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>224</v>
       </c>
@@ -4172,7 +4997,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>225</v>
       </c>
@@ -4207,7 +5032,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>215</v>
       </c>
@@ -4242,7 +5067,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>229</v>
       </c>
@@ -4274,7 +5099,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>231</v>
       </c>
@@ -4306,7 +5131,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>238</v>
       </c>
@@ -4341,7 +5166,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>239</v>
       </c>
@@ -4376,7 +5201,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>242</v>
       </c>
@@ -4411,7 +5236,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>248</v>
       </c>
@@ -4446,7 +5271,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>250</v>
       </c>
@@ -4481,7 +5306,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>254</v>
       </c>
@@ -4516,7 +5341,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>258</v>
       </c>
@@ -4551,7 +5376,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>264</v>
       </c>
@@ -4586,7 +5411,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>270</v>
       </c>
@@ -4621,7 +5446,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>266</v>
       </c>
@@ -4656,7 +5481,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>276</v>
       </c>
@@ -4691,7 +5516,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>281</v>
       </c>
@@ -4731,7 +5556,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA629D80-511C-42AD-ACB3-22237E3BD282}">
   <dimension ref="A1:B66"/>
   <sheetViews>
@@ -4739,9 +5564,9 @@
       <selection activeCell="H71" sqref="H71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4749,7 +5574,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -4757,7 +5582,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -4765,7 +5590,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -4773,7 +5598,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -4781,7 +5606,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -4789,7 +5614,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -4797,7 +5622,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -4805,7 +5630,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -4813,7 +5638,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -4821,7 +5646,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -4829,7 +5654,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -4837,7 +5662,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -4845,7 +5670,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>58</v>
       </c>
@@ -4853,7 +5678,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>62</v>
       </c>
@@ -4861,7 +5686,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>63</v>
       </c>
@@ -4869,7 +5694,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>74</v>
       </c>
@@ -4877,7 +5702,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>79</v>
       </c>
@@ -4885,7 +5710,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>70</v>
       </c>
@@ -4893,7 +5718,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>72</v>
       </c>
@@ -4901,7 +5726,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>68</v>
       </c>
@@ -4909,7 +5734,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>66</v>
       </c>
@@ -4917,7 +5742,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>76</v>
       </c>
@@ -4925,7 +5750,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>103</v>
       </c>
@@ -4933,7 +5758,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>104</v>
       </c>
@@ -4941,7 +5766,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>105</v>
       </c>
@@ -4949,7 +5774,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>106</v>
       </c>
@@ -4957,7 +5782,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>107</v>
       </c>
@@ -4965,7 +5790,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>108</v>
       </c>
@@ -4973,7 +5798,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>109</v>
       </c>
@@ -4981,7 +5806,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>110</v>
       </c>
@@ -4989,7 +5814,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>111</v>
       </c>
@@ -4997,7 +5822,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>112</v>
       </c>
@@ -5005,7 +5830,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>130</v>
       </c>
@@ -5013,7 +5838,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>131</v>
       </c>
@@ -5021,7 +5846,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>155</v>
       </c>
@@ -5029,7 +5854,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>132</v>
       </c>
@@ -5037,7 +5862,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>147</v>
       </c>
@@ -5045,7 +5870,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>148</v>
       </c>
@@ -5053,7 +5878,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>149</v>
       </c>
@@ -5061,7 +5886,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>150</v>
       </c>
@@ -5069,7 +5894,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>151</v>
       </c>
@@ -5077,7 +5902,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>152</v>
       </c>
@@ -5085,7 +5910,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>153</v>
       </c>
@@ -5093,7 +5918,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>186</v>
       </c>
@@ -5101,7 +5926,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>189</v>
       </c>
@@ -5109,7 +5934,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>220</v>
       </c>
@@ -5117,7 +5942,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>195</v>
       </c>
@@ -5125,7 +5950,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>198</v>
       </c>
@@ -5133,7 +5958,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>219</v>
       </c>
@@ -5141,7 +5966,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>221</v>
       </c>
@@ -5149,7 +5974,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>222</v>
       </c>
@@ -5157,7 +5982,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>223</v>
       </c>
@@ -5165,7 +5990,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>224</v>
       </c>
@@ -5173,7 +5998,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>225</v>
       </c>
@@ -5181,7 +6006,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>215</v>
       </c>
@@ -5189,7 +6014,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>248</v>
       </c>
@@ -5197,7 +6022,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>250</v>
       </c>
@@ -5205,7 +6030,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>254</v>
       </c>
@@ -5213,7 +6038,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>270</v>
       </c>
@@ -5221,7 +6046,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>31</v>
       </c>
@@ -5229,7 +6054,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>286</v>
       </c>
@@ -5237,7 +6062,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>290</v>
       </c>
@@ -5245,7 +6070,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>295</v>
       </c>
@@ -5253,7 +6078,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>281</v>
       </c>
@@ -5261,7 +6086,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>102</v>
       </c>

</xml_diff>

<commit_message>
Changed inputs and treatment of fuel tax
IFT replaces IFT1-5.
IXS1-5 has been entered in the masterfiles
</commit_message>
<xml_diff>
--- a/Inputs/_MasterFiles/FTT_variables.xlsx
+++ b/Inputs/_MasterFiles/FTT_variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\E3ME\FTT_Stand_Alone\Inputs\_MasterFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cambridgeeconometrics-my.sharepoint.com/personal/pv_camecon_com/Documents/Documents/GitHub/FTT_StandAlone_new/Inputs/_MasterFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6AAC6B1-6F73-4CBC-BFCC-308507F8D1EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{B6AAC6B1-6F73-4CBC-BFCC-308507F8D1EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{30525D3E-0C38-4855-8628-B01FF457BFA8}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FTT-P" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,12 @@
     <sheet name="FTT-H" sheetId="3" r:id="rId3"/>
     <sheet name="FTT-S" sheetId="4" r:id="rId4"/>
     <sheet name="FTT-Fr" sheetId="7" r:id="rId5"/>
-    <sheet name="Time_Horizons" sheetId="6" r:id="rId6"/>
+    <sheet name="FTT-IH-CHI" sheetId="8" r:id="rId6"/>
+    <sheet name="FTT-IH-FBT" sheetId="9" r:id="rId7"/>
+    <sheet name="FTT-IH_MTM" sheetId="10" r:id="rId8"/>
+    <sheet name="FTT-IH-NMM" sheetId="11" r:id="rId9"/>
+    <sheet name="FTT-IH-OIS" sheetId="12" r:id="rId10"/>
+    <sheet name="Time_Horizons" sheetId="6" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'FTT-P'!$A$1:$G$19</definedName>
@@ -42,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="295">
   <si>
     <t>Variable name</t>
   </si>
@@ -906,6 +911,27 @@
   </si>
   <si>
     <t>FTT-Fr T-Scaling</t>
+  </si>
+  <si>
+    <t>ITTI</t>
+  </si>
+  <si>
+    <t>ISX1</t>
+  </si>
+  <si>
+    <t>ISX2</t>
+  </si>
+  <si>
+    <t>ISX3</t>
+  </si>
+  <si>
+    <t>ISX4</t>
+  </si>
+  <si>
+    <t>ISX5</t>
+  </si>
+  <si>
+    <t>tl_2000</t>
   </si>
 </sst>
 </file>
@@ -965,10 +991,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
@@ -1254,19 +1279,19 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.59765625" customWidth="1"/>
+    <col min="4" max="4" width="19.6328125" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="12.86328125" customWidth="1"/>
-    <col min="7" max="7" width="14.3984375" customWidth="1"/>
+    <col min="6" max="6" width="12.81640625" customWidth="1"/>
+    <col min="7" max="7" width="14.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1289,7 +1314,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1312,7 +1337,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>60</v>
       </c>
@@ -1335,7 +1360,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>64</v>
       </c>
@@ -1358,7 +1383,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>65</v>
       </c>
@@ -1381,7 +1406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>76</v>
       </c>
@@ -1404,7 +1429,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>87</v>
       </c>
@@ -1427,7 +1452,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>57</v>
       </c>
@@ -1450,7 +1475,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>81</v>
       </c>
@@ -1473,7 +1498,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>72</v>
       </c>
@@ -1496,7 +1521,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>74</v>
       </c>
@@ -1519,7 +1544,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>70</v>
       </c>
@@ -1542,7 +1567,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>84</v>
       </c>
@@ -1565,7 +1590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>91</v>
       </c>
@@ -1588,7 +1613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>93</v>
       </c>
@@ -1611,7 +1636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>83</v>
       </c>
@@ -1634,7 +1659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>85</v>
       </c>
@@ -1657,7 +1682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>68</v>
       </c>
@@ -1680,7 +1705,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>78</v>
       </c>
@@ -1714,6 +1739,606 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F744C93-4F2B-4668-98F6-93AE628E611E}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" t="s">
+        <v>288</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA629D80-511C-42AD-ACB3-22237E3BD282}">
+  <dimension ref="A1:B69"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="J41" sqref="J41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>106</v>
+      </c>
+      <c r="B24" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>107</v>
+      </c>
+      <c r="B25" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>108</v>
+      </c>
+      <c r="B26" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>109</v>
+      </c>
+      <c r="B27" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>110</v>
+      </c>
+      <c r="B28" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>111</v>
+      </c>
+      <c r="B29" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>112</v>
+      </c>
+      <c r="B30" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>113</v>
+      </c>
+      <c r="B31" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>114</v>
+      </c>
+      <c r="B32" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>115</v>
+      </c>
+      <c r="B33" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>133</v>
+      </c>
+      <c r="B34" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>134</v>
+      </c>
+      <c r="B35" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>158</v>
+      </c>
+      <c r="B36" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>135</v>
+      </c>
+      <c r="B37" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>150</v>
+      </c>
+      <c r="B38" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>151</v>
+      </c>
+      <c r="B39" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>152</v>
+      </c>
+      <c r="B40" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>153</v>
+      </c>
+      <c r="B41" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>154</v>
+      </c>
+      <c r="B42" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>155</v>
+      </c>
+      <c r="B43" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>156</v>
+      </c>
+      <c r="B44" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>189</v>
+      </c>
+      <c r="B45" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>192</v>
+      </c>
+      <c r="B46" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>223</v>
+      </c>
+      <c r="B47" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>198</v>
+      </c>
+      <c r="B48" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>201</v>
+      </c>
+      <c r="B49" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>222</v>
+      </c>
+      <c r="B50" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>224</v>
+      </c>
+      <c r="B51" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>225</v>
+      </c>
+      <c r="B52" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>226</v>
+      </c>
+      <c r="B53" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>227</v>
+      </c>
+      <c r="B54" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>228</v>
+      </c>
+      <c r="B55" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>218</v>
+      </c>
+      <c r="B56" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>251</v>
+      </c>
+      <c r="B57" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>253</v>
+      </c>
+      <c r="B58" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>257</v>
+      </c>
+      <c r="B59" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>273</v>
+      </c>
+      <c r="B60" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>289</v>
+      </c>
+      <c r="B61" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>290</v>
+      </c>
+      <c r="B62" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>291</v>
+      </c>
+      <c r="B63" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>292</v>
+      </c>
+      <c r="B64" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>293</v>
+      </c>
+      <c r="B65" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A69" s="3"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E04294AC-DBC1-4E51-84ED-2EC5066B9024}">
   <dimension ref="A1:G23"/>
@@ -1722,14 +2347,14 @@
       <selection activeCell="A2" sqref="A2:A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.59765625" customWidth="1"/>
+    <col min="2" max="2" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1752,7 +2377,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1775,7 +2400,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1798,7 +2423,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1821,7 +2446,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1844,7 +2469,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1867,7 +2492,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1890,7 +2515,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1913,7 +2538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -1936,7 +2561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1959,7 +2584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -1982,7 +2607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -2005,7 +2630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -2028,7 +2653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -2051,7 +2676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -2074,7 +2699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -2097,7 +2722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -2120,7 +2745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -2143,7 +2768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -2166,7 +2791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -2189,7 +2814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>37</v>
       </c>
@@ -2212,7 +2837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -2235,7 +2860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>54</v>
       </c>
@@ -2271,13 +2896,13 @@
       <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="8.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.3984375" customWidth="1"/>
+    <col min="2" max="2" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2300,7 +2925,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>99</v>
       </c>
@@ -2323,7 +2948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>102</v>
       </c>
@@ -2346,7 +2971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>103</v>
       </c>
@@ -2369,7 +2994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>104</v>
       </c>
@@ -2392,7 +3017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>105</v>
       </c>
@@ -2415,7 +3040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>106</v>
       </c>
@@ -2438,7 +3063,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>107</v>
       </c>
@@ -2461,7 +3086,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>108</v>
       </c>
@@ -2484,7 +3109,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>109</v>
       </c>
@@ -2507,7 +3132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>110</v>
       </c>
@@ -2530,7 +3155,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>111</v>
       </c>
@@ -2553,7 +3178,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>112</v>
       </c>
@@ -2576,7 +3201,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>113</v>
       </c>
@@ -2599,7 +3224,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>114</v>
       </c>
@@ -2622,7 +3247,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>115</v>
       </c>
@@ -2645,7 +3270,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>116</v>
       </c>
@@ -2681,14 +3306,14 @@
       <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.59765625" customWidth="1"/>
-    <col min="5" max="5" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.6328125" customWidth="1"/>
+    <col min="5" max="5" width="9.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2711,7 +3336,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>134</v>
       </c>
@@ -2734,7 +3359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>158</v>
       </c>
@@ -2757,7 +3382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>135</v>
       </c>
@@ -2780,7 +3405,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>136</v>
       </c>
@@ -2803,7 +3428,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>137</v>
       </c>
@@ -2826,7 +3451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>138</v>
       </c>
@@ -2849,7 +3474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>139</v>
       </c>
@@ -2872,7 +3497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>140</v>
       </c>
@@ -2895,7 +3520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>141</v>
       </c>
@@ -2918,7 +3543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>142</v>
       </c>
@@ -2941,7 +3566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>143</v>
       </c>
@@ -2964,7 +3589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>144</v>
       </c>
@@ -2987,7 +3612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>145</v>
       </c>
@@ -3010,7 +3635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>146</v>
       </c>
@@ -3033,7 +3658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>147</v>
       </c>
@@ -3056,7 +3681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>148</v>
       </c>
@@ -3079,7 +3704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>149</v>
       </c>
@@ -3102,7 +3727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>150</v>
       </c>
@@ -3125,7 +3750,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>151</v>
       </c>
@@ -3148,7 +3773,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>152</v>
       </c>
@@ -3171,7 +3796,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>153</v>
       </c>
@@ -3194,7 +3819,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>154</v>
       </c>
@@ -3217,7 +3842,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>155</v>
       </c>
@@ -3240,7 +3865,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>156</v>
       </c>
@@ -3272,21 +3897,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85BB7FF7-82D6-482E-815B-F3751454FF7D}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.06640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.46484375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.53125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.06640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3315,7 +3940,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>189</v>
       </c>
@@ -3344,7 +3969,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>192</v>
       </c>
@@ -3373,7 +3998,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>223</v>
       </c>
@@ -3395,14 +4020,14 @@
       <c r="G4" t="s">
         <v>56</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" t="s">
         <v>220</v>
       </c>
       <c r="I4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>198</v>
       </c>
@@ -3424,14 +4049,14 @@
       <c r="G5">
         <v>0</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" t="s">
         <v>236</v>
       </c>
       <c r="I5" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>201</v>
       </c>
@@ -3460,7 +4085,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>222</v>
       </c>
@@ -3489,7 +4114,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>224</v>
       </c>
@@ -3518,7 +4143,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>225</v>
       </c>
@@ -3547,7 +4172,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>226</v>
       </c>
@@ -3576,7 +4201,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>227</v>
       </c>
@@ -3605,7 +4230,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>228</v>
       </c>
@@ -3634,7 +4259,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>218</v>
       </c>
@@ -3663,7 +4288,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>232</v>
       </c>
@@ -3689,7 +4314,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>234</v>
       </c>
@@ -3715,7 +4340,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>241</v>
       </c>
@@ -3744,7 +4369,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>242</v>
       </c>
@@ -3773,14 +4398,14 @@
         <v>238</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>245</v>
       </c>
       <c r="B18">
         <v>0</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="2">
         <v>35340000</v>
       </c>
       <c r="D18" t="s">
@@ -3802,14 +4427,14 @@
         <v>249</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>251</v>
       </c>
       <c r="B19">
         <v>0</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="2">
         <v>35350000</v>
       </c>
       <c r="D19" t="s">
@@ -3831,7 +4456,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>253</v>
       </c>
@@ -3860,7 +4485,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>257</v>
       </c>
@@ -3889,14 +4514,14 @@
         <v>259</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>261</v>
       </c>
       <c r="B22">
         <v>0</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="2">
         <v>35360000</v>
       </c>
       <c r="D22" t="s">
@@ -3905,7 +4530,7 @@
       <c r="E22" t="s">
         <v>56</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="F22" s="3" t="s">
         <v>280</v>
       </c>
       <c r="G22">
@@ -3918,14 +4543,14 @@
         <v>262</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>267</v>
       </c>
       <c r="B23">
         <v>0</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="2">
         <v>35370000</v>
       </c>
       <c r="D23" t="s">
@@ -3947,14 +4572,14 @@
         <v>266</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>273</v>
       </c>
       <c r="B24">
         <v>0</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="2">
         <v>35380000</v>
       </c>
       <c r="D24" t="s">
@@ -3976,7 +4601,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>269</v>
       </c>
@@ -3992,7 +4617,7 @@
       <c r="E25" t="s">
         <v>195</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F25" t="s">
         <v>41</v>
       </c>
       <c r="G25">
@@ -4005,26 +4630,26 @@
         <v>275</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A26" s="4" t="s">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26" s="3" t="s">
         <v>279</v>
       </c>
       <c r="B26">
         <v>0</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="2">
         <v>35390000</v>
       </c>
       <c r="D26" t="s">
         <v>276</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="F26" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="G26" s="4" t="s">
+      <c r="G26" s="3" t="s">
         <v>56</v>
       </c>
       <c r="H26" t="s">
@@ -4034,17 +4659,17 @@
         <v>278</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>284</v>
       </c>
       <c r="B27">
         <v>0</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27" s="2">
         <v>35410000</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="2" t="s">
         <v>287</v>
       </c>
       <c r="E27" t="s">
@@ -4069,500 +4694,245 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA629D80-511C-42AD-ACB3-22237E3BD282}">
-  <dimension ref="A1:B69"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1602429-35F9-4396-9EF9-8B9E187CA926}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+        <v>157</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>60</v>
-      </c>
-      <c r="B14" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
-        <v>64</v>
-      </c>
-      <c r="B15" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
-        <v>65</v>
-      </c>
-      <c r="B16" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
-        <v>76</v>
-      </c>
-      <c r="B17" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
-        <v>81</v>
-      </c>
-      <c r="B18" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
-        <v>72</v>
-      </c>
-      <c r="B19" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
-        <v>74</v>
-      </c>
-      <c r="B20" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
-        <v>70</v>
-      </c>
-      <c r="B21" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
-        <v>68</v>
-      </c>
-      <c r="B22" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
-        <v>78</v>
-      </c>
-      <c r="B23" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
-        <v>106</v>
-      </c>
-      <c r="B24" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
-        <v>107</v>
-      </c>
-      <c r="B25" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
-        <v>108</v>
-      </c>
-      <c r="B26" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
-        <v>109</v>
-      </c>
-      <c r="B27" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
-        <v>110</v>
-      </c>
-      <c r="B28" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
-        <v>111</v>
-      </c>
-      <c r="B29" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
-        <v>112</v>
-      </c>
-      <c r="B30" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A31" t="s">
-        <v>113</v>
-      </c>
-      <c r="B31" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A32" t="s">
-        <v>114</v>
-      </c>
-      <c r="B32" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A33" t="s">
-        <v>115</v>
-      </c>
-      <c r="B33" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A34" t="s">
-        <v>133</v>
-      </c>
-      <c r="B34" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A35" t="s">
-        <v>134</v>
-      </c>
-      <c r="B35" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A36" t="s">
-        <v>158</v>
-      </c>
-      <c r="B36" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A37" t="s">
-        <v>135</v>
-      </c>
-      <c r="B37" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A38" t="s">
-        <v>150</v>
-      </c>
-      <c r="B38" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A39" t="s">
-        <v>151</v>
-      </c>
-      <c r="B39" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A40" t="s">
-        <v>152</v>
-      </c>
-      <c r="B40" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A41" t="s">
-        <v>153</v>
-      </c>
-      <c r="B41" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A42" t="s">
-        <v>154</v>
-      </c>
-      <c r="B42" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A43" t="s">
-        <v>155</v>
-      </c>
-      <c r="B43" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A44" t="s">
-        <v>156</v>
-      </c>
-      <c r="B44" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A45" t="s">
-        <v>189</v>
-      </c>
-      <c r="B45" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A46" t="s">
-        <v>192</v>
-      </c>
-      <c r="B46" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A47" t="s">
-        <v>223</v>
-      </c>
-      <c r="B47" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A48" t="s">
-        <v>198</v>
-      </c>
-      <c r="B48" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A49" t="s">
-        <v>201</v>
-      </c>
-      <c r="B49" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A50" t="s">
-        <v>222</v>
-      </c>
-      <c r="B50" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A51" t="s">
-        <v>224</v>
-      </c>
-      <c r="B51" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A52" t="s">
-        <v>225</v>
-      </c>
-      <c r="B52" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A53" t="s">
-        <v>226</v>
-      </c>
-      <c r="B53" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A54" t="s">
-        <v>227</v>
-      </c>
-      <c r="B54" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A55" t="s">
-        <v>228</v>
-      </c>
-      <c r="B55" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A56" t="s">
-        <v>218</v>
-      </c>
-      <c r="B56" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A57" t="s">
-        <v>251</v>
-      </c>
-      <c r="B57" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A58" t="s">
-        <v>253</v>
-      </c>
-      <c r="B58" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A59" t="s">
-        <v>257</v>
-      </c>
-      <c r="B59" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A60" t="s">
-        <v>273</v>
-      </c>
-      <c r="B60" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A69" s="4"/>
+        <v>289</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" t="s">
+        <v>288</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
+        <v>56</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A14D33F-5EAB-4CF7-9FC8-8D43CCE0C35E}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>290</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" t="s">
+        <v>288</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{281A7C66-7938-420A-8F94-1D8374170D8F}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" t="s">
+        <v>288</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD8D846E-AADD-43BA-9AE0-C87DF0DD7A8C}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>292</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" t="s">
+        <v>288</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
expand calculation of operational costs
And correct the calculation
</commit_message>
<xml_diff>
--- a/Inputs/_MasterFiles/FTT_variables.xlsx
+++ b/Inputs/_MasterFiles/FTT_variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/cl852_exeter_ac_uk/Documents/Documents/GitHub/FTT_StandAlone/Inputs/_MasterFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/f_j_m_m_nijsse_exeter_ac_uk/Documents/Documents/GitHub/FTT_StandAlone/Inputs/_MasterFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{96C6DCC7-F135-4F9F-BBD1-97530C10B60C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{633FC2CE-8022-472C-9BE9-1C2649AABB15}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FTT-P" sheetId="1" r:id="rId1"/>
@@ -1239,16 +1239,16 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="12.81640625" customWidth="1"/>
-    <col min="7" max="7" width="14.453125" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1277,7 +1277,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1306,7 +1306,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>58</v>
       </c>
@@ -1335,7 +1335,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>62</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>63</v>
       </c>
@@ -1393,7 +1393,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>74</v>
       </c>
@@ -1422,7 +1422,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>84</v>
       </c>
@@ -1451,7 +1451,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -1480,7 +1480,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>79</v>
       </c>
@@ -1509,7 +1509,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>70</v>
       </c>
@@ -1538,7 +1538,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>72</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -1596,7 +1596,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>81</v>
       </c>
@@ -1625,7 +1625,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>88</v>
       </c>
@@ -1654,7 +1654,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>90</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>80</v>
       </c>
@@ -1712,7 +1712,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>82</v>
       </c>
@@ -1741,7 +1741,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>66</v>
       </c>
@@ -1770,7 +1770,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>76</v>
       </c>
@@ -1818,14 +1818,14 @@
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.54296875" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1854,7 +1854,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1883,7 +1883,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1912,7 +1912,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1941,7 +1941,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1970,7 +1970,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1999,7 +1999,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -2028,7 +2028,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -2086,7 +2086,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -2115,7 +2115,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -2144,7 +2144,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -2173,7 +2173,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -2202,7 +2202,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -2231,7 +2231,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -2260,7 +2260,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -2289,7 +2289,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -2318,7 +2318,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -2347,7 +2347,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -2405,7 +2405,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -2434,7 +2434,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>52</v>
       </c>
@@ -2476,13 +2476,13 @@
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.453125" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2511,7 +2511,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>96</v>
       </c>
@@ -2540,7 +2540,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>99</v>
       </c>
@@ -2569,7 +2569,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>100</v>
       </c>
@@ -2598,7 +2598,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>101</v>
       </c>
@@ -2627,7 +2627,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>102</v>
       </c>
@@ -2656,7 +2656,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>103</v>
       </c>
@@ -2685,7 +2685,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>104</v>
       </c>
@@ -2714,7 +2714,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>105</v>
       </c>
@@ -2743,7 +2743,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>106</v>
       </c>
@@ -2772,7 +2772,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>107</v>
       </c>
@@ -2801,7 +2801,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>108</v>
       </c>
@@ -2830,7 +2830,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>109</v>
       </c>
@@ -2859,7 +2859,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>110</v>
       </c>
@@ -2888,7 +2888,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>111</v>
       </c>
@@ -2917,7 +2917,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>112</v>
       </c>
@@ -2946,7 +2946,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>113</v>
       </c>
@@ -2988,14 +2988,14 @@
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="50.54296875" customWidth="1"/>
-    <col min="5" max="5" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.5703125" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3024,7 +3024,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>131</v>
       </c>
@@ -3053,7 +3053,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>155</v>
       </c>
@@ -3082,7 +3082,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>132</v>
       </c>
@@ -3111,7 +3111,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>133</v>
       </c>
@@ -3140,7 +3140,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>134</v>
       </c>
@@ -3169,7 +3169,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>135</v>
       </c>
@@ -3198,7 +3198,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>136</v>
       </c>
@@ -3227,7 +3227,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>137</v>
       </c>
@@ -3256,7 +3256,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>138</v>
       </c>
@@ -3285,7 +3285,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>139</v>
       </c>
@@ -3314,7 +3314,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>140</v>
       </c>
@@ -3343,7 +3343,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>141</v>
       </c>
@@ -3372,7 +3372,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>142</v>
       </c>
@@ -3401,7 +3401,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>143</v>
       </c>
@@ -3430,7 +3430,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>144</v>
       </c>
@@ -3459,7 +3459,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>145</v>
       </c>
@@ -3488,7 +3488,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>146</v>
       </c>
@@ -3517,7 +3517,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>147</v>
       </c>
@@ -3546,7 +3546,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>148</v>
       </c>
@@ -3575,7 +3575,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>149</v>
       </c>
@@ -3604,7 +3604,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>150</v>
       </c>
@@ -3633,7 +3633,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>151</v>
       </c>
@@ -3662,7 +3662,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>152</v>
       </c>
@@ -3691,7 +3691,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>153</v>
       </c>
@@ -3729,21 +3729,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85BB7FF7-82D6-482E-815B-F3751454FF7D}">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3778,7 +3778,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>186</v>
       </c>
@@ -3813,7 +3813,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>189</v>
       </c>
@@ -3848,7 +3848,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>217</v>
       </c>
@@ -3883,7 +3883,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>195</v>
       </c>
@@ -3918,7 +3918,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>286</v>
       </c>
@@ -3953,7 +3953,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>216</v>
       </c>
@@ -3988,7 +3988,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>218</v>
       </c>
@@ -4023,7 +4023,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>219</v>
       </c>
@@ -4058,7 +4058,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>220</v>
       </c>
@@ -4093,7 +4093,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>221</v>
       </c>
@@ -4128,7 +4128,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>222</v>
       </c>
@@ -4163,7 +4163,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>231</v>
       </c>
@@ -4198,7 +4198,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>232</v>
       </c>
@@ -4233,7 +4233,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>237</v>
       </c>
@@ -4268,7 +4268,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>239</v>
       </c>
@@ -4303,7 +4303,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>243</v>
       </c>
@@ -4338,7 +4338,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>247</v>
       </c>
@@ -4373,7 +4373,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>253</v>
       </c>
@@ -4408,7 +4408,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>259</v>
       </c>
@@ -4443,7 +4443,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>255</v>
       </c>
@@ -4478,7 +4478,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>265</v>
       </c>
@@ -4513,7 +4513,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>270</v>
       </c>
@@ -4557,13 +4557,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA629D80-511C-42AD-ACB3-22237E3BD282}">
   <dimension ref="A1:B65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4571,7 +4571,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -4579,7 +4579,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -4587,7 +4587,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -4595,7 +4595,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -4603,7 +4603,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -4611,7 +4611,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -4619,7 +4619,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -4627,7 +4627,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -4635,7 +4635,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -4643,7 +4643,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -4651,7 +4651,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -4659,7 +4659,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -4667,7 +4667,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>58</v>
       </c>
@@ -4675,7 +4675,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>62</v>
       </c>
@@ -4683,7 +4683,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>63</v>
       </c>
@@ -4691,7 +4691,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>74</v>
       </c>
@@ -4699,7 +4699,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>79</v>
       </c>
@@ -4707,7 +4707,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>70</v>
       </c>
@@ -4715,7 +4715,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>72</v>
       </c>
@@ -4723,7 +4723,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>68</v>
       </c>
@@ -4731,7 +4731,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>66</v>
       </c>
@@ -4739,7 +4739,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>76</v>
       </c>
@@ -4747,7 +4747,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>103</v>
       </c>
@@ -4755,7 +4755,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>104</v>
       </c>
@@ -4763,7 +4763,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>105</v>
       </c>
@@ -4771,7 +4771,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>106</v>
       </c>
@@ -4779,7 +4779,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>107</v>
       </c>
@@ -4787,7 +4787,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>108</v>
       </c>
@@ -4795,7 +4795,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>109</v>
       </c>
@@ -4803,7 +4803,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>110</v>
       </c>
@@ -4811,7 +4811,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>111</v>
       </c>
@@ -4819,7 +4819,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>112</v>
       </c>
@@ -4827,7 +4827,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>130</v>
       </c>
@@ -4835,7 +4835,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>131</v>
       </c>
@@ -4843,7 +4843,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>155</v>
       </c>
@@ -4851,7 +4851,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>132</v>
       </c>
@@ -4859,7 +4859,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>147</v>
       </c>
@@ -4867,7 +4867,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>148</v>
       </c>
@@ -4875,7 +4875,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>149</v>
       </c>
@@ -4883,7 +4883,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>150</v>
       </c>
@@ -4891,7 +4891,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>151</v>
       </c>
@@ -4899,7 +4899,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>152</v>
       </c>
@@ -4907,7 +4907,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>153</v>
       </c>
@@ -4915,7 +4915,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>186</v>
       </c>
@@ -4923,7 +4923,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>189</v>
       </c>
@@ -4931,7 +4931,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>217</v>
       </c>
@@ -4939,7 +4939,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>195</v>
       </c>
@@ -4947,7 +4947,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>286</v>
       </c>
@@ -4955,7 +4955,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>216</v>
       </c>
@@ -4963,7 +4963,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>218</v>
       </c>
@@ -4971,7 +4971,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>219</v>
       </c>
@@ -4979,7 +4979,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>220</v>
       </c>
@@ -4987,7 +4987,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>221</v>
       </c>
@@ -4995,7 +4995,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>222</v>
       </c>
@@ -5003,7 +5003,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>237</v>
       </c>
@@ -5011,7 +5011,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>239</v>
       </c>
@@ -5019,7 +5019,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>243</v>
       </c>
@@ -5027,7 +5027,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>259</v>
       </c>
@@ -5035,7 +5035,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>31</v>
       </c>
@@ -5043,7 +5043,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>275</v>
       </c>
@@ -5051,7 +5051,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>279</v>
       </c>
@@ -5059,7 +5059,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>284</v>
       </c>
@@ -5067,7 +5067,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>270</v>
       </c>
@@ -5075,7 +5075,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>102</v>
       </c>

</xml_diff>

<commit_message>
Basic Bass model for fertilisers
The CLean Energy Adoption in Fertiliser Sector (CLEAFS) module added to the FTT framework. The module currently uses a basic Bass diffusion model to estimate the diffusion of green fertiliser.
</commit_message>
<xml_diff>
--- a/Inputs/_MasterFiles/FTT_variables.xlsx
+++ b/Inputs/_MasterFiles/FTT_variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/cl852_exeter_ac_uk/Documents/Documents/GitHub/FTT_StandAlone/Inputs/_MasterFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FTT_StandAlone\FTT_StandAlone\Inputs\_MasterFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{96C6DCC7-F135-4F9F-BBD1-97530C10B60C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{771B7194-D847-4D0A-A393-E2F94739CDC5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87473702-408B-4CD3-88D6-6E4DA3B3907C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-4830" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FTT-P" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="FTT-H" sheetId="3" r:id="rId3"/>
     <sheet name="FTT-S" sheetId="4" r:id="rId4"/>
     <sheet name="FTT-Fr" sheetId="7" r:id="rId5"/>
-    <sheet name="Time_Horizons" sheetId="6" r:id="rId6"/>
+    <sheet name="CLEAFS" sheetId="8" r:id="rId6"/>
+    <sheet name="Time_Horizons" sheetId="6" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'FTT-P'!$A$1:$G$19</definedName>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="310">
   <si>
     <t>Variable name</t>
   </si>
@@ -933,6 +934,45 @@
   </si>
   <si>
     <t>tl_2019</t>
+  </si>
+  <si>
+    <t>FERTD</t>
+  </si>
+  <si>
+    <t>BFTC</t>
+  </si>
+  <si>
+    <t>CLEAFS Fertiliser demand (tN/year)</t>
+  </si>
+  <si>
+    <t>CLEAFS matrix of technology costs</t>
+  </si>
+  <si>
+    <t>TFTI</t>
+  </si>
+  <si>
+    <t>CFTI</t>
+  </si>
+  <si>
+    <t>tl_1960</t>
+  </si>
+  <si>
+    <t>MFERTD</t>
+  </si>
+  <si>
+    <t>AQR</t>
+  </si>
+  <si>
+    <t>tl_2010</t>
+  </si>
+  <si>
+    <t>CLEAFS Maximum potential fertiliser demand (tN/year)</t>
+  </si>
+  <si>
+    <t>Agriculture output projection</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -1279,8 +1319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1858,7 +1898,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E04294AC-DBC1-4E51-84ED-2EC5066B9024}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -2516,8 +2556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{893746F0-70F0-4C21-8E46-9B5DBA6E54BB}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3773,8 +3813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85BB7FF7-82D6-482E-815B-F3751454FF7D}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4732,11 +4772,171 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFA5FF52-AB16-41E7-A79B-14E0FF373C97}">
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
+        <v>288</v>
+      </c>
+      <c r="I1" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>3601000</v>
+      </c>
+      <c r="D2" t="s">
+        <v>299</v>
+      </c>
+      <c r="E2" t="s">
+        <v>301</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>304</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>3602000</v>
+      </c>
+      <c r="D3" t="s">
+        <v>307</v>
+      </c>
+      <c r="E3" t="s">
+        <v>301</v>
+      </c>
+      <c r="F3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>298</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>3603000</v>
+      </c>
+      <c r="D4" t="s">
+        <v>300</v>
+      </c>
+      <c r="E4" t="s">
+        <v>301</v>
+      </c>
+      <c r="F4" t="s">
+        <v>302</v>
+      </c>
+      <c r="G4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>305</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>3604000</v>
+      </c>
+      <c r="D5" t="s">
+        <v>308</v>
+      </c>
+      <c r="E5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" t="s">
+        <v>309</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>292</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA629D80-511C-42AD-ACB3-22237E3BD282}">
-  <dimension ref="A1:B66"/>
+  <dimension ref="A1:B69"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="H71" sqref="H71"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5269,6 +5469,30 @@
         <v>287</v>
       </c>
     </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>297</v>
+      </c>
+      <c r="B67" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>304</v>
+      </c>
+      <c r="B68" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>305</v>
+      </c>
+      <c r="B69" t="s">
+        <v>306</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fertiliser module: update financial factors in green fertiliser diffusion
</commit_message>
<xml_diff>
--- a/Inputs/_MasterFiles/FTT_variables.xlsx
+++ b/Inputs/_MasterFiles/FTT_variables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FTT_StandAlone\FTT_StandAlone\Inputs\_MasterFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{331BAB01-942E-4606-AC20-107CADF4D738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9AEE770-8AFE-480D-BA0B-1EB4A6C0C580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-4830" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FTT-P" sheetId="1" r:id="rId1"/>
@@ -958,18 +958,12 @@
     <t>tl_1960</t>
   </si>
   <si>
-    <t>MFERTD</t>
-  </si>
-  <si>
     <t>AQR</t>
   </si>
   <si>
     <t>tl_2010</t>
   </si>
   <si>
-    <t>CLEAFS Maximum potential fertiliser demand (tN/year)</t>
-  </si>
-  <si>
     <t>Agriculture output projection</t>
   </si>
   <si>
@@ -1013,6 +1007,12 @@
   </si>
   <si>
     <t>tl_2022</t>
+  </si>
+  <si>
+    <t>PFRA</t>
+  </si>
+  <si>
+    <t>CLEAFS Ammonia price</t>
   </si>
 </sst>
 </file>
@@ -4816,7 +4816,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4881,7 +4881,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>304</v>
+        <v>321</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -4890,7 +4890,7 @@
         <v>3602000</v>
       </c>
       <c r="D3" t="s">
-        <v>307</v>
+        <v>322</v>
       </c>
       <c r="E3" t="s">
         <v>301</v>
@@ -4939,7 +4939,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -4948,7 +4948,7 @@
         <v>3604000</v>
       </c>
       <c r="D5" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E5" t="s">
         <v>54</v>
@@ -5012,7 +5012,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -5021,13 +5021,13 @@
         <v>3605000</v>
       </c>
       <c r="D2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="G2" t="s">
         <v>54</v>
@@ -5041,7 +5041,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -5050,10 +5050,10 @@
         <v>3606000</v>
       </c>
       <c r="D3" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E3" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F3" t="s">
         <v>24</v>
@@ -5070,7 +5070,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -5079,7 +5079,7 @@
         <v>3607000</v>
       </c>
       <c r="D4" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E4" t="s">
         <v>54</v>
@@ -5099,7 +5099,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -5108,10 +5108,10 @@
         <v>3608000</v>
       </c>
       <c r="D5" t="s">
+        <v>315</v>
+      </c>
+      <c r="E5" t="s">
         <v>317</v>
-      </c>
-      <c r="E5" t="s">
-        <v>319</v>
       </c>
       <c r="F5" t="s">
         <v>40</v>
@@ -5128,7 +5128,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -5137,10 +5137,10 @@
         <v>3609000</v>
       </c>
       <c r="D6" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E6" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -5164,8 +5164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA629D80-511C-42AD-ACB3-22237E3BD282}">
   <dimension ref="A1:B72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5708,42 +5708,42 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>304</v>
+        <v>321</v>
       </c>
       <c r="B68" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
+        <v>304</v>
+      </c>
+      <c r="B69" t="s">
         <v>305</v>
-      </c>
-      <c r="B69" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B70" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B71" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B72" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
H2 cost-supply curves + draft pooledtrading
</commit_message>
<xml_diff>
--- a/Inputs/_MasterFiles/FTT_variables.xlsx
+++ b/Inputs/_MasterFiles/FTT_variables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FTT_StandAlone\FTT_StandAlone\Inputs\_MasterFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9AEE770-8AFE-480D-BA0B-1EB4A6C0C580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897C4E3A-A29C-47B0-8D41-B6ADCBDDEF05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-4830" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FTT-P" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="325">
   <si>
     <t>Variable name</t>
   </si>
@@ -1003,9 +1003,6 @@
     <t>C7TI</t>
   </si>
   <si>
-    <t>tl_2011</t>
-  </si>
-  <si>
     <t>tl_2022</t>
   </si>
   <si>
@@ -1013,6 +1010,15 @@
   </si>
   <si>
     <t>CLEAFS Ammonia price</t>
+  </si>
+  <si>
+    <t>HYEXPSH</t>
+  </si>
+  <si>
+    <t>tl_2020</t>
+  </si>
+  <si>
+    <t>FTT:Hydrogen hydrogen export shares</t>
   </si>
 </sst>
 </file>
@@ -4881,7 +4887,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -4890,7 +4896,7 @@
         <v>3602000</v>
       </c>
       <c r="D3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E3" t="s">
         <v>301</v>
@@ -4973,10 +4979,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05986654-6C49-4A34-BECD-4482E94CE084}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5152,6 +5158,35 @@
         <v>24</v>
       </c>
       <c r="I6" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>322</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>3610000</v>
+      </c>
+      <c r="D7" t="s">
+        <v>324</v>
+      </c>
+      <c r="E7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7" t="s">
         <v>292</v>
       </c>
     </row>
@@ -5162,10 +5197,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA629D80-511C-42AD-ACB3-22237E3BD282}">
-  <dimension ref="A1:B72"/>
+  <dimension ref="A1:B73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5708,7 +5743,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B68" t="s">
         <v>305</v>
@@ -5727,7 +5762,7 @@
         <v>308</v>
       </c>
       <c r="B70" t="s">
-        <v>319</v>
+        <v>95</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
@@ -5735,7 +5770,7 @@
         <v>309</v>
       </c>
       <c r="B71" t="s">
-        <v>319</v>
+        <v>95</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
@@ -5743,7 +5778,15 @@
         <v>311</v>
       </c>
       <c r="B72" t="s">
-        <v>320</v>
+        <v>319</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>322</v>
+      </c>
+      <c r="B73" t="s">
+        <v>323</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
start adding new freight update
Note: this is highly likely to be broken.
</commit_message>
<xml_diff>
--- a/Inputs/_MasterFiles/FTT_variables.xlsx
+++ b/Inputs/_MasterFiles/FTT_variables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/f_j_m_m_nijsse_exeter_ac_uk/Documents/Documents/GitHub/FTT_StandAlone/Inputs/_MasterFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{96C6DCC7-F135-4F9F-BBD1-97530C10B60C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{633FC2CE-8022-472C-9BE9-1C2649AABB15}"/>
+  <xr:revisionPtr revIDLastSave="66" documentId="13_ncr:1_{96C6DCC7-F135-4F9F-BBD1-97530C10B60C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{99DEB3FD-5686-411E-B667-D81B4189779D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="275">
   <si>
     <t>Variable name</t>
   </si>
@@ -614,18 +614,12 @@
     <t>RFLZ</t>
   </si>
   <si>
-    <t>D</t>
-  </si>
-  <si>
     <t>Utot</t>
   </si>
   <si>
     <t>FTTI</t>
   </si>
   <si>
-    <t>FTT-Fr Demand in Million Tkm</t>
-  </si>
-  <si>
     <t>FTT-Fr Number in Fleet</t>
   </si>
   <si>
@@ -689,9 +683,6 @@
     <t>S</t>
   </si>
   <si>
-    <t>FTT-Fr Vehicle Sales</t>
-  </si>
-  <si>
     <t>ZREG</t>
   </si>
   <si>
@@ -722,9 +713,6 @@
     <t>REG</t>
   </si>
   <si>
-    <t>Xitot</t>
-  </si>
-  <si>
     <t>FTT-Fr Spillover Matrix</t>
   </si>
   <si>
@@ -749,18 +737,9 @@
     <t>FTT-Fr Exchange Matrix</t>
   </si>
   <si>
-    <t>Costs (Sales History)</t>
-  </si>
-  <si>
-    <t>XiH</t>
-  </si>
-  <si>
     <t>RVHH</t>
   </si>
   <si>
-    <t>FTT-Fr Sales History</t>
-  </si>
-  <si>
     <t>ZESF</t>
   </si>
   <si>
@@ -776,27 +755,6 @@
     <t>ZSFD</t>
   </si>
   <si>
-    <t>dEll</t>
-  </si>
-  <si>
-    <t>Costs (Survival Function Age Derivative)</t>
-  </si>
-  <si>
-    <t>FTT-Fr Survival Function Age Derivative</t>
-  </si>
-  <si>
-    <t>ZLOD</t>
-  </si>
-  <si>
-    <t>Costs (t/v)</t>
-  </si>
-  <si>
-    <t>Load</t>
-  </si>
-  <si>
-    <t>FTT-Fr Load factors</t>
-  </si>
-  <si>
     <t>Slratio</t>
   </si>
   <si>
@@ -839,12 +797,6 @@
     <t xml:space="preserve">Costs </t>
   </si>
   <si>
-    <t>ZCET</t>
-  </si>
-  <si>
-    <t>LODZ</t>
-  </si>
-  <si>
     <t>C6TI</t>
   </si>
   <si>
@@ -903,6 +855,18 @@
   </si>
   <si>
     <t>RZFT</t>
+  </si>
+  <si>
+    <t>ZEWW</t>
+  </si>
+  <si>
+    <t>FTT-Fr Cumulative Capacities</t>
+  </si>
+  <si>
+    <t>FSTI</t>
+  </si>
+  <si>
+    <t>BZTC</t>
   </si>
 </sst>
 </file>
@@ -1271,10 +1235,10 @@
         <v>25</v>
       </c>
       <c r="H1" t="s">
-        <v>277</v>
+        <v>261</v>
       </c>
       <c r="I1" t="s">
-        <v>280</v>
+        <v>264</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1303,7 +1267,7 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1332,7 +1296,7 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1361,7 +1325,7 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1390,7 +1354,7 @@
         <v>24</v>
       </c>
       <c r="I5" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1419,7 +1383,7 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1448,7 +1412,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1477,7 +1441,7 @@
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1491,7 +1455,7 @@
         <v>31090000</v>
       </c>
       <c r="D9" t="s">
-        <v>283</v>
+        <v>267</v>
       </c>
       <c r="E9" t="s">
         <v>56</v>
@@ -1506,7 +1470,7 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1535,7 +1499,7 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1564,7 +1528,7 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1593,7 +1557,7 @@
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1622,7 +1586,7 @@
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1651,7 +1615,7 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1680,7 +1644,7 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1709,7 +1673,7 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1738,7 +1702,7 @@
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1767,7 +1731,7 @@
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1796,7 +1760,7 @@
         <v>0</v>
       </c>
       <c r="I19" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -1814,7 +1778,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E04294AC-DBC1-4E51-84ED-2EC5066B9024}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -1848,10 +1812,10 @@
         <v>25</v>
       </c>
       <c r="H1" t="s">
-        <v>277</v>
+        <v>261</v>
       </c>
       <c r="I1" t="s">
-        <v>280</v>
+        <v>264</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1877,10 +1841,10 @@
         <v>54</v>
       </c>
       <c r="H2" t="s">
-        <v>278</v>
+        <v>262</v>
       </c>
       <c r="I2" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1909,7 +1873,7 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1938,7 +1902,7 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1967,7 +1931,7 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1996,7 +1960,7 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -2025,7 +1989,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -2054,7 +2018,7 @@
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -2083,7 +2047,7 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -2112,7 +2076,7 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -2141,7 +2105,7 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -2170,7 +2134,7 @@
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -2199,7 +2163,7 @@
         <v>24</v>
       </c>
       <c r="I13" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -2228,7 +2192,7 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -2257,7 +2221,7 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -2286,7 +2250,7 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -2315,7 +2279,7 @@
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -2344,7 +2308,7 @@
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -2373,7 +2337,7 @@
         <v>0</v>
       </c>
       <c r="I19" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -2402,7 +2366,7 @@
         <v>0</v>
       </c>
       <c r="I20" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -2431,7 +2395,7 @@
         <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -2460,7 +2424,7 @@
         <v>0</v>
       </c>
       <c r="I22" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -2505,10 +2469,10 @@
         <v>25</v>
       </c>
       <c r="H1" t="s">
-        <v>277</v>
+        <v>261</v>
       </c>
       <c r="I1" t="s">
-        <v>280</v>
+        <v>264</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2537,7 +2501,7 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2566,7 +2530,7 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -2595,7 +2559,7 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -2624,7 +2588,7 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -2653,7 +2617,7 @@
         <v>24</v>
       </c>
       <c r="I6" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -2682,7 +2646,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -2711,7 +2675,7 @@
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -2740,7 +2704,7 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -2769,7 +2733,7 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -2798,7 +2762,7 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -2827,7 +2791,7 @@
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -2856,7 +2820,7 @@
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -2885,7 +2849,7 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -2914,7 +2878,7 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -2943,7 +2907,7 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -2969,10 +2933,10 @@
         <v>54</v>
       </c>
       <c r="H17" t="s">
-        <v>278</v>
+        <v>262</v>
       </c>
       <c r="I17" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -3018,10 +2982,10 @@
         <v>25</v>
       </c>
       <c r="H1" t="s">
-        <v>277</v>
+        <v>261</v>
       </c>
       <c r="I1" t="s">
-        <v>280</v>
+        <v>264</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -3050,7 +3014,7 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -3079,7 +3043,7 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -3108,7 +3072,7 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -3137,7 +3101,7 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -3166,7 +3130,7 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -3195,7 +3159,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -3224,7 +3188,7 @@
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -3253,7 +3217,7 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -3282,7 +3246,7 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -3311,7 +3275,7 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -3340,7 +3304,7 @@
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -3369,7 +3333,7 @@
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -3398,7 +3362,7 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -3427,7 +3391,7 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -3456,7 +3420,7 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -3485,7 +3449,7 @@
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -3514,7 +3478,7 @@
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -3543,7 +3507,7 @@
         <v>0</v>
       </c>
       <c r="I19" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -3572,7 +3536,7 @@
         <v>0</v>
       </c>
       <c r="I20" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -3601,7 +3565,7 @@
         <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -3630,7 +3594,7 @@
         <v>0</v>
       </c>
       <c r="I22" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -3659,7 +3623,7 @@
         <v>0</v>
       </c>
       <c r="I23" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -3688,7 +3652,7 @@
         <v>0</v>
       </c>
       <c r="I24" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -3717,7 +3681,7 @@
         <v>0</v>
       </c>
       <c r="I25" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -3727,10 +3691,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85BB7FF7-82D6-482E-815B-F3751454FF7D}">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3772,185 +3736,185 @@
         <v>188</v>
       </c>
       <c r="J1" t="s">
-        <v>277</v>
+        <v>261</v>
       </c>
       <c r="K1" t="s">
-        <v>280</v>
+        <v>264</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2">
-        <v>35330000</v>
+        <v>35320000</v>
       </c>
       <c r="D2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E2" t="s">
-        <v>54</v>
+        <v>273</v>
       </c>
       <c r="F2" t="s">
         <v>24</v>
       </c>
-      <c r="G2">
-        <v>0</v>
+      <c r="G2" t="s">
+        <v>54</v>
       </c>
       <c r="H2" t="s">
         <v>190</v>
       </c>
       <c r="I2" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="J2">
         <v>0</v>
       </c>
       <c r="K2" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>189</v>
+        <v>214</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3">
-        <v>35320000</v>
+        <v>35060000</v>
       </c>
       <c r="D3" t="s">
         <v>194</v>
       </c>
       <c r="E3" t="s">
-        <v>54</v>
+        <v>191</v>
       </c>
       <c r="F3" t="s">
         <v>24</v>
       </c>
-      <c r="G3">
-        <v>0</v>
+      <c r="G3" t="s">
+        <v>54</v>
       </c>
       <c r="H3" t="s">
-        <v>191</v>
+        <v>212</v>
       </c>
       <c r="I3" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="J3">
         <v>0</v>
       </c>
       <c r="K3" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>217</v>
+        <v>270</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4">
-        <v>35060000</v>
+        <v>35140000</v>
       </c>
       <c r="D4" t="s">
-        <v>196</v>
+        <v>209</v>
       </c>
       <c r="E4" t="s">
-        <v>192</v>
+        <v>54</v>
       </c>
       <c r="F4" t="s">
         <v>24</v>
       </c>
-      <c r="G4" t="s">
-        <v>54</v>
+      <c r="G4">
+        <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="I4" t="s">
-        <v>14</v>
+        <v>195</v>
       </c>
       <c r="J4">
         <v>0</v>
       </c>
       <c r="K4" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>195</v>
+        <v>213</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5">
-        <v>35070000</v>
+        <v>35040000</v>
       </c>
       <c r="D5" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="E5" t="s">
-        <v>54</v>
+        <v>191</v>
       </c>
       <c r="F5" t="s">
         <v>24</v>
       </c>
-      <c r="G5">
-        <v>0</v>
+      <c r="G5" t="s">
+        <v>54</v>
       </c>
       <c r="H5" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="I5" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="J5">
         <v>0</v>
       </c>
       <c r="K5" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>286</v>
+        <v>215</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6">
-        <v>35140000</v>
+        <v>35050000</v>
       </c>
       <c r="D6" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="E6" t="s">
-        <v>54</v>
+        <v>191</v>
       </c>
       <c r="F6" t="s">
         <v>24</v>
       </c>
-      <c r="G6">
-        <v>0</v>
+      <c r="G6" t="s">
+        <v>54</v>
       </c>
       <c r="H6" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="I6" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="J6">
         <v>0</v>
       </c>
       <c r="K6" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -3961,13 +3925,13 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>35040000</v>
+        <v>35020000</v>
       </c>
       <c r="D7" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F7" t="s">
         <v>24</v>
@@ -3976,33 +3940,33 @@
         <v>54</v>
       </c>
       <c r="H7" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="I7" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="J7">
         <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8">
-        <v>35050000</v>
+        <v>35030000</v>
       </c>
       <c r="D8" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F8" t="s">
         <v>24</v>
@@ -4011,7 +3975,7 @@
         <v>54</v>
       </c>
       <c r="H8" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="I8" t="s">
         <v>204</v>
@@ -4020,33 +3984,33 @@
         <v>0</v>
       </c>
       <c r="K8" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9">
-        <v>35020000</v>
+        <v>35150000</v>
       </c>
       <c r="D9" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="E9" t="s">
-        <v>192</v>
+        <v>54</v>
       </c>
       <c r="F9" t="s">
         <v>24</v>
       </c>
-      <c r="G9" t="s">
-        <v>54</v>
+      <c r="G9">
+        <v>0</v>
       </c>
       <c r="H9" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="I9" t="s">
         <v>205</v>
@@ -4055,33 +4019,33 @@
         <v>0</v>
       </c>
       <c r="K9" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10">
-        <v>35030000</v>
+        <v>35130000</v>
       </c>
       <c r="D10" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="E10" t="s">
-        <v>192</v>
+        <v>54</v>
       </c>
       <c r="F10" t="s">
         <v>24</v>
       </c>
-      <c r="G10" t="s">
-        <v>54</v>
+      <c r="G10">
+        <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>200</v>
+        <v>26</v>
       </c>
       <c r="I10" t="s">
         <v>206</v>
@@ -4090,161 +4054,161 @@
         <v>0</v>
       </c>
       <c r="K10" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11">
-        <v>35150000</v>
+        <v>35160000</v>
       </c>
       <c r="D11" t="s">
-        <v>209</v>
+        <v>230</v>
       </c>
       <c r="E11" t="s">
-        <v>54</v>
+        <v>191</v>
       </c>
       <c r="F11" t="s">
-        <v>24</v>
+        <v>191</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
       <c r="H11" t="s">
-        <v>210</v>
+        <v>229</v>
       </c>
       <c r="I11" t="s">
-        <v>207</v>
+        <v>225</v>
       </c>
       <c r="J11">
         <v>0</v>
       </c>
       <c r="K11" t="s">
-        <v>282</v>
+        <v>265</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12">
-        <v>35130000</v>
+        <v>35170000</v>
       </c>
       <c r="D12" t="s">
-        <v>198</v>
+        <v>223</v>
       </c>
       <c r="E12" t="s">
-        <v>54</v>
+        <v>191</v>
       </c>
       <c r="F12" t="s">
-        <v>24</v>
+        <v>191</v>
       </c>
       <c r="G12">
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>26</v>
+        <v>226</v>
       </c>
       <c r="I12" t="s">
-        <v>208</v>
+        <v>224</v>
       </c>
       <c r="J12">
         <v>0</v>
       </c>
       <c r="K12" t="s">
-        <v>282</v>
+        <v>265</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13">
-        <v>35160000</v>
+        <v>35190000</v>
       </c>
       <c r="D13" t="s">
+        <v>233</v>
+      </c>
+      <c r="E13" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13" t="s">
         <v>234</v>
       </c>
-      <c r="E13" t="s">
-        <v>192</v>
-      </c>
-      <c r="F13" t="s">
-        <v>192</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13" t="s">
-        <v>233</v>
-      </c>
       <c r="I13" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="J13">
         <v>0</v>
       </c>
       <c r="K13" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14">
-        <v>35170000</v>
+        <v>35370000</v>
       </c>
       <c r="D14" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="E14" t="s">
-        <v>192</v>
-      </c>
-      <c r="F14" t="s">
-        <v>192</v>
+        <v>54</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
       </c>
       <c r="G14">
         <v>0</v>
       </c>
       <c r="H14" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
       <c r="I14" t="s">
-        <v>228</v>
+        <v>238</v>
       </c>
       <c r="J14">
         <v>0</v>
       </c>
       <c r="K14" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>237</v>
+        <v>245</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15">
-        <v>35350000</v>
+        <v>35380000</v>
       </c>
       <c r="D15" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="E15" t="s">
         <v>54</v>
@@ -4256,138 +4220,138 @@
         <v>0</v>
       </c>
       <c r="H15" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="I15" t="s">
-        <v>235</v>
+        <v>244</v>
       </c>
       <c r="J15">
         <v>0</v>
       </c>
       <c r="K15" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16">
-        <v>35190000</v>
+        <v>35230000</v>
       </c>
       <c r="D16" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="E16" t="s">
-        <v>54</v>
+        <v>191</v>
       </c>
       <c r="F16" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="G16">
         <v>0</v>
       </c>
       <c r="H16" t="s">
-        <v>241</v>
+        <v>35</v>
       </c>
       <c r="I16" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="J16">
         <v>0</v>
       </c>
       <c r="K16" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>243</v>
+        <v>274</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17">
-        <v>35200000</v>
+        <v>35390000</v>
       </c>
       <c r="D17" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="E17" t="s">
-        <v>54</v>
+        <v>191</v>
       </c>
       <c r="F17" t="s">
-        <v>24</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
+        <v>251</v>
+      </c>
+      <c r="G17" t="s">
+        <v>54</v>
       </c>
       <c r="H17" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="I17" t="s">
-        <v>245</v>
-      </c>
-      <c r="J17">
-        <v>0</v>
+        <v>250</v>
+      </c>
+      <c r="J17" t="s">
+        <v>262</v>
       </c>
       <c r="K17" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18">
-        <v>35360000</v>
+        <v>35410000</v>
       </c>
       <c r="D18" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="E18" t="s">
         <v>54</v>
       </c>
-      <c r="F18" t="s">
-        <v>266</v>
+      <c r="F18">
+        <v>0</v>
       </c>
       <c r="G18">
         <v>0</v>
       </c>
       <c r="H18" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="I18" t="s">
-        <v>248</v>
-      </c>
-      <c r="J18">
-        <v>0</v>
+        <v>256</v>
+      </c>
+      <c r="J18" t="s">
+        <v>24</v>
       </c>
       <c r="K18" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>253</v>
+        <v>271</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19">
-        <v>35370000</v>
+        <v>35420000</v>
       </c>
       <c r="D19" t="s">
-        <v>254</v>
+        <v>272</v>
       </c>
       <c r="E19" t="s">
-        <v>54</v>
+        <v>191</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -4395,157 +4359,11 @@
       <c r="G19">
         <v>0</v>
       </c>
-      <c r="H19" t="s">
-        <v>251</v>
-      </c>
-      <c r="I19" t="s">
-        <v>252</v>
-      </c>
-      <c r="J19">
-        <v>0</v>
+      <c r="J19" t="s">
+        <v>24</v>
       </c>
       <c r="K19" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>259</v>
-      </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20">
-        <v>35380000</v>
-      </c>
-      <c r="D20" t="s">
-        <v>256</v>
-      </c>
-      <c r="E20" t="s">
-        <v>54</v>
-      </c>
-      <c r="F20" t="s">
-        <v>24</v>
-      </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20" t="s">
-        <v>257</v>
-      </c>
-      <c r="I20" t="s">
-        <v>258</v>
-      </c>
-      <c r="J20">
-        <v>0</v>
-      </c>
-      <c r="K20" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>255</v>
-      </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21">
-        <v>35230000</v>
-      </c>
-      <c r="D21" t="s">
-        <v>260</v>
-      </c>
-      <c r="E21" t="s">
-        <v>192</v>
-      </c>
-      <c r="F21" t="s">
-        <v>40</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21" t="s">
-        <v>35</v>
-      </c>
-      <c r="I21" t="s">
-        <v>261</v>
-      </c>
-      <c r="J21">
-        <v>0</v>
-      </c>
-      <c r="K21" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>265</v>
-      </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="C22">
-        <v>35390000</v>
-      </c>
-      <c r="D22" t="s">
-        <v>262</v>
-      </c>
-      <c r="E22" t="s">
-        <v>192</v>
-      </c>
-      <c r="F22" t="s">
-        <v>267</v>
-      </c>
-      <c r="G22" t="s">
-        <v>54</v>
-      </c>
-      <c r="H22" t="s">
-        <v>263</v>
-      </c>
-      <c r="I22" t="s">
-        <v>264</v>
-      </c>
-      <c r="J22" t="s">
-        <v>278</v>
-      </c>
-      <c r="K22" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>270</v>
-      </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="C23">
-        <v>35410000</v>
-      </c>
-      <c r="D23" t="s">
-        <v>273</v>
-      </c>
-      <c r="E23" t="s">
-        <v>54</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23">
-        <v>0</v>
-      </c>
-      <c r="H23" t="s">
-        <v>271</v>
-      </c>
-      <c r="I23" t="s">
-        <v>272</v>
-      </c>
-      <c r="J23" t="s">
-        <v>24</v>
-      </c>
-      <c r="K23" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -4555,10 +4373,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA629D80-511C-42AD-ACB3-22237E3BD282}">
-  <dimension ref="A1:B65"/>
+  <dimension ref="A1:B66"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4920,7 +4738,7 @@
         <v>186</v>
       </c>
       <c r="B45" t="s">
-        <v>268</v>
+        <v>252</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -4928,12 +4746,12 @@
         <v>189</v>
       </c>
       <c r="B46" t="s">
-        <v>268</v>
+        <v>95</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B47" t="s">
         <v>95</v>
@@ -4941,71 +4759,71 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B48" t="s">
-        <v>268</v>
+        <v>252</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>286</v>
+        <v>270</v>
       </c>
       <c r="B49" t="s">
-        <v>269</v>
+        <v>253</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B50" t="s">
-        <v>269</v>
+        <v>253</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B51" t="s">
-        <v>269</v>
+        <v>253</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B52" t="s">
-        <v>269</v>
+        <v>253</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B53" t="s">
-        <v>269</v>
+        <v>253</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B54" t="s">
-        <v>269</v>
+        <v>253</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B55" t="s">
-        <v>269</v>
+        <v>253</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="B56" t="s">
         <v>94</v>
@@ -5013,7 +4831,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="B57" t="s">
         <v>94</v>
@@ -5021,7 +4839,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="B58" t="s">
         <v>94</v>
@@ -5029,7 +4847,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="B59" t="s">
         <v>94</v>
@@ -5040,39 +4858,39 @@
         <v>31</v>
       </c>
       <c r="B60" t="s">
-        <v>274</v>
+        <v>258</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>275</v>
+        <v>259</v>
       </c>
       <c r="B61" t="s">
-        <v>276</v>
+        <v>260</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>279</v>
+        <v>263</v>
       </c>
       <c r="B62" t="s">
-        <v>276</v>
+        <v>260</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>284</v>
+        <v>268</v>
       </c>
       <c r="B63" t="s">
-        <v>276</v>
+        <v>260</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="B64" t="s">
-        <v>285</v>
+        <v>269</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -5080,7 +4898,15 @@
         <v>102</v>
       </c>
       <c r="B65" t="s">
-        <v>276</v>
+        <v>260</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>271</v>
+      </c>
+      <c r="B66" t="s">
+        <v>253</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Connected with CLEAFS and included a split market
Information on endogenous green fertiliser demand now flows to FTT:H2 where it operates in a split market
</commit_message>
<xml_diff>
--- a/Inputs/_MasterFiles/FTT_variables.xlsx
+++ b/Inputs/_MasterFiles/FTT_variables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cambridgeeconometrics-my.sharepoint.com/personal/pv_camecon_com/Documents/Documents/GitHub/FTT_H2_dev_v2/Inputs/_MasterFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="13_ncr:1_{AFC2604D-5623-4395-A28B-4C6AB9ECB063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0202E112-6033-48B3-9AB6-B02F56A5825A}"/>
+  <xr:revisionPtr revIDLastSave="78" documentId="13_ncr:1_{AFC2604D-5623-4395-A28B-4C6AB9ECB063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9B0D7664-2D8E-4B0D-9C12-AF548B4DF588}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FTT-P" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1050" uniqueCount="378">
   <si>
     <t>Variable name</t>
   </si>
@@ -1127,6 +1127,57 @@
   </si>
   <si>
     <t>FTT:Hydrogen fixed trade, subject to demand</t>
+  </si>
+  <si>
+    <t>tl_2020</t>
+  </si>
+  <si>
+    <t>WDM1</t>
+  </si>
+  <si>
+    <t>WDM2</t>
+  </si>
+  <si>
+    <t>WDM3</t>
+  </si>
+  <si>
+    <t>WDM4</t>
+  </si>
+  <si>
+    <t>WDM5</t>
+  </si>
+  <si>
+    <t>Mandate for NH3 for fertiliser</t>
+  </si>
+  <si>
+    <t>Mandate for NH3 for chemicals</t>
+  </si>
+  <si>
+    <t>Mandate for MeOH for chemicals</t>
+  </si>
+  <si>
+    <t>Mandate for H2 for oil refining</t>
+  </si>
+  <si>
+    <t>Mandate for H2 for energy purposes</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>S4</t>
+  </si>
+  <si>
+    <t>S5</t>
+  </si>
+  <si>
+    <t>HYGR</t>
   </si>
 </sst>
 </file>
@@ -5087,10 +5138,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05986654-6C49-4A34-BECD-4482E94CE084}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:A25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5771,7 +5822,7 @@
         <v>1</v>
       </c>
       <c r="C24">
-        <f t="shared" ref="C24:C25" si="0">C23+1000</f>
+        <f t="shared" ref="C24:C30" si="0">C23+1000</f>
         <v>3628000</v>
       </c>
       <c r="D24" t="s">
@@ -5820,6 +5871,185 @@
         <v>0</v>
       </c>
       <c r="I25" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>362</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>3630000</v>
+      </c>
+      <c r="D26" t="s">
+        <v>367</v>
+      </c>
+      <c r="E26" t="s">
+        <v>54</v>
+      </c>
+      <c r="F26" t="s">
+        <v>24</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>363</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>3631000</v>
+      </c>
+      <c r="D27" t="s">
+        <v>368</v>
+      </c>
+      <c r="E27" t="s">
+        <v>54</v>
+      </c>
+      <c r="F27" t="s">
+        <v>24</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>364</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>3632000</v>
+      </c>
+      <c r="D28" t="s">
+        <v>369</v>
+      </c>
+      <c r="E28" t="s">
+        <v>54</v>
+      </c>
+      <c r="F28" t="s">
+        <v>24</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>365</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>3633000</v>
+      </c>
+      <c r="D29" t="s">
+        <v>370</v>
+      </c>
+      <c r="E29" t="s">
+        <v>54</v>
+      </c>
+      <c r="F29" t="s">
+        <v>24</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>366</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>3634000</v>
+      </c>
+      <c r="D30" t="s">
+        <v>371</v>
+      </c>
+      <c r="E30" t="s">
+        <v>54</v>
+      </c>
+      <c r="F30" t="s">
+        <v>24</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>377</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>3609000</v>
+      </c>
+      <c r="D31" t="s">
+        <v>316</v>
+      </c>
+      <c r="E31" t="s">
+        <v>317</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31" t="s">
+        <v>24</v>
+      </c>
+      <c r="I31" t="s">
         <v>292</v>
       </c>
     </row>
@@ -5831,10 +6061,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA629D80-511C-42AD-ACB3-22237E3BD282}">
-  <dimension ref="A1:B90"/>
+  <dimension ref="A1:B96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B90" sqref="B90"/>
+    <sheetView topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="E97" sqref="E97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6380,7 +6610,7 @@
         <v>320</v>
       </c>
       <c r="B68" t="s">
-        <v>305</v>
+        <v>361</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -6557,6 +6787,54 @@
       </c>
       <c r="B90" t="s">
         <v>95</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>362</v>
+      </c>
+      <c r="B91" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>363</v>
+      </c>
+      <c r="B92" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>364</v>
+      </c>
+      <c r="B93" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>365</v>
+      </c>
+      <c r="B94" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>366</v>
+      </c>
+      <c r="B95" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>377</v>
+      </c>
+      <c r="B96" t="s">
+        <v>319</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Version used for policy brief v1
Fixed a mistake to off-grid electrolytic capacity factors.

Hard-coded lifetime adjustments to the Aij matrix to reflect that low carbon capacity is new and probably won't phase out as quickly.
</commit_message>
<xml_diff>
--- a/Inputs/_MasterFiles/FTT_variables.xlsx
+++ b/Inputs/_MasterFiles/FTT_variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cambridgeeconometrics-my.sharepoint.com/personal/pv_camecon_com/Documents/Documents/GitHub/FTT_H2_dev_v2/Inputs/_MasterFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="96" documentId="13_ncr:1_{AFC2604D-5623-4395-A28B-4C6AB9ECB063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BAC31FC2-2FE2-4358-B0B5-617FC6AA0A4E}"/>
+  <xr:revisionPtr revIDLastSave="103" documentId="13_ncr:1_{AFC2604D-5623-4395-A28B-4C6AB9ECB063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{13BDABD5-692B-48F8-9EE4-9EB7BCA6A258}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FTT-P" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1079" uniqueCount="381">
   <si>
     <t>Variable name</t>
   </si>
@@ -1181,6 +1181,12 @@
   </si>
   <si>
     <t>Share of dedicated green power tech that is solar</t>
+  </si>
+  <si>
+    <t>WBMT</t>
+  </si>
+  <si>
+    <t>Capacity additions for the default market</t>
   </si>
 </sst>
 </file>
@@ -1531,16 +1537,16 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.81640625" customWidth="1"/>
+    <col min="7" max="7" width="14.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1569,7 +1575,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1598,7 +1604,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>58</v>
       </c>
@@ -1627,7 +1633,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>62</v>
       </c>
@@ -1656,7 +1662,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>63</v>
       </c>
@@ -1685,7 +1691,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>74</v>
       </c>
@@ -1714,7 +1720,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>84</v>
       </c>
@@ -1743,7 +1749,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -1772,7 +1778,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>79</v>
       </c>
@@ -1801,7 +1807,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>70</v>
       </c>
@@ -1830,7 +1836,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>72</v>
       </c>
@@ -1859,7 +1865,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -1888,7 +1894,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>81</v>
       </c>
@@ -1917,7 +1923,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>88</v>
       </c>
@@ -1946,7 +1952,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>90</v>
       </c>
@@ -1975,7 +1981,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>80</v>
       </c>
@@ -2004,7 +2010,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>82</v>
       </c>
@@ -2033,7 +2039,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>66</v>
       </c>
@@ -2062,7 +2068,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>76</v>
       </c>
@@ -2110,14 +2116,14 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.5703125" customWidth="1"/>
+    <col min="2" max="2" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2146,7 +2152,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2175,7 +2181,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2204,7 +2210,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -2233,7 +2239,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2262,7 +2268,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -2291,7 +2297,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -2320,7 +2326,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -2349,7 +2355,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -2378,7 +2384,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -2407,7 +2413,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -2436,7 +2442,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -2465,7 +2471,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -2494,7 +2500,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -2523,7 +2529,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -2552,7 +2558,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -2581,7 +2587,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -2610,7 +2616,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -2639,7 +2645,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -2668,7 +2674,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -2697,7 +2703,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -2726,7 +2732,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>52</v>
       </c>
@@ -2768,13 +2774,13 @@
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.42578125" customWidth="1"/>
+    <col min="2" max="2" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2803,7 +2809,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>96</v>
       </c>
@@ -2832,7 +2838,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>99</v>
       </c>
@@ -2861,7 +2867,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>100</v>
       </c>
@@ -2890,7 +2896,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>101</v>
       </c>
@@ -2919,7 +2925,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>102</v>
       </c>
@@ -2948,7 +2954,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>103</v>
       </c>
@@ -2977,7 +2983,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>104</v>
       </c>
@@ -3006,7 +3012,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>105</v>
       </c>
@@ -3035,7 +3041,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>106</v>
       </c>
@@ -3064,7 +3070,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>107</v>
       </c>
@@ -3093,7 +3099,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>108</v>
       </c>
@@ -3122,7 +3128,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>109</v>
       </c>
@@ -3151,7 +3157,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>110</v>
       </c>
@@ -3180,7 +3186,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>111</v>
       </c>
@@ -3209,7 +3215,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>112</v>
       </c>
@@ -3238,7 +3244,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>113</v>
       </c>
@@ -3280,14 +3286,14 @@
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="50.5703125" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.54296875" customWidth="1"/>
+    <col min="5" max="5" width="9.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3316,7 +3322,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>131</v>
       </c>
@@ -3345,7 +3351,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>155</v>
       </c>
@@ -3374,7 +3380,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>132</v>
       </c>
@@ -3403,7 +3409,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>133</v>
       </c>
@@ -3432,7 +3438,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>134</v>
       </c>
@@ -3461,7 +3467,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>135</v>
       </c>
@@ -3490,7 +3496,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>136</v>
       </c>
@@ -3519,7 +3525,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>137</v>
       </c>
@@ -3548,7 +3554,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>138</v>
       </c>
@@ -3577,7 +3583,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>139</v>
       </c>
@@ -3606,7 +3612,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>140</v>
       </c>
@@ -3635,7 +3641,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>141</v>
       </c>
@@ -3664,7 +3670,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>142</v>
       </c>
@@ -3693,7 +3699,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>143</v>
       </c>
@@ -3722,7 +3728,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>144</v>
       </c>
@@ -3751,7 +3757,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>145</v>
       </c>
@@ -3780,7 +3786,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>146</v>
       </c>
@@ -3809,7 +3815,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>147</v>
       </c>
@@ -3838,7 +3844,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>148</v>
       </c>
@@ -3867,7 +3873,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>149</v>
       </c>
@@ -3896,7 +3902,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>150</v>
       </c>
@@ -3925,7 +3931,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>151</v>
       </c>
@@ -3954,7 +3960,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>152</v>
       </c>
@@ -3983,7 +3989,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>153</v>
       </c>
@@ -4025,17 +4031,17 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.54296875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4070,7 +4076,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>186</v>
       </c>
@@ -4105,7 +4111,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>189</v>
       </c>
@@ -4140,7 +4146,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>220</v>
       </c>
@@ -4175,7 +4181,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>195</v>
       </c>
@@ -4210,7 +4216,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>198</v>
       </c>
@@ -4245,7 +4251,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>219</v>
       </c>
@@ -4280,7 +4286,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>221</v>
       </c>
@@ -4315,7 +4321,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>222</v>
       </c>
@@ -4350,7 +4356,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>223</v>
       </c>
@@ -4385,7 +4391,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>224</v>
       </c>
@@ -4420,7 +4426,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>225</v>
       </c>
@@ -4455,7 +4461,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>215</v>
       </c>
@@ -4490,7 +4496,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>229</v>
       </c>
@@ -4522,7 +4528,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>231</v>
       </c>
@@ -4554,7 +4560,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>238</v>
       </c>
@@ -4589,7 +4595,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>239</v>
       </c>
@@ -4624,7 +4630,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>242</v>
       </c>
@@ -4659,7 +4665,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>248</v>
       </c>
@@ -4694,7 +4700,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>250</v>
       </c>
@@ -4729,7 +4735,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>254</v>
       </c>
@@ -4764,7 +4770,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>258</v>
       </c>
@@ -4799,7 +4805,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>264</v>
       </c>
@@ -4834,7 +4840,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>270</v>
       </c>
@@ -4869,7 +4875,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>266</v>
       </c>
@@ -4904,7 +4910,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>276</v>
       </c>
@@ -4939,7 +4945,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>281</v>
       </c>
@@ -4987,9 +4993,9 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5018,7 +5024,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>297</v>
       </c>
@@ -5047,7 +5053,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>320</v>
       </c>
@@ -5076,7 +5082,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>298</v>
       </c>
@@ -5105,7 +5111,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>304</v>
       </c>
@@ -5141,15 +5147,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05986654-6C49-4A34-BECD-4482E94CE084}">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:A34"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35:I35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5178,7 +5184,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>307</v>
       </c>
@@ -5207,7 +5213,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>308</v>
       </c>
@@ -5236,7 +5242,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>309</v>
       </c>
@@ -5265,7 +5271,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>310</v>
       </c>
@@ -5294,7 +5300,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>311</v>
       </c>
@@ -5323,7 +5329,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>322</v>
       </c>
@@ -5352,7 +5358,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>325</v>
       </c>
@@ -5381,7 +5387,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>326</v>
       </c>
@@ -5410,7 +5416,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>327</v>
       </c>
@@ -5439,7 +5445,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>328</v>
       </c>
@@ -5468,7 +5474,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>329</v>
       </c>
@@ -5497,7 +5503,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>330</v>
       </c>
@@ -5526,7 +5532,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>331</v>
       </c>
@@ -5555,7 +5561,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>332</v>
       </c>
@@ -5584,7 +5590,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>333</v>
       </c>
@@ -5613,7 +5619,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>334</v>
       </c>
@@ -5642,7 +5648,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>335</v>
       </c>
@@ -5671,7 +5677,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>336</v>
       </c>
@@ -5700,7 +5706,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>337</v>
       </c>
@@ -5729,7 +5735,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>338</v>
       </c>
@@ -5758,7 +5764,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>339</v>
       </c>
@@ -5787,7 +5793,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>355</v>
       </c>
@@ -5817,7 +5823,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>356</v>
       </c>
@@ -5847,7 +5853,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>357</v>
       </c>
@@ -5877,7 +5883,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>362</v>
       </c>
@@ -5907,7 +5913,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>363</v>
       </c>
@@ -5937,7 +5943,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>364</v>
       </c>
@@ -5967,7 +5973,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>365</v>
       </c>
@@ -5997,7 +6003,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>366</v>
       </c>
@@ -6027,7 +6033,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>372</v>
       </c>
@@ -6056,7 +6062,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>373</v>
       </c>
@@ -6085,7 +6091,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>374</v>
       </c>
@@ -6114,7 +6120,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>375</v>
       </c>
@@ -6140,6 +6146,35 @@
         <v>0</v>
       </c>
       <c r="I34" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>379</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>36380000</v>
+      </c>
+      <c r="D35" t="s">
+        <v>380</v>
+      </c>
+      <c r="E35" t="s">
+        <v>317</v>
+      </c>
+      <c r="F35" t="s">
+        <v>24</v>
+      </c>
+      <c r="G35" t="s">
+        <v>54</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35" t="s">
         <v>292</v>
       </c>
     </row>
@@ -6151,15 +6186,15 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA629D80-511C-42AD-ACB3-22237E3BD282}">
-  <dimension ref="A1:B99"/>
+  <dimension ref="A1:B100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="B99" sqref="B99"/>
+      <selection activeCell="B100" sqref="B100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6167,7 +6202,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -6175,7 +6210,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -6183,7 +6218,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -6191,7 +6226,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -6199,7 +6234,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -6207,7 +6242,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -6215,7 +6250,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -6223,7 +6258,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -6231,7 +6266,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -6239,7 +6274,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -6247,7 +6282,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -6255,7 +6290,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -6263,7 +6298,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>58</v>
       </c>
@@ -6271,7 +6306,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>62</v>
       </c>
@@ -6279,7 +6314,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>63</v>
       </c>
@@ -6287,7 +6322,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>74</v>
       </c>
@@ -6295,7 +6330,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>79</v>
       </c>
@@ -6303,7 +6338,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>70</v>
       </c>
@@ -6311,7 +6346,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>72</v>
       </c>
@@ -6319,7 +6354,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>68</v>
       </c>
@@ -6327,7 +6362,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>66</v>
       </c>
@@ -6335,7 +6370,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>76</v>
       </c>
@@ -6343,7 +6378,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>103</v>
       </c>
@@ -6351,7 +6386,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>104</v>
       </c>
@@ -6359,7 +6394,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>105</v>
       </c>
@@ -6367,7 +6402,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>106</v>
       </c>
@@ -6375,7 +6410,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>107</v>
       </c>
@@ -6383,7 +6418,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>108</v>
       </c>
@@ -6391,7 +6426,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>109</v>
       </c>
@@ -6399,7 +6434,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>110</v>
       </c>
@@ -6407,7 +6442,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>111</v>
       </c>
@@ -6415,7 +6450,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>112</v>
       </c>
@@ -6423,7 +6458,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>130</v>
       </c>
@@ -6431,7 +6466,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>131</v>
       </c>
@@ -6439,7 +6474,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>155</v>
       </c>
@@ -6447,7 +6482,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>132</v>
       </c>
@@ -6455,7 +6490,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>147</v>
       </c>
@@ -6463,7 +6498,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>148</v>
       </c>
@@ -6471,7 +6506,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>149</v>
       </c>
@@ -6479,7 +6514,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>150</v>
       </c>
@@ -6487,7 +6522,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>151</v>
       </c>
@@ -6495,7 +6530,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>152</v>
       </c>
@@ -6503,7 +6538,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>153</v>
       </c>
@@ -6511,7 +6546,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>186</v>
       </c>
@@ -6519,7 +6554,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>189</v>
       </c>
@@ -6527,7 +6562,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>220</v>
       </c>
@@ -6535,7 +6570,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>195</v>
       </c>
@@ -6543,7 +6578,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>198</v>
       </c>
@@ -6551,7 +6586,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>219</v>
       </c>
@@ -6559,7 +6594,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>221</v>
       </c>
@@ -6567,7 +6602,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>222</v>
       </c>
@@ -6575,7 +6610,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>223</v>
       </c>
@@ -6583,7 +6618,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>224</v>
       </c>
@@ -6591,7 +6626,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>225</v>
       </c>
@@ -6599,7 +6634,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>215</v>
       </c>
@@ -6607,7 +6642,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>248</v>
       </c>
@@ -6615,7 +6650,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>250</v>
       </c>
@@ -6623,7 +6658,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>254</v>
       </c>
@@ -6631,7 +6666,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>270</v>
       </c>
@@ -6639,7 +6674,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>31</v>
       </c>
@@ -6647,7 +6682,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>286</v>
       </c>
@@ -6655,7 +6690,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>290</v>
       </c>
@@ -6663,7 +6698,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>295</v>
       </c>
@@ -6671,7 +6706,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>281</v>
       </c>
@@ -6679,7 +6714,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>102</v>
       </c>
@@ -6687,7 +6722,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>297</v>
       </c>
@@ -6695,7 +6730,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>320</v>
       </c>
@@ -6703,7 +6738,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>304</v>
       </c>
@@ -6711,7 +6746,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>308</v>
       </c>
@@ -6719,7 +6754,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>311</v>
       </c>
@@ -6727,7 +6762,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>322</v>
       </c>
@@ -6735,7 +6770,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>309</v>
       </c>
@@ -6743,7 +6778,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>325</v>
       </c>
@@ -6751,7 +6786,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>326</v>
       </c>
@@ -6759,7 +6794,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>327</v>
       </c>
@@ -6767,7 +6802,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>328</v>
       </c>
@@ -6775,7 +6810,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>329</v>
       </c>
@@ -6783,7 +6818,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>330</v>
       </c>
@@ -6791,7 +6826,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>331</v>
       </c>
@@ -6799,7 +6834,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>332</v>
       </c>
@@ -6807,7 +6842,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>333</v>
       </c>
@@ -6815,7 +6850,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>334</v>
       </c>
@@ -6823,7 +6858,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>335</v>
       </c>
@@ -6831,7 +6866,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>336</v>
       </c>
@@ -6839,7 +6874,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>337</v>
       </c>
@@ -6847,7 +6882,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>339</v>
       </c>
@@ -6855,7 +6890,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>355</v>
       </c>
@@ -6863,7 +6898,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>356</v>
       </c>
@@ -6871,7 +6906,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>357</v>
       </c>
@@ -6879,7 +6914,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>362</v>
       </c>
@@ -6887,7 +6922,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>363</v>
       </c>
@@ -6895,7 +6930,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>364</v>
       </c>
@@ -6903,7 +6938,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>365</v>
       </c>
@@ -6911,7 +6946,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>366</v>
       </c>
@@ -6919,7 +6954,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>372</v>
       </c>
@@ -6927,7 +6962,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>373</v>
       </c>
@@ -6935,7 +6970,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>374</v>
       </c>
@@ -6943,11 +6978,19 @@
         <v>95</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>375</v>
       </c>
       <c r="B99" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>379</v>
+      </c>
+      <c r="B100" t="s">
         <v>95</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Master file and variables list update
Adding all input csvs to the master
</commit_message>
<xml_diff>
--- a/Inputs/_MasterFiles/FTT_variables.xlsx
+++ b/Inputs/_MasterFiles/FTT_variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cambridgeeconometrics-my.sharepoint.com/personal/pv_camecon_com/Documents/Documents/GitHub/FTT_H2_dev_v2/Inputs/_MasterFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cambridgeeconometrics-my.sharepoint.com/personal/bb_camecon_com/Documents/Documents/GitHub/FTT_StandAlone/Inputs/_MasterFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="103" documentId="13_ncr:1_{AFC2604D-5623-4395-A28B-4C6AB9ECB063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{13BDABD5-692B-48F8-9EE4-9EB7BCA6A258}"/>
+  <xr:revisionPtr revIDLastSave="171" documentId="13_ncr:1_{AFC2604D-5623-4395-A28B-4C6AB9ECB063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{325B89AB-3974-4A7B-86D8-DD71DD53CA61}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-45" yWindow="-16200" windowWidth="14610" windowHeight="15585" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FTT-P" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1079" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1142" uniqueCount="399">
   <si>
     <t>Variable name</t>
   </si>
@@ -1187,13 +1187,67 @@
   </si>
   <si>
     <t>Capacity additions for the default market</t>
+  </si>
+  <si>
+    <t>WWIC</t>
+  </si>
+  <si>
+    <t>WOIC</t>
+  </si>
+  <si>
+    <t>WSIC</t>
+  </si>
+  <si>
+    <t>WWOM</t>
+  </si>
+  <si>
+    <t>WOOM</t>
+  </si>
+  <si>
+    <t>WSOM</t>
+  </si>
+  <si>
+    <t>WWLF</t>
+  </si>
+  <si>
+    <t>WOLF</t>
+  </si>
+  <si>
+    <t>WSLF</t>
+  </si>
+  <si>
+    <t>Solar load factor</t>
+  </si>
+  <si>
+    <t>Offshore wind load factor</t>
+  </si>
+  <si>
+    <t>Onshore wind load factor</t>
+  </si>
+  <si>
+    <t>Onshore wind CAPEX</t>
+  </si>
+  <si>
+    <t>Offshore wind CAPEX</t>
+  </si>
+  <si>
+    <t>Solar CAPEX</t>
+  </si>
+  <si>
+    <t>Onshore wind OPEX</t>
+  </si>
+  <si>
+    <t>Offshore wind OPEX</t>
+  </si>
+  <si>
+    <t>Solar OPEX</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1203,6 +1257,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1246,11 +1307,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1537,16 +1599,16 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="12.81640625" customWidth="1"/>
-    <col min="7" max="7" width="14.453125" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1575,7 +1637,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1604,7 +1666,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>58</v>
       </c>
@@ -1633,7 +1695,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>62</v>
       </c>
@@ -1662,7 +1724,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>63</v>
       </c>
@@ -1691,7 +1753,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>74</v>
       </c>
@@ -1720,7 +1782,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>84</v>
       </c>
@@ -1749,7 +1811,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -1778,7 +1840,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>79</v>
       </c>
@@ -1807,7 +1869,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>70</v>
       </c>
@@ -1836,7 +1898,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>72</v>
       </c>
@@ -1865,7 +1927,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -1894,7 +1956,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>81</v>
       </c>
@@ -1923,7 +1985,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>88</v>
       </c>
@@ -1952,7 +2014,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>90</v>
       </c>
@@ -1981,7 +2043,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>80</v>
       </c>
@@ -2010,7 +2072,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>82</v>
       </c>
@@ -2039,7 +2101,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>66</v>
       </c>
@@ -2068,7 +2130,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>76</v>
       </c>
@@ -2116,14 +2178,14 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.54296875" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2152,7 +2214,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2181,7 +2243,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2210,7 +2272,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -2239,7 +2301,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2268,7 +2330,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -2297,7 +2359,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -2326,7 +2388,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -2355,7 +2417,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -2384,7 +2446,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -2413,7 +2475,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -2442,7 +2504,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -2471,7 +2533,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -2500,7 +2562,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -2529,7 +2591,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -2558,7 +2620,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -2587,7 +2649,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -2616,7 +2678,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -2645,7 +2707,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -2674,7 +2736,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -2703,7 +2765,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -2732,7 +2794,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>52</v>
       </c>
@@ -2774,13 +2836,13 @@
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.453125" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2809,7 +2871,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>96</v>
       </c>
@@ -2838,7 +2900,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>99</v>
       </c>
@@ -2867,7 +2929,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>100</v>
       </c>
@@ -2896,7 +2958,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>101</v>
       </c>
@@ -2925,7 +2987,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>102</v>
       </c>
@@ -2954,7 +3016,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>103</v>
       </c>
@@ -2983,7 +3045,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>104</v>
       </c>
@@ -3012,7 +3074,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>105</v>
       </c>
@@ -3041,7 +3103,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>106</v>
       </c>
@@ -3070,7 +3132,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>107</v>
       </c>
@@ -3099,7 +3161,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>108</v>
       </c>
@@ -3128,7 +3190,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>109</v>
       </c>
@@ -3157,7 +3219,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>110</v>
       </c>
@@ -3186,7 +3248,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>111</v>
       </c>
@@ -3215,7 +3277,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>112</v>
       </c>
@@ -3244,7 +3306,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>113</v>
       </c>
@@ -3286,14 +3348,14 @@
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="50.54296875" customWidth="1"/>
-    <col min="5" max="5" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.5703125" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3322,7 +3384,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>131</v>
       </c>
@@ -3351,7 +3413,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>155</v>
       </c>
@@ -3380,7 +3442,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>132</v>
       </c>
@@ -3409,7 +3471,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>133</v>
       </c>
@@ -3438,7 +3500,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>134</v>
       </c>
@@ -3467,7 +3529,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>135</v>
       </c>
@@ -3496,7 +3558,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>136</v>
       </c>
@@ -3525,7 +3587,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>137</v>
       </c>
@@ -3554,7 +3616,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>138</v>
       </c>
@@ -3583,7 +3645,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>139</v>
       </c>
@@ -3612,7 +3674,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>140</v>
       </c>
@@ -3641,7 +3703,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>141</v>
       </c>
@@ -3670,7 +3732,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>142</v>
       </c>
@@ -3699,7 +3761,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>143</v>
       </c>
@@ -3728,7 +3790,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>144</v>
       </c>
@@ -3757,7 +3819,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>145</v>
       </c>
@@ -3786,7 +3848,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>146</v>
       </c>
@@ -3815,7 +3877,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>147</v>
       </c>
@@ -3844,7 +3906,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>148</v>
       </c>
@@ -3873,7 +3935,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>149</v>
       </c>
@@ -3902,7 +3964,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>150</v>
       </c>
@@ -3931,7 +3993,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>151</v>
       </c>
@@ -3960,7 +4022,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>152</v>
       </c>
@@ -3989,7 +4051,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>153</v>
       </c>
@@ -4031,17 +4093,17 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4076,7 +4138,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>186</v>
       </c>
@@ -4111,7 +4173,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>189</v>
       </c>
@@ -4146,7 +4208,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>220</v>
       </c>
@@ -4181,7 +4243,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>195</v>
       </c>
@@ -4216,7 +4278,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>198</v>
       </c>
@@ -4251,7 +4313,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>219</v>
       </c>
@@ -4286,7 +4348,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>221</v>
       </c>
@@ -4321,7 +4383,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>222</v>
       </c>
@@ -4356,7 +4418,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>223</v>
       </c>
@@ -4391,7 +4453,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>224</v>
       </c>
@@ -4426,7 +4488,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>225</v>
       </c>
@@ -4461,7 +4523,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>215</v>
       </c>
@@ -4496,7 +4558,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>229</v>
       </c>
@@ -4528,7 +4590,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>231</v>
       </c>
@@ -4560,7 +4622,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>238</v>
       </c>
@@ -4595,7 +4657,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>239</v>
       </c>
@@ -4630,7 +4692,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>242</v>
       </c>
@@ -4665,7 +4727,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>248</v>
       </c>
@@ -4700,7 +4762,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>250</v>
       </c>
@@ -4735,7 +4797,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>254</v>
       </c>
@@ -4770,7 +4832,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>258</v>
       </c>
@@ -4805,7 +4867,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>264</v>
       </c>
@@ -4840,7 +4902,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>270</v>
       </c>
@@ -4875,7 +4937,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>266</v>
       </c>
@@ -4910,7 +4972,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>276</v>
       </c>
@@ -4945,7 +5007,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>281</v>
       </c>
@@ -4993,9 +5055,9 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5024,7 +5086,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>297</v>
       </c>
@@ -5053,7 +5115,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>320</v>
       </c>
@@ -5082,7 +5144,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>298</v>
       </c>
@@ -5111,7 +5173,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>304</v>
       </c>
@@ -5147,15 +5209,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05986654-6C49-4A34-BECD-4482E94CE084}">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35:I35"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5184,7 +5246,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>307</v>
       </c>
@@ -5213,7 +5275,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>308</v>
       </c>
@@ -5242,7 +5304,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>309</v>
       </c>
@@ -5271,7 +5333,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>310</v>
       </c>
@@ -5300,7 +5362,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>311</v>
       </c>
@@ -5329,7 +5391,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>322</v>
       </c>
@@ -5358,7 +5420,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>325</v>
       </c>
@@ -5387,7 +5449,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>326</v>
       </c>
@@ -5416,7 +5478,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>327</v>
       </c>
@@ -5445,7 +5507,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>328</v>
       </c>
@@ -5474,7 +5536,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>329</v>
       </c>
@@ -5503,7 +5565,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>330</v>
       </c>
@@ -5532,7 +5594,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>331</v>
       </c>
@@ -5561,7 +5623,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>332</v>
       </c>
@@ -5590,7 +5652,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>333</v>
       </c>
@@ -5619,7 +5681,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>334</v>
       </c>
@@ -5648,7 +5710,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>335</v>
       </c>
@@ -5677,7 +5739,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>336</v>
       </c>
@@ -5706,7 +5768,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>337</v>
       </c>
@@ -5735,7 +5797,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>338</v>
       </c>
@@ -5764,7 +5826,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>339</v>
       </c>
@@ -5793,7 +5855,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>355</v>
       </c>
@@ -5823,7 +5885,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>356</v>
       </c>
@@ -5853,7 +5915,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>357</v>
       </c>
@@ -5883,7 +5945,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>362</v>
       </c>
@@ -5913,7 +5975,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>363</v>
       </c>
@@ -5943,7 +6005,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>364</v>
       </c>
@@ -5973,7 +6035,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>365</v>
       </c>
@@ -6003,7 +6065,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>366</v>
       </c>
@@ -6033,7 +6095,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>372</v>
       </c>
@@ -6062,7 +6124,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>373</v>
       </c>
@@ -6091,7 +6153,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>374</v>
       </c>
@@ -6120,7 +6182,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>375</v>
       </c>
@@ -6149,7 +6211,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>379</v>
       </c>
@@ -6177,6 +6239,276 @@
       <c r="I35" t="s">
         <v>292</v>
       </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>36390000</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="E36" t="s">
+        <v>54</v>
+      </c>
+      <c r="F36" t="s">
+        <v>24</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>36400000</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="E37" t="s">
+        <v>54</v>
+      </c>
+      <c r="F37" t="s">
+        <v>24</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <v>36410000</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="E38" t="s">
+        <v>54</v>
+      </c>
+      <c r="F38" t="s">
+        <v>24</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>36420000</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="E39" t="s">
+        <v>54</v>
+      </c>
+      <c r="F39" t="s">
+        <v>24</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <v>36430000</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="E40" t="s">
+        <v>54</v>
+      </c>
+      <c r="F40" t="s">
+        <v>24</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <v>36440000</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="E41" t="s">
+        <v>54</v>
+      </c>
+      <c r="F41" t="s">
+        <v>24</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>36450000</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="E42" t="s">
+        <v>54</v>
+      </c>
+      <c r="F42" t="s">
+        <v>24</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>388</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <v>36460000</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="E43" t="s">
+        <v>54</v>
+      </c>
+      <c r="F43" t="s">
+        <v>24</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>389</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <v>36470000</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="E44" t="s">
+        <v>54</v>
+      </c>
+      <c r="F44" t="s">
+        <v>24</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="4"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="4"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -6186,15 +6518,15 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA629D80-511C-42AD-ACB3-22237E3BD282}">
-  <dimension ref="A1:B100"/>
+  <dimension ref="A1:B109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="B100" sqref="B100"/>
+    <sheetView topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="B109" sqref="B109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6202,7 +6534,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -6210,7 +6542,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -6218,7 +6550,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -6226,7 +6558,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -6234,7 +6566,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -6242,7 +6574,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -6250,7 +6582,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -6258,7 +6590,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -6266,7 +6598,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -6274,7 +6606,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -6282,7 +6614,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -6290,7 +6622,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -6298,7 +6630,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>58</v>
       </c>
@@ -6306,7 +6638,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>62</v>
       </c>
@@ -6314,7 +6646,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>63</v>
       </c>
@@ -6322,7 +6654,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>74</v>
       </c>
@@ -6330,7 +6662,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>79</v>
       </c>
@@ -6338,7 +6670,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>70</v>
       </c>
@@ -6346,7 +6678,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>72</v>
       </c>
@@ -6354,7 +6686,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>68</v>
       </c>
@@ -6362,7 +6694,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>66</v>
       </c>
@@ -6370,7 +6702,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>76</v>
       </c>
@@ -6378,7 +6710,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>103</v>
       </c>
@@ -6386,7 +6718,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>104</v>
       </c>
@@ -6394,7 +6726,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>105</v>
       </c>
@@ -6402,7 +6734,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>106</v>
       </c>
@@ -6410,7 +6742,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>107</v>
       </c>
@@ -6418,7 +6750,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>108</v>
       </c>
@@ -6426,7 +6758,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>109</v>
       </c>
@@ -6434,7 +6766,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>110</v>
       </c>
@@ -6442,7 +6774,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>111</v>
       </c>
@@ -6450,7 +6782,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>112</v>
       </c>
@@ -6458,7 +6790,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>130</v>
       </c>
@@ -6466,7 +6798,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>131</v>
       </c>
@@ -6474,7 +6806,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>155</v>
       </c>
@@ -6482,7 +6814,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>132</v>
       </c>
@@ -6490,7 +6822,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>147</v>
       </c>
@@ -6498,7 +6830,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>148</v>
       </c>
@@ -6506,7 +6838,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>149</v>
       </c>
@@ -6514,7 +6846,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>150</v>
       </c>
@@ -6522,7 +6854,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>151</v>
       </c>
@@ -6530,7 +6862,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>152</v>
       </c>
@@ -6538,7 +6870,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>153</v>
       </c>
@@ -6546,7 +6878,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>186</v>
       </c>
@@ -6554,7 +6886,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>189</v>
       </c>
@@ -6562,7 +6894,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>220</v>
       </c>
@@ -6570,7 +6902,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>195</v>
       </c>
@@ -6578,7 +6910,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>198</v>
       </c>
@@ -6586,7 +6918,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>219</v>
       </c>
@@ -6594,7 +6926,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>221</v>
       </c>
@@ -6602,7 +6934,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>222</v>
       </c>
@@ -6610,7 +6942,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>223</v>
       </c>
@@ -6618,7 +6950,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>224</v>
       </c>
@@ -6626,7 +6958,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>225</v>
       </c>
@@ -6634,7 +6966,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>215</v>
       </c>
@@ -6642,7 +6974,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>248</v>
       </c>
@@ -6650,7 +6982,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>250</v>
       </c>
@@ -6658,7 +6990,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>254</v>
       </c>
@@ -6666,7 +6998,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>270</v>
       </c>
@@ -6674,7 +7006,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>31</v>
       </c>
@@ -6682,7 +7014,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>286</v>
       </c>
@@ -6690,7 +7022,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>290</v>
       </c>
@@ -6698,7 +7030,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>295</v>
       </c>
@@ -6706,7 +7038,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>281</v>
       </c>
@@ -6714,7 +7046,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>102</v>
       </c>
@@ -6722,7 +7054,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>297</v>
       </c>
@@ -6730,7 +7062,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>320</v>
       </c>
@@ -6738,7 +7070,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>304</v>
       </c>
@@ -6746,7 +7078,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>308</v>
       </c>
@@ -6754,7 +7086,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>311</v>
       </c>
@@ -6762,7 +7094,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>322</v>
       </c>
@@ -6770,7 +7102,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>309</v>
       </c>
@@ -6778,7 +7110,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>325</v>
       </c>
@@ -6786,7 +7118,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>326</v>
       </c>
@@ -6794,7 +7126,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>327</v>
       </c>
@@ -6802,7 +7134,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>328</v>
       </c>
@@ -6810,7 +7142,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>329</v>
       </c>
@@ -6818,7 +7150,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>330</v>
       </c>
@@ -6826,7 +7158,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>331</v>
       </c>
@@ -6834,7 +7166,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>332</v>
       </c>
@@ -6842,7 +7174,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>333</v>
       </c>
@@ -6850,7 +7182,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>334</v>
       </c>
@@ -6858,7 +7190,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>335</v>
       </c>
@@ -6866,7 +7198,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>336</v>
       </c>
@@ -6874,7 +7206,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>337</v>
       </c>
@@ -6882,7 +7214,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>339</v>
       </c>
@@ -6890,7 +7222,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>355</v>
       </c>
@@ -6898,7 +7230,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>356</v>
       </c>
@@ -6906,7 +7238,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>357</v>
       </c>
@@ -6914,7 +7246,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>362</v>
       </c>
@@ -6922,7 +7254,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>363</v>
       </c>
@@ -6930,7 +7262,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>364</v>
       </c>
@@ -6938,7 +7270,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>365</v>
       </c>
@@ -6946,7 +7278,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>366</v>
       </c>
@@ -6954,7 +7286,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>372</v>
       </c>
@@ -6962,7 +7294,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>373</v>
       </c>
@@ -6970,7 +7302,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>374</v>
       </c>
@@ -6978,7 +7310,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>375</v>
       </c>
@@ -6986,12 +7318,84 @@
         <v>95</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>379</v>
       </c>
       <c r="B100" t="s">
         <v>95</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>381</v>
+      </c>
+      <c r="B101" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>382</v>
+      </c>
+      <c r="B102" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>383</v>
+      </c>
+      <c r="B103" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>384</v>
+      </c>
+      <c r="B104" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>385</v>
+      </c>
+      <c r="B105" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>386</v>
+      </c>
+      <c r="B106" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>387</v>
+      </c>
+      <c r="B107" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>388</v>
+      </c>
+      <c r="B108" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>389</v>
+      </c>
+      <c r="B109" t="s">
+        <v>305</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Make large hydro dispatchable
It was classified as variable for some kind of reason.. Remove MGAM from as a separate sheet
</commit_message>
<xml_diff>
--- a/Inputs/_MasterFiles/FTT_variables.xlsx
+++ b/Inputs/_MasterFiles/FTT_variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/f_j_m_m_nijsse_exeter_ac_uk/Documents/Documents/GitHub/FTT_StandAlone/Inputs/_MasterFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="66" documentId="13_ncr:1_{96C6DCC7-F135-4F9F-BBD1-97530C10B60C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{99DEB3FD-5686-411E-B667-D81B4189779D}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="13_ncr:1_{96C6DCC7-F135-4F9F-BBD1-97530C10B60C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{889BCDAA-4F39-4546-93A5-063B9AFA8152}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FTT-P" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Time_Horizons" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'FTT-P'!$A$1:$G$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'FTT-P'!$A$1:$G$18</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'FTT-Tr'!$A$1:$G$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="274">
   <si>
     <t>Variable name</t>
   </si>
@@ -243,9 +243,6 @@
   </si>
   <si>
     <t>MGAM</t>
-  </si>
-  <si>
-    <t>FTT-Power gamma values</t>
   </si>
   <si>
     <t>MWKA</t>
@@ -1197,10 +1194,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1217,7 +1214,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1235,10 +1232,10 @@
         <v>25</v>
       </c>
       <c r="H1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="I1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1267,7 +1264,7 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1296,7 +1293,7 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1325,7 +1322,7 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1354,12 +1351,12 @@
         <v>24</v>
       </c>
       <c r="I5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1368,10 +1365,10 @@
         <v>31050000</v>
       </c>
       <c r="D6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F6" t="s">
         <v>24</v>
@@ -1383,12 +1380,12 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -1397,7 +1394,7 @@
         <v>31060000</v>
       </c>
       <c r="D7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E7" t="s">
         <v>56</v>
@@ -1412,7 +1409,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1441,12 +1438,12 @@
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1455,7 +1452,7 @@
         <v>31090000</v>
       </c>
       <c r="D9" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E9" t="s">
         <v>56</v>
@@ -1470,12 +1467,12 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1484,7 +1481,7 @@
         <v>31100000</v>
       </c>
       <c r="D10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E10" t="s">
         <v>56</v>
@@ -1499,12 +1496,12 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1513,7 +1510,7 @@
         <v>31110000</v>
       </c>
       <c r="D11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E11" t="s">
         <v>56</v>
@@ -1528,12 +1525,12 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1542,7 +1539,7 @@
         <v>31120000</v>
       </c>
       <c r="D12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E12" t="s">
         <v>56</v>
@@ -1557,12 +1554,12 @@
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -1571,7 +1568,7 @@
         <v>31130000</v>
       </c>
       <c r="D13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E13" t="s">
         <v>56</v>
@@ -1586,12 +1583,12 @@
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -1600,13 +1597,13 @@
         <v>31140000</v>
       </c>
       <c r="D14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E14" t="s">
         <v>56</v>
       </c>
       <c r="F14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -1615,12 +1612,12 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -1629,13 +1626,13 @@
         <v>31150000</v>
       </c>
       <c r="D15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E15" t="s">
         <v>56</v>
       </c>
       <c r="F15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -1644,12 +1641,12 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1658,7 +1655,7 @@
         <v>31180000</v>
       </c>
       <c r="D16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E16" t="s">
         <v>56</v>
@@ -1673,12 +1670,12 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -1687,7 +1684,7 @@
         <v>31190000</v>
       </c>
       <c r="D17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E17" t="s">
         <v>56</v>
@@ -1702,24 +1699,24 @@
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18">
-        <v>31200000</v>
+        <v>31210000</v>
       </c>
       <c r="D18" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="E18" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="F18" t="s">
         <v>24</v>
@@ -1734,38 +1731,9 @@
         <v>265</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>76</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19">
-        <v>31210000</v>
-      </c>
-      <c r="D19" t="s">
-        <v>77</v>
-      </c>
-      <c r="E19" t="s">
-        <v>78</v>
-      </c>
-      <c r="F19" t="s">
-        <v>24</v>
-      </c>
-      <c r="G19" t="s">
-        <v>54</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19" t="s">
-        <v>266</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:G19" xr:uid="{D571B62A-2039-4939-8FED-A328CB35831E}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G20">
+  <autoFilter ref="A1:G18" xr:uid="{D571B62A-2039-4939-8FED-A328CB35831E}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G19">
       <sortCondition ref="C1"/>
     </sortState>
   </autoFilter>
@@ -1794,7 +1762,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1812,10 +1780,10 @@
         <v>25</v>
       </c>
       <c r="H1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="I1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1841,10 +1809,10 @@
         <v>54</v>
       </c>
       <c r="H2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="I2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1873,7 +1841,7 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1902,7 +1870,7 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1931,7 +1899,7 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1960,7 +1928,7 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1989,7 +1957,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -2018,7 +1986,7 @@
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -2047,7 +2015,7 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -2076,7 +2044,7 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -2105,7 +2073,7 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -2134,7 +2102,7 @@
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -2163,7 +2131,7 @@
         <v>24</v>
       </c>
       <c r="I13" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -2192,7 +2160,7 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -2221,7 +2189,7 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -2250,7 +2218,7 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -2279,7 +2247,7 @@
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -2308,7 +2276,7 @@
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -2337,7 +2305,7 @@
         <v>0</v>
       </c>
       <c r="I19" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -2366,7 +2334,7 @@
         <v>0</v>
       </c>
       <c r="I20" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -2395,7 +2363,7 @@
         <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -2424,7 +2392,7 @@
         <v>0</v>
       </c>
       <c r="I22" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -2451,7 +2419,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -2469,15 +2437,15 @@
         <v>25</v>
       </c>
       <c r="H1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="I1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2486,10 +2454,10 @@
         <v>33130000</v>
       </c>
       <c r="D2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E2" t="s">
         <v>97</v>
-      </c>
-      <c r="E2" t="s">
-        <v>98</v>
       </c>
       <c r="F2" t="s">
         <v>40</v>
@@ -2501,12 +2469,12 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -2515,7 +2483,7 @@
         <v>33180000</v>
       </c>
       <c r="D3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E3" t="s">
         <v>40</v>
@@ -2530,12 +2498,12 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -2544,13 +2512,13 @@
         <v>33020000</v>
       </c>
       <c r="D4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -2559,12 +2527,12 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2573,13 +2541,13 @@
         <v>33030000</v>
       </c>
       <c r="D5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -2588,12 +2556,12 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -2602,10 +2570,10 @@
         <v>33050000</v>
       </c>
       <c r="D6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -2617,12 +2585,12 @@
         <v>24</v>
       </c>
       <c r="I6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -2631,10 +2599,10 @@
         <v>33120000</v>
       </c>
       <c r="D7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F7" t="s">
         <v>24</v>
@@ -2646,12 +2614,12 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -2660,7 +2628,7 @@
         <v>33140000</v>
       </c>
       <c r="D8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E8" t="s">
         <v>40</v>
@@ -2675,12 +2643,12 @@
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -2689,10 +2657,10 @@
         <v>33040000</v>
       </c>
       <c r="D9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F9" t="s">
         <v>24</v>
@@ -2704,12 +2672,12 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -2718,7 +2686,7 @@
         <v>33170000</v>
       </c>
       <c r="D10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E10" t="s">
         <v>54</v>
@@ -2733,12 +2701,12 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -2747,10 +2715,10 @@
         <v>33060000</v>
       </c>
       <c r="D11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F11" t="s">
         <v>24</v>
@@ -2762,12 +2730,12 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -2776,10 +2744,10 @@
         <v>33070000</v>
       </c>
       <c r="D12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F12" t="s">
         <v>24</v>
@@ -2791,12 +2759,12 @@
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -2805,10 +2773,10 @@
         <v>33080000</v>
       </c>
       <c r="D13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F13" t="s">
         <v>24</v>
@@ -2820,12 +2788,12 @@
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -2834,10 +2802,10 @@
         <v>33090000</v>
       </c>
       <c r="D14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F14" t="s">
         <v>24</v>
@@ -2849,12 +2817,12 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -2863,10 +2831,10 @@
         <v>33100000</v>
       </c>
       <c r="D15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F15" t="s">
         <v>24</v>
@@ -2878,12 +2846,12 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -2892,10 +2860,10 @@
         <v>33110000</v>
       </c>
       <c r="D16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F16" t="s">
         <v>24</v>
@@ -2907,12 +2875,12 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -2921,22 +2889,22 @@
         <v>33010000</v>
       </c>
       <c r="D17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G17" t="s">
         <v>54</v>
       </c>
       <c r="H17" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="I17" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -2964,7 +2932,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -2982,15 +2950,15 @@
         <v>25</v>
       </c>
       <c r="H1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="I1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2999,7 +2967,7 @@
         <v>34230000</v>
       </c>
       <c r="D2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E2" t="s">
         <v>54</v>
@@ -3014,12 +2982,12 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3028,7 +2996,7 @@
         <v>34290000</v>
       </c>
       <c r="D3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E3" t="s">
         <v>54</v>
@@ -3043,12 +3011,12 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3057,10 +3025,10 @@
         <v>34240000</v>
       </c>
       <c r="D4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F4" t="s">
         <v>24</v>
@@ -3072,12 +3040,12 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3086,13 +3054,13 @@
         <v>34010000</v>
       </c>
       <c r="D5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G5" t="s">
         <v>54</v>
@@ -3101,12 +3069,12 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3115,10 +3083,10 @@
         <v>34050000</v>
       </c>
       <c r="D6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F6" t="s">
         <v>54</v>
@@ -3130,12 +3098,12 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3144,13 +3112,13 @@
         <v>34020000</v>
       </c>
       <c r="D7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -3159,12 +3127,12 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3173,13 +3141,13 @@
         <v>34320000</v>
       </c>
       <c r="D8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -3188,12 +3156,12 @@
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3202,13 +3170,13 @@
         <v>34030000</v>
       </c>
       <c r="D9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -3217,12 +3185,12 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -3231,13 +3199,13 @@
         <v>34040000</v>
       </c>
       <c r="D10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -3246,12 +3214,12 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3260,13 +3228,13 @@
         <v>34110000</v>
       </c>
       <c r="D11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E11" t="s">
         <v>54</v>
       </c>
       <c r="F11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -3275,12 +3243,12 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -3289,13 +3257,13 @@
         <v>34120000</v>
       </c>
       <c r="D12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E12" t="s">
         <v>54</v>
       </c>
       <c r="F12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -3304,12 +3272,12 @@
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -3318,13 +3286,13 @@
         <v>34130000</v>
       </c>
       <c r="D13" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E13" t="s">
         <v>54</v>
       </c>
       <c r="F13" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G13">
         <v>0</v>
@@ -3333,12 +3301,12 @@
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -3347,13 +3315,13 @@
         <v>34140000</v>
       </c>
       <c r="D14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E14" t="s">
         <v>54</v>
       </c>
       <c r="F14" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -3362,12 +3330,12 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -3376,13 +3344,13 @@
         <v>34070000</v>
       </c>
       <c r="D15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -3391,12 +3359,12 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -3405,13 +3373,13 @@
         <v>34080000</v>
       </c>
       <c r="D16" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E16" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G16">
         <v>0</v>
@@ -3420,12 +3388,12 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -3434,10 +3402,10 @@
         <v>34100000</v>
       </c>
       <c r="D17" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -3449,12 +3417,12 @@
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -3463,10 +3431,10 @@
         <v>34090000</v>
       </c>
       <c r="D18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E18" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -3478,12 +3446,12 @@
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -3492,10 +3460,10 @@
         <v>34160000</v>
       </c>
       <c r="D19" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E19" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F19" t="s">
         <v>24</v>
@@ -3507,12 +3475,12 @@
         <v>0</v>
       </c>
       <c r="I19" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -3521,10 +3489,10 @@
         <v>34170000</v>
       </c>
       <c r="D20" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E20" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F20" t="s">
         <v>24</v>
@@ -3536,12 +3504,12 @@
         <v>0</v>
       </c>
       <c r="I20" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -3550,10 +3518,10 @@
         <v>34180000</v>
       </c>
       <c r="D21" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E21" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F21" t="s">
         <v>24</v>
@@ -3565,12 +3533,12 @@
         <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -3579,10 +3547,10 @@
         <v>34190000</v>
       </c>
       <c r="D22" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F22" t="s">
         <v>24</v>
@@ -3594,12 +3562,12 @@
         <v>0</v>
       </c>
       <c r="I22" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -3608,10 +3576,10 @@
         <v>34220000</v>
       </c>
       <c r="D23" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E23" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F23" t="s">
         <v>24</v>
@@ -3623,12 +3591,12 @@
         <v>0</v>
       </c>
       <c r="I23" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -3637,10 +3605,10 @@
         <v>34200000</v>
       </c>
       <c r="D24" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E24" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F24" t="s">
         <v>24</v>
@@ -3652,12 +3620,12 @@
         <v>0</v>
       </c>
       <c r="I24" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -3666,11 +3634,11 @@
         <v>34210000</v>
       </c>
       <c r="D25" t="s">
+        <v>178</v>
+      </c>
+      <c r="E25" t="s">
         <v>179</v>
       </c>
-      <c r="E25" t="s">
-        <v>180</v>
-      </c>
       <c r="F25" t="s">
         <v>24</v>
       </c>
@@ -3681,7 +3649,7 @@
         <v>0</v>
       </c>
       <c r="I25" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -3693,7 +3661,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85BB7FF7-82D6-482E-815B-F3751454FF7D}">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -3712,7 +3680,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -3730,21 +3698,21 @@
         <v>25</v>
       </c>
       <c r="H1" t="s">
+        <v>186</v>
+      </c>
+      <c r="I1" t="s">
         <v>187</v>
       </c>
-      <c r="I1" t="s">
-        <v>188</v>
-      </c>
       <c r="J1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="K1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3753,10 +3721,10 @@
         <v>35320000</v>
       </c>
       <c r="D2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F2" t="s">
         <v>24</v>
@@ -3765,7 +3733,7 @@
         <v>54</v>
       </c>
       <c r="H2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I2" t="s">
         <v>36</v>
@@ -3774,12 +3742,12 @@
         <v>0</v>
       </c>
       <c r="K2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3788,10 +3756,10 @@
         <v>35060000</v>
       </c>
       <c r="D3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F3" t="s">
         <v>24</v>
@@ -3800,7 +3768,7 @@
         <v>54</v>
       </c>
       <c r="H3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I3" t="s">
         <v>14</v>
@@ -3809,12 +3777,12 @@
         <v>0</v>
       </c>
       <c r="K3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3823,33 +3791,33 @@
         <v>35140000</v>
       </c>
       <c r="D4" t="s">
+        <v>208</v>
+      </c>
+      <c r="E4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
         <v>209</v>
       </c>
-      <c r="E4" t="s">
-        <v>54</v>
-      </c>
-      <c r="F4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4" t="s">
-        <v>210</v>
-      </c>
       <c r="I4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J4">
         <v>0</v>
       </c>
       <c r="K4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3858,10 +3826,10 @@
         <v>35040000</v>
       </c>
       <c r="D5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F5" t="s">
         <v>24</v>
@@ -3870,21 +3838,21 @@
         <v>54</v>
       </c>
       <c r="H5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J5">
         <v>0</v>
       </c>
       <c r="K5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3893,33 +3861,33 @@
         <v>35050000</v>
       </c>
       <c r="D6" t="s">
+        <v>200</v>
+      </c>
+      <c r="E6" t="s">
+        <v>190</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H6" t="s">
+        <v>198</v>
+      </c>
+      <c r="I6" t="s">
         <v>201</v>
       </c>
-      <c r="E6" t="s">
-        <v>191</v>
-      </c>
-      <c r="F6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G6" t="s">
-        <v>54</v>
-      </c>
-      <c r="H6" t="s">
-        <v>199</v>
-      </c>
-      <c r="I6" t="s">
-        <v>202</v>
-      </c>
       <c r="J6">
         <v>0</v>
       </c>
       <c r="K6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3928,10 +3896,10 @@
         <v>35020000</v>
       </c>
       <c r="D7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F7" t="s">
         <v>24</v>
@@ -3940,21 +3908,21 @@
         <v>54</v>
       </c>
       <c r="H7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J7">
         <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3963,10 +3931,10 @@
         <v>35030000</v>
       </c>
       <c r="D8" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F8" t="s">
         <v>24</v>
@@ -3975,21 +3943,21 @@
         <v>54</v>
       </c>
       <c r="H8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J8">
         <v>0</v>
       </c>
       <c r="K8" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3998,33 +3966,33 @@
         <v>35150000</v>
       </c>
       <c r="D9" t="s">
+        <v>206</v>
+      </c>
+      <c r="E9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9" t="s">
         <v>207</v>
       </c>
-      <c r="E9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9" t="s">
-        <v>208</v>
-      </c>
       <c r="I9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J9">
         <v>0</v>
       </c>
       <c r="K9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -4033,7 +4001,7 @@
         <v>35130000</v>
       </c>
       <c r="D10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E10" t="s">
         <v>54</v>
@@ -4048,18 +4016,18 @@
         <v>26</v>
       </c>
       <c r="I10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J10">
         <v>0</v>
       </c>
       <c r="K10" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -4068,33 +4036,33 @@
         <v>35160000</v>
       </c>
       <c r="D11" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
       <c r="H11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J11">
         <v>0</v>
       </c>
       <c r="K11" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -4103,33 +4071,33 @@
         <v>35170000</v>
       </c>
       <c r="D12" t="s">
+        <v>222</v>
+      </c>
+      <c r="E12" t="s">
+        <v>190</v>
+      </c>
+      <c r="F12" t="s">
+        <v>190</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12" t="s">
+        <v>225</v>
+      </c>
+      <c r="I12" t="s">
         <v>223</v>
       </c>
-      <c r="E12" t="s">
-        <v>191</v>
-      </c>
-      <c r="F12" t="s">
-        <v>191</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12" t="s">
-        <v>226</v>
-      </c>
-      <c r="I12" t="s">
-        <v>224</v>
-      </c>
       <c r="J12">
         <v>0</v>
       </c>
       <c r="K12" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -4138,33 +4106,33 @@
         <v>35190000</v>
       </c>
       <c r="D13" t="s">
+        <v>232</v>
+      </c>
+      <c r="E13" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13" t="s">
         <v>233</v>
       </c>
-      <c r="E13" t="s">
-        <v>54</v>
-      </c>
-      <c r="F13" t="s">
-        <v>24</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>234</v>
       </c>
-      <c r="I13" t="s">
-        <v>235</v>
-      </c>
       <c r="J13">
         <v>0</v>
       </c>
       <c r="K13" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -4173,7 +4141,7 @@
         <v>35370000</v>
       </c>
       <c r="D14" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E14" t="s">
         <v>54</v>
@@ -4185,21 +4153,21 @@
         <v>0</v>
       </c>
       <c r="H14" t="s">
+        <v>236</v>
+      </c>
+      <c r="I14" t="s">
         <v>237</v>
       </c>
-      <c r="I14" t="s">
-        <v>238</v>
-      </c>
       <c r="J14">
         <v>0</v>
       </c>
       <c r="K14" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -4208,33 +4176,33 @@
         <v>35380000</v>
       </c>
       <c r="D15" t="s">
+        <v>241</v>
+      </c>
+      <c r="E15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15" t="s">
         <v>242</v>
       </c>
-      <c r="E15" t="s">
-        <v>54</v>
-      </c>
-      <c r="F15" t="s">
-        <v>24</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>243</v>
       </c>
-      <c r="I15" t="s">
-        <v>244</v>
-      </c>
       <c r="J15">
         <v>0</v>
       </c>
       <c r="K15" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -4243,10 +4211,10 @@
         <v>35230000</v>
       </c>
       <c r="D16" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E16" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F16" t="s">
         <v>40</v>
@@ -4258,18 +4226,18 @@
         <v>35</v>
       </c>
       <c r="I16" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J16">
         <v>0</v>
       </c>
       <c r="K16" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -4278,33 +4246,33 @@
         <v>35390000</v>
       </c>
       <c r="D17" t="s">
+        <v>247</v>
+      </c>
+      <c r="E17" t="s">
+        <v>190</v>
+      </c>
+      <c r="F17" t="s">
+        <v>250</v>
+      </c>
+      <c r="G17" t="s">
+        <v>54</v>
+      </c>
+      <c r="H17" t="s">
         <v>248</v>
       </c>
-      <c r="E17" t="s">
-        <v>191</v>
-      </c>
-      <c r="F17" t="s">
-        <v>251</v>
-      </c>
-      <c r="G17" t="s">
-        <v>54</v>
-      </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
         <v>249</v>
       </c>
-      <c r="I17" t="s">
-        <v>250</v>
-      </c>
       <c r="J17" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K17" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -4313,7 +4281,7 @@
         <v>35410000</v>
       </c>
       <c r="D18" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E18" t="s">
         <v>54</v>
@@ -4325,21 +4293,21 @@
         <v>0</v>
       </c>
       <c r="H18" t="s">
+        <v>254</v>
+      </c>
+      <c r="I18" t="s">
         <v>255</v>
       </c>
-      <c r="I18" t="s">
-        <v>256</v>
-      </c>
       <c r="J18" t="s">
         <v>24</v>
       </c>
       <c r="K18" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -4348,10 +4316,10 @@
         <v>35420000</v>
       </c>
       <c r="D19" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E19" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -4363,7 +4331,7 @@
         <v>24</v>
       </c>
       <c r="K19" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -4386,7 +4354,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -4394,7 +4362,7 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -4402,7 +4370,7 @@
         <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -4410,7 +4378,7 @@
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -4418,7 +4386,7 @@
         <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -4426,7 +4394,7 @@
         <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -4434,7 +4402,7 @@
         <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -4442,7 +4410,7 @@
         <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -4450,7 +4418,7 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -4458,7 +4426,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -4466,7 +4434,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -4474,7 +4442,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -4482,7 +4450,7 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -4490,7 +4458,7 @@
         <v>58</v>
       </c>
       <c r="B14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -4498,7 +4466,7 @@
         <v>62</v>
       </c>
       <c r="B15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -4506,47 +4474,47 @@
         <v>63</v>
       </c>
       <c r="B16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -4554,303 +4522,303 @@
         <v>66</v>
       </c>
       <c r="B22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B32" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B34" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B35" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B36" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B37" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B38" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B39" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B40" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B41" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B42" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B43" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B44" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B45" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B47" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B48" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B49" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B50" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B51" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B52" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B53" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B54" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B55" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B56" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B57" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B58" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B59" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -4858,55 +4826,55 @@
         <v>31</v>
       </c>
       <c r="B60" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>258</v>
+      </c>
+      <c r="B61" t="s">
         <v>259</v>
-      </c>
-      <c r="B61" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B62" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B63" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B64" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B65" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B66" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Clean and update master file and Variables excel
</commit_message>
<xml_diff>
--- a/Inputs/_MasterFiles/FTT_variables.xlsx
+++ b/Inputs/_MasterFiles/FTT_variables.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cambridgeeconometrics-my.sharepoint.com/personal/bb_camecon_com/Documents/Documents/GitHub/FTT_StandAlone/Inputs/_MasterFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\E3ME\EEIST2_FTT-H2_dev\In\FTTAssumptions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="171" documentId="13_ncr:1_{AFC2604D-5623-4395-A28B-4C6AB9ECB063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{325B89AB-3974-4A7B-86D8-DD71DD53CA61}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62A0F244-D621-4931-9BF9-28DFD2CA0B35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-45" yWindow="-16200" windowWidth="14610" windowHeight="15585" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="8745" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FTT-P" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1142" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1165" uniqueCount="410">
   <si>
     <t>Variable name</t>
   </si>
@@ -988,9 +988,6 @@
     <t>FTT:Hydrogen total hydrogen supply by technology (kt H2)</t>
   </si>
   <si>
-    <t>FTT:Hydrogen total hydrogen supply (kt H2)</t>
-  </si>
-  <si>
     <t>FTT:Hydrogen technology to fuel matrix</t>
   </si>
   <si>
@@ -1241,6 +1238,42 @@
   </si>
   <si>
     <t>Solar OPEX</t>
+  </si>
+  <si>
+    <t>HYWA</t>
+  </si>
+  <si>
+    <t>Substitution frequency matrix</t>
+  </si>
+  <si>
+    <t>NH3-fert</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>HYWT</t>
+  </si>
+  <si>
+    <t>HYWR</t>
+  </si>
+  <si>
+    <t>HYKA</t>
+  </si>
+  <si>
+    <t>FTT:Hydrogen subsidies on upfront investment</t>
+  </si>
+  <si>
+    <t>FTT:Hydrogen Regulations</t>
+  </si>
+  <si>
+    <t>FTT:Hydrogen Exogenous capacity levels</t>
   </si>
 </sst>
 </file>
@@ -1307,12 +1340,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2832,9 +2866,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{893746F0-70F0-4C21-8E46-9B5DBA6E54BB}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3344,8 +3376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F76D307B-9060-4C33-AF9D-2A846C2CA587}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4089,15 +4121,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85BB7FF7-82D6-482E-815B-F3751454FF7D}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="29" customWidth="1"/>
@@ -5052,7 +5084,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5094,7 +5126,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>3601000</v>
+        <v>36000001</v>
       </c>
       <c r="D2" t="s">
         <v>299</v>
@@ -5117,16 +5149,16 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>319</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>36000002</v>
+      </c>
+      <c r="D3" t="s">
         <v>320</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>3602000</v>
-      </c>
-      <c r="D3" t="s">
-        <v>321</v>
       </c>
       <c r="E3" t="s">
         <v>301</v>
@@ -5152,7 +5184,7 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>3603000</v>
+        <v>36000003</v>
       </c>
       <c r="D4" t="s">
         <v>300</v>
@@ -5181,7 +5213,7 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>3604000</v>
+        <v>36000004</v>
       </c>
       <c r="D5" t="s">
         <v>306</v>
@@ -5209,13 +5241,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05986654-6C49-4A34-BECD-4482E94CE084}">
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="39.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -5247,24 +5281,24 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="5" t="s">
         <v>307</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2">
-        <v>3605000</v>
+        <v>36010000</v>
       </c>
       <c r="D2" t="s">
         <v>312</v>
       </c>
       <c r="E2" t="s">
+        <v>316</v>
+      </c>
+      <c r="F2" t="s">
         <v>317</v>
       </c>
-      <c r="F2" t="s">
-        <v>318</v>
-      </c>
       <c r="G2" t="s">
         <v>54</v>
       </c>
@@ -5276,20 +5310,20 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="5" t="s">
         <v>308</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3">
-        <v>3606000</v>
+        <v>36020000</v>
       </c>
       <c r="D3" t="s">
         <v>313</v>
       </c>
       <c r="E3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F3" t="s">
         <v>24</v>
@@ -5305,23 +5339,23 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>309</v>
+      <c r="A4" s="5" t="s">
+        <v>310</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4">
-        <v>3607000</v>
+        <v>36030000</v>
       </c>
       <c r="D4" t="s">
         <v>314</v>
       </c>
       <c r="E4" t="s">
-        <v>54</v>
+        <v>316</v>
       </c>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -5334,933 +5368,925 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>310</v>
+      <c r="A5" s="5" t="s">
+        <v>311</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5">
-        <v>3608000</v>
+        <v>36040000</v>
       </c>
       <c r="D5" t="s">
         <v>315</v>
       </c>
       <c r="E5" t="s">
-        <v>317</v>
-      </c>
-      <c r="F5" t="s">
-        <v>40</v>
+        <v>316</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
-      <c r="H5">
-        <v>0</v>
+      <c r="H5" t="s">
+        <v>24</v>
       </c>
       <c r="I5" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>311</v>
+      <c r="A6" s="5" t="s">
+        <v>321</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6">
-        <v>3609000</v>
+        <v>36050000</v>
       </c>
       <c r="D6" t="s">
+        <v>322</v>
+      </c>
+      <c r="E6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>36060000</v>
+      </c>
+      <c r="D7" t="s">
+        <v>400</v>
+      </c>
+      <c r="E7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>36070000</v>
+      </c>
+      <c r="D8" t="s">
+        <v>339</v>
+      </c>
+      <c r="E8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>36080000</v>
+      </c>
+      <c r="D9" t="s">
+        <v>340</v>
+      </c>
+      <c r="E9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>36090000</v>
+      </c>
+      <c r="D10" t="s">
+        <v>341</v>
+      </c>
+      <c r="E10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>36100000</v>
+      </c>
+      <c r="D11" t="s">
+        <v>342</v>
+      </c>
+      <c r="E11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>36110000</v>
+      </c>
+      <c r="D12" t="s">
+        <v>343</v>
+      </c>
+      <c r="E12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>36120000</v>
+      </c>
+      <c r="D13" t="s">
+        <v>344</v>
+      </c>
+      <c r="E13" t="s">
         <v>316</v>
       </c>
-      <c r="E6" t="s">
-        <v>317</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I6" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>322</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>3610000</v>
-      </c>
-      <c r="D7" t="s">
-        <v>323</v>
-      </c>
-      <c r="E7" t="s">
-        <v>54</v>
-      </c>
-      <c r="F7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>325</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>3612000</v>
-      </c>
-      <c r="D8" t="s">
-        <v>340</v>
-      </c>
-      <c r="E8" t="s">
-        <v>54</v>
-      </c>
-      <c r="F8" t="s">
-        <v>24</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>326</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>3613000</v>
-      </c>
-      <c r="D9" t="s">
-        <v>341</v>
-      </c>
-      <c r="E9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>327</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>3614000</v>
-      </c>
-      <c r="D10" t="s">
-        <v>342</v>
-      </c>
-      <c r="E10" t="s">
-        <v>54</v>
-      </c>
-      <c r="F10" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>328</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11">
-        <v>3615000</v>
-      </c>
-      <c r="D11" t="s">
-        <v>343</v>
-      </c>
-      <c r="E11" t="s">
-        <v>54</v>
-      </c>
-      <c r="F11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>329</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>3616000</v>
-      </c>
-      <c r="D12" t="s">
-        <v>344</v>
-      </c>
-      <c r="E12" t="s">
-        <v>54</v>
-      </c>
-      <c r="F12" t="s">
-        <v>24</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="F13" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" t="s">
+        <v>54</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>330</v>
       </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13">
-        <v>3617000</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>36130000</v>
+      </c>
+      <c r="D14" t="s">
         <v>345</v>
       </c>
-      <c r="E13" t="s">
-        <v>317</v>
-      </c>
-      <c r="F13" t="s">
-        <v>24</v>
-      </c>
-      <c r="G13" t="s">
-        <v>54</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="E14" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>331</v>
       </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14">
-        <v>3618000</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>36140000</v>
+      </c>
+      <c r="D15" t="s">
         <v>346</v>
       </c>
-      <c r="E14" t="s">
-        <v>54</v>
-      </c>
-      <c r="F14" t="s">
-        <v>24</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="E15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
         <v>332</v>
       </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15">
-        <v>3619000</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>36150000</v>
+      </c>
+      <c r="D16" t="s">
         <v>347</v>
       </c>
-      <c r="E15" t="s">
-        <v>54</v>
-      </c>
-      <c r="F15" t="s">
-        <v>24</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="E16" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" t="s">
+        <v>24</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
         <v>333</v>
       </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16">
-        <v>3620000</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>36160000</v>
+      </c>
+      <c r="D17" t="s">
         <v>348</v>
       </c>
-      <c r="E16" t="s">
-        <v>54</v>
-      </c>
-      <c r="F16" t="s">
-        <v>24</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="E17" t="s">
+        <v>54</v>
+      </c>
+      <c r="F17" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17">
-        <v>3621000</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>36170000</v>
+      </c>
+      <c r="D18" t="s">
         <v>349</v>
       </c>
-      <c r="E17" t="s">
-        <v>54</v>
-      </c>
-      <c r="F17" t="s">
-        <v>24</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="E18" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" t="s">
+        <v>24</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>335</v>
       </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18">
-        <v>3622000</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>36180000</v>
+      </c>
+      <c r="D19" t="s">
         <v>350</v>
       </c>
-      <c r="E18" t="s">
-        <v>54</v>
-      </c>
-      <c r="F18" t="s">
-        <v>24</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="E19" t="s">
+        <v>54</v>
+      </c>
+      <c r="F19" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
         <v>336</v>
       </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19">
-        <v>3623000</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>36190000</v>
+      </c>
+      <c r="D20" t="s">
         <v>351</v>
       </c>
-      <c r="E19" t="s">
-        <v>54</v>
-      </c>
-      <c r="F19" t="s">
-        <v>24</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="E20" t="s">
+        <v>54</v>
+      </c>
+      <c r="F20" t="s">
+        <v>54</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>398</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>36200000</v>
+      </c>
+      <c r="D21" t="s">
+        <v>399</v>
+      </c>
+      <c r="E21" t="s">
+        <v>316</v>
+      </c>
+      <c r="F21" t="s">
+        <v>316</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
         <v>337</v>
       </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20">
-        <v>3624000</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>36210000</v>
+      </c>
+      <c r="D22" t="s">
         <v>352</v>
       </c>
-      <c r="E20" t="s">
-        <v>54</v>
-      </c>
-      <c r="F20" t="s">
-        <v>54</v>
-      </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="E22" t="s">
+        <v>316</v>
+      </c>
+      <c r="F22" t="s">
+        <v>316</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
         <v>338</v>
       </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21">
-        <v>3625000</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>36220000</v>
+      </c>
+      <c r="D23" t="s">
         <v>353</v>
       </c>
-      <c r="E21" t="s">
-        <v>317</v>
-      </c>
-      <c r="F21" t="s">
-        <v>317</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>339</v>
-      </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="C22">
-        <v>3626000</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="E23" t="s">
+        <v>316</v>
+      </c>
+      <c r="F23" t="s">
+        <v>24</v>
+      </c>
+      <c r="G23" t="s">
+        <v>54</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
         <v>354</v>
       </c>
-      <c r="E22" t="s">
-        <v>317</v>
-      </c>
-      <c r="F22" t="s">
-        <v>24</v>
-      </c>
-      <c r="G22" t="s">
-        <v>54</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-      <c r="I22" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>36230000</v>
+      </c>
+      <c r="D24" t="s">
+        <v>357</v>
+      </c>
+      <c r="E24" t="s">
+        <v>316</v>
+      </c>
+      <c r="F24" t="s">
+        <v>24</v>
+      </c>
+      <c r="G24" t="s">
+        <v>54</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
         <v>355</v>
       </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="C23">
-        <f>C22+1000</f>
-        <v>3627000</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>36240000</v>
+      </c>
+      <c r="D25" t="s">
         <v>358</v>
       </c>
-      <c r="E23" t="s">
-        <v>317</v>
-      </c>
-      <c r="F23" t="s">
-        <v>24</v>
-      </c>
-      <c r="G23" t="s">
-        <v>54</v>
-      </c>
-      <c r="H23">
-        <v>0</v>
-      </c>
-      <c r="I23" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="E25" t="s">
+        <v>54</v>
+      </c>
+      <c r="F25" t="s">
+        <v>24</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
         <v>356</v>
       </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="C24">
-        <f t="shared" ref="C24:C30" si="0">C23+1000</f>
-        <v>3628000</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>36250000</v>
+      </c>
+      <c r="D26" t="s">
         <v>359</v>
       </c>
-      <c r="E24" t="s">
-        <v>54</v>
-      </c>
-      <c r="F24" t="s">
-        <v>24</v>
-      </c>
-      <c r="G24">
-        <v>0</v>
-      </c>
-      <c r="H24">
-        <v>0</v>
-      </c>
-      <c r="I24" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>357</v>
-      </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="C25">
-        <f t="shared" si="0"/>
-        <v>3629000</v>
-      </c>
-      <c r="D25" t="s">
-        <v>360</v>
-      </c>
-      <c r="E25" t="s">
-        <v>54</v>
-      </c>
-      <c r="F25" t="s">
-        <v>24</v>
-      </c>
-      <c r="G25">
-        <v>0</v>
-      </c>
-      <c r="H25">
-        <v>0</v>
-      </c>
-      <c r="I25" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="E26" t="s">
+        <v>54</v>
+      </c>
+      <c r="F26" t="s">
+        <v>24</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>36260000</v>
+      </c>
+      <c r="D27" t="s">
+        <v>366</v>
+      </c>
+      <c r="E27" t="s">
+        <v>54</v>
+      </c>
+      <c r="F27" t="s">
+        <v>24</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
         <v>362</v>
       </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26">
-        <f t="shared" si="0"/>
-        <v>3630000</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>36270000</v>
+      </c>
+      <c r="D28" t="s">
         <v>367</v>
       </c>
-      <c r="E26" t="s">
-        <v>54</v>
-      </c>
-      <c r="F26" t="s">
-        <v>24</v>
-      </c>
-      <c r="G26">
-        <v>0</v>
-      </c>
-      <c r="H26">
-        <v>0</v>
-      </c>
-      <c r="I26" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="E28" t="s">
+        <v>54</v>
+      </c>
+      <c r="F28" t="s">
+        <v>24</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
         <v>363</v>
       </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="C27">
-        <f t="shared" si="0"/>
-        <v>3631000</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>36280000</v>
+      </c>
+      <c r="D29" t="s">
         <v>368</v>
       </c>
-      <c r="E27" t="s">
-        <v>54</v>
-      </c>
-      <c r="F27" t="s">
-        <v>24</v>
-      </c>
-      <c r="G27">
-        <v>0</v>
-      </c>
-      <c r="H27">
-        <v>0</v>
-      </c>
-      <c r="I27" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="E29" t="s">
+        <v>54</v>
+      </c>
+      <c r="F29" t="s">
+        <v>24</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
         <v>364</v>
       </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28">
-        <f t="shared" si="0"/>
-        <v>3632000</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>36290000</v>
+      </c>
+      <c r="D30" t="s">
         <v>369</v>
       </c>
-      <c r="E28" t="s">
-        <v>54</v>
-      </c>
-      <c r="F28" t="s">
-        <v>24</v>
-      </c>
-      <c r="G28">
-        <v>0</v>
-      </c>
-      <c r="H28">
-        <v>0</v>
-      </c>
-      <c r="I28" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="E30" t="s">
+        <v>54</v>
+      </c>
+      <c r="F30" t="s">
+        <v>24</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
         <v>365</v>
       </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-      <c r="C29">
-        <f t="shared" si="0"/>
-        <v>3633000</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>36300000</v>
+      </c>
+      <c r="D31" t="s">
         <v>370</v>
       </c>
-      <c r="E29" t="s">
-        <v>54</v>
-      </c>
-      <c r="F29" t="s">
-        <v>24</v>
-      </c>
-      <c r="G29">
-        <v>0</v>
-      </c>
-      <c r="H29">
-        <v>0</v>
-      </c>
-      <c r="I29" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>366</v>
-      </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="C30">
-        <f t="shared" si="0"/>
-        <v>3634000</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="E31" t="s">
+        <v>54</v>
+      </c>
+      <c r="F31" t="s">
+        <v>24</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
         <v>371</v>
       </c>
-      <c r="E30" t="s">
-        <v>54</v>
-      </c>
-      <c r="F30" t="s">
-        <v>24</v>
-      </c>
-      <c r="G30">
-        <v>0</v>
-      </c>
-      <c r="H30">
-        <v>0</v>
-      </c>
-      <c r="I30" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>36310000</v>
+      </c>
+      <c r="D32" t="s">
+        <v>315</v>
+      </c>
+      <c r="E32" t="s">
+        <v>316</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32" t="s">
+        <v>24</v>
+      </c>
+      <c r="I32" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
         <v>372</v>
       </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="C31">
-        <v>3609000</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>36320000</v>
+      </c>
+      <c r="D33" t="s">
+        <v>375</v>
+      </c>
+      <c r="E33" t="s">
+        <v>54</v>
+      </c>
+      <c r="F33" t="s">
+        <v>24</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>36330000</v>
+      </c>
+      <c r="D34" t="s">
+        <v>376</v>
+      </c>
+      <c r="E34" t="s">
+        <v>54</v>
+      </c>
+      <c r="F34" t="s">
+        <v>24</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>374</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>36340000</v>
+      </c>
+      <c r="D35" t="s">
+        <v>377</v>
+      </c>
+      <c r="E35" t="s">
+        <v>54</v>
+      </c>
+      <c r="F35" t="s">
+        <v>24</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>36350000</v>
+      </c>
+      <c r="D36" t="s">
+        <v>379</v>
+      </c>
+      <c r="E36" t="s">
         <v>316</v>
       </c>
-      <c r="E31" t="s">
-        <v>317</v>
-      </c>
-      <c r="F31">
-        <v>0</v>
-      </c>
-      <c r="G31">
-        <v>0</v>
-      </c>
-      <c r="H31" t="s">
-        <v>24</v>
-      </c>
-      <c r="I31" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>373</v>
-      </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="C32">
-        <v>36350000</v>
-      </c>
-      <c r="D32" t="s">
-        <v>376</v>
-      </c>
-      <c r="E32" t="s">
-        <v>54</v>
-      </c>
-      <c r="F32" t="s">
-        <v>24</v>
-      </c>
-      <c r="G32">
-        <v>0</v>
-      </c>
-      <c r="H32">
-        <v>0</v>
-      </c>
-      <c r="I32" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>374</v>
-      </c>
-      <c r="B33">
-        <v>1</v>
-      </c>
-      <c r="C33">
-        <v>36360000</v>
-      </c>
-      <c r="D33" t="s">
-        <v>377</v>
-      </c>
-      <c r="E33" t="s">
-        <v>54</v>
-      </c>
-      <c r="F33" t="s">
-        <v>24</v>
-      </c>
-      <c r="G33">
-        <v>0</v>
-      </c>
-      <c r="H33">
-        <v>0</v>
-      </c>
-      <c r="I33" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>375</v>
-      </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-      <c r="C34">
-        <v>36370000</v>
-      </c>
-      <c r="D34" t="s">
-        <v>378</v>
-      </c>
-      <c r="E34" t="s">
-        <v>54</v>
-      </c>
-      <c r="F34" t="s">
-        <v>24</v>
-      </c>
-      <c r="G34">
-        <v>0</v>
-      </c>
-      <c r="H34">
-        <v>0</v>
-      </c>
-      <c r="I34" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>379</v>
-      </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-      <c r="C35">
-        <v>36380000</v>
-      </c>
-      <c r="D35" t="s">
-        <v>380</v>
-      </c>
-      <c r="E35" t="s">
-        <v>317</v>
-      </c>
-      <c r="F35" t="s">
-        <v>24</v>
-      </c>
-      <c r="G35" t="s">
-        <v>54</v>
-      </c>
-      <c r="H35">
-        <v>0</v>
-      </c>
-      <c r="I35" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>381</v>
-      </c>
-      <c r="B36">
-        <v>1</v>
-      </c>
-      <c r="C36">
-        <v>36390000</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>393</v>
-      </c>
-      <c r="E36" t="s">
-        <v>54</v>
-      </c>
       <c r="F36" t="s">
         <v>24</v>
       </c>
-      <c r="G36">
-        <v>0</v>
+      <c r="G36" t="s">
+        <v>54</v>
       </c>
       <c r="H36">
         <v>0</v>
@@ -6271,16 +6297,16 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B37">
         <v>1</v>
       </c>
       <c r="C37">
-        <v>36400000</v>
+        <v>36360000</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="E37" t="s">
         <v>54</v>
@@ -6300,16 +6326,16 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B38">
         <v>1</v>
       </c>
       <c r="C38">
-        <v>36410000</v>
+        <v>36370000</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="E38" t="s">
         <v>54</v>
@@ -6329,16 +6355,16 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B39">
         <v>1</v>
       </c>
       <c r="C39">
-        <v>36420000</v>
+        <v>36380000</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="E39" t="s">
         <v>54</v>
@@ -6358,16 +6384,16 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B40">
         <v>1</v>
       </c>
       <c r="C40">
-        <v>36430000</v>
+        <v>36390000</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="E40" t="s">
         <v>54</v>
@@ -6387,16 +6413,16 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B41">
         <v>1</v>
       </c>
       <c r="C41">
-        <v>36440000</v>
+        <v>36400000</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="E41" t="s">
         <v>54</v>
@@ -6416,16 +6442,16 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B42">
         <v>1</v>
       </c>
       <c r="C42">
-        <v>36450000</v>
+        <v>36410000</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>392</v>
+        <v>397</v>
       </c>
       <c r="E42" t="s">
         <v>54</v>
@@ -6445,13 +6471,13 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B43">
         <v>1</v>
       </c>
       <c r="C43">
-        <v>36460000</v>
+        <v>36420000</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>391</v>
@@ -6474,13 +6500,13 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B44">
         <v>1</v>
       </c>
       <c r="C44">
-        <v>36470000</v>
+        <v>36430000</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>390</v>
@@ -6502,13 +6528,120 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="4"/>
+      <c r="A45" s="4" t="s">
+        <v>388</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45">
+        <v>36440000</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>389</v>
+      </c>
+      <c r="E45" t="s">
+        <v>54</v>
+      </c>
+      <c r="F45" t="s">
+        <v>24</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="4"/>
+      <c r="A46" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <v>36450000</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="E46" t="s">
+        <v>316</v>
+      </c>
+      <c r="F46" t="s">
+        <v>24</v>
+      </c>
+      <c r="G46" t="s">
+        <v>54</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46" t="s">
+        <v>401</v>
+      </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="4"/>
+      <c r="A47" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+      <c r="C47">
+        <v>36460000</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="E47" t="s">
+        <v>316</v>
+      </c>
+      <c r="F47" t="s">
+        <v>24</v>
+      </c>
+      <c r="G47" t="s">
+        <v>54</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+      <c r="C48">
+        <v>36470000</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="E48" t="s">
+        <v>316</v>
+      </c>
+      <c r="F48" t="s">
+        <v>24</v>
+      </c>
+      <c r="G48" t="s">
+        <v>54</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48" t="s">
+        <v>403</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -7064,10 +7197,10 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B68" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -7091,15 +7224,15 @@
         <v>311</v>
       </c>
       <c r="B71" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B72" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -7112,7 +7245,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B74" t="s">
         <v>95</v>
@@ -7120,7 +7253,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B75" t="s">
         <v>95</v>
@@ -7128,7 +7261,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B76" t="s">
         <v>95</v>
@@ -7136,7 +7269,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B77" t="s">
         <v>95</v>
@@ -7144,7 +7277,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B78" t="s">
         <v>95</v>
@@ -7152,7 +7285,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B79" t="s">
         <v>95</v>
@@ -7160,7 +7293,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B80" t="s">
         <v>95</v>
@@ -7168,7 +7301,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B81" t="s">
         <v>95</v>
@@ -7176,7 +7309,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B82" t="s">
         <v>95</v>
@@ -7184,7 +7317,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B83" t="s">
         <v>95</v>
@@ -7192,7 +7325,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B84" t="s">
         <v>95</v>
@@ -7200,7 +7333,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B85" t="s">
         <v>95</v>
@@ -7208,7 +7341,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B86" t="s">
         <v>95</v>
@@ -7216,7 +7349,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B87" t="s">
         <v>95</v>
@@ -7224,7 +7357,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B88" t="s">
         <v>95</v>
@@ -7232,7 +7365,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B89" t="s">
         <v>95</v>
@@ -7240,7 +7373,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B90" t="s">
         <v>95</v>
@@ -7248,7 +7381,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B91" t="s">
         <v>95</v>
@@ -7256,7 +7389,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B92" t="s">
         <v>95</v>
@@ -7264,7 +7397,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B93" t="s">
         <v>95</v>
@@ -7272,7 +7405,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B94" t="s">
         <v>95</v>
@@ -7280,7 +7413,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B95" t="s">
         <v>95</v>
@@ -7288,15 +7421,15 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B96" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B97" t="s">
         <v>95</v>
@@ -7304,7 +7437,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B98" t="s">
         <v>95</v>
@@ -7312,7 +7445,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B99" t="s">
         <v>95</v>
@@ -7320,7 +7453,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B100" t="s">
         <v>95</v>
@@ -7328,7 +7461,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B101" t="s">
         <v>305</v>
@@ -7336,7 +7469,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B102" t="s">
         <v>305</v>
@@ -7344,7 +7477,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B103" t="s">
         <v>305</v>
@@ -7352,7 +7485,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B104" t="s">
         <v>305</v>
@@ -7360,7 +7493,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B105" t="s">
         <v>305</v>
@@ -7368,7 +7501,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B106" t="s">
         <v>305</v>
@@ -7376,7 +7509,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B107" t="s">
         <v>305</v>
@@ -7384,7 +7517,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B108" t="s">
         <v>305</v>
@@ -7392,7 +7525,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B109" t="s">
         <v>305</v>

</xml_diff>

<commit_message>
Put base registration rate as separate sheet
</commit_message>
<xml_diff>
--- a/Inputs/_MasterFiles/FTT_variables.xlsx
+++ b/Inputs/_MasterFiles/FTT_variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/f_j_m_m_nijsse_exeter_ac_uk/Documents/Documents/GitHub/FTT_StandAlone/Inputs/_MasterFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="67" documentId="13_ncr:1_{96C6DCC7-F135-4F9F-BBD1-97530C10B60C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{889BCDAA-4F39-4546-93A5-063B9AFA8152}"/>
+  <xr:revisionPtr revIDLastSave="76" documentId="13_ncr:1_{96C6DCC7-F135-4F9F-BBD1-97530C10B60C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE8E03F7-4FBD-495E-92BD-7DCE410BAAB3}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FTT-P" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="276">
   <si>
     <t>Variable name</t>
   </si>
@@ -864,6 +864,12 @@
   </si>
   <si>
     <t>BZTC</t>
+  </si>
+  <si>
+    <t>Base registration rate</t>
+  </si>
+  <si>
+    <t>FTT-Tr relative registration tax or subsidy</t>
   </si>
 </sst>
 </file>
@@ -1196,7 +1202,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -1744,17 +1750,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E04294AC-DBC1-4E51-84ED-2EC5066B9024}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.5703125" customWidth="1"/>
+    <col min="4" max="4" width="46.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -1962,25 +1968,25 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>274</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8">
-        <v>32130000</v>
+        <v>-99</v>
       </c>
       <c r="D8" t="s">
-        <v>46</v>
+        <v>275</v>
       </c>
       <c r="E8" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="F8" t="s">
         <v>24</v>
       </c>
-      <c r="G8">
-        <v>0</v>
+      <c r="G8" t="s">
+        <v>54</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -1991,16 +1997,16 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9">
-        <v>32140000</v>
+        <v>32130000</v>
       </c>
       <c r="D9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E9" t="s">
         <v>54</v>
@@ -2020,16 +2026,16 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10">
-        <v>32150000</v>
+        <v>32140000</v>
       </c>
       <c r="D10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E10" t="s">
         <v>54</v>
@@ -2049,22 +2055,22 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11">
-        <v>32160000</v>
+        <v>32150000</v>
       </c>
       <c r="D11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E11" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="F11" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -2073,21 +2079,21 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12">
-        <v>32170000</v>
+        <v>32160000</v>
       </c>
       <c r="D12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E12" t="s">
         <v>22</v>
@@ -2107,28 +2113,28 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13">
-        <v>32180000</v>
+        <v>32170000</v>
       </c>
       <c r="D13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E13" t="s">
         <v>22</v>
       </c>
-      <c r="F13">
-        <v>0</v>
+      <c r="F13" t="s">
+        <v>22</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
-      <c r="H13" t="s">
-        <v>24</v>
+      <c r="H13">
+        <v>0</v>
       </c>
       <c r="I13" t="s">
         <v>264</v>
@@ -2136,28 +2142,28 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14">
-        <v>32190000</v>
+        <v>32180000</v>
       </c>
       <c r="D14" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="E14" t="s">
-        <v>39</v>
-      </c>
-      <c r="F14" t="s">
-        <v>54</v>
+        <v>22</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
       </c>
       <c r="G14">
         <v>0</v>
       </c>
-      <c r="H14">
-        <v>0</v>
+      <c r="H14" t="s">
+        <v>24</v>
       </c>
       <c r="I14" t="s">
         <v>264</v>
@@ -2165,16 +2171,16 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15">
-        <v>32210000</v>
+        <v>32190000</v>
       </c>
       <c r="D15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E15" t="s">
         <v>39</v>
@@ -2194,16 +2200,16 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16">
-        <v>32220000</v>
+        <v>32210000</v>
       </c>
       <c r="D16" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="E16" t="s">
         <v>39</v>
@@ -2223,22 +2229,22 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17">
-        <v>32230000</v>
+        <v>32220000</v>
       </c>
       <c r="D17" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E17" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="F17" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -2252,22 +2258,22 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18">
-        <v>32300000</v>
+        <v>32230000</v>
       </c>
       <c r="D18" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E18" t="s">
-        <v>54</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
+        <v>22</v>
+      </c>
+      <c r="F18" t="s">
+        <v>40</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -2281,16 +2287,16 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19">
-        <v>32310000</v>
+        <v>32300000</v>
       </c>
       <c r="D19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E19" t="s">
         <v>54</v>
@@ -2310,22 +2316,22 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20">
-        <v>32320000</v>
+        <v>32310000</v>
       </c>
       <c r="D20" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E20" t="s">
         <v>54</v>
       </c>
-      <c r="F20" t="s">
-        <v>24</v>
+      <c r="F20">
+        <v>0</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -2339,16 +2345,16 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21">
-        <v>32330000</v>
+        <v>32320000</v>
       </c>
       <c r="D21" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="E21" t="s">
         <v>54</v>
@@ -2368,30 +2374,59 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>32330000</v>
+      </c>
+      <c r="D22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" t="s">
+        <v>54</v>
+      </c>
+      <c r="F22" t="s">
+        <v>24</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>52</v>
       </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="C22">
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
         <v>32340000</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D23" t="s">
         <v>53</v>
       </c>
-      <c r="E22" t="s">
-        <v>54</v>
-      </c>
-      <c r="F22" t="s">
-        <v>24</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-      <c r="I22" t="s">
+      <c r="E23" t="s">
+        <v>54</v>
+      </c>
+      <c r="F23" t="s">
+        <v>24</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23" t="s">
         <v>264</v>
       </c>
     </row>
@@ -4341,10 +4376,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA629D80-511C-42AD-ACB3-22237E3BD282}">
-  <dimension ref="A1:B66"/>
+  <dimension ref="A1:B67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4423,7 +4458,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>274</v>
       </c>
       <c r="B10" t="s">
         <v>94</v>
@@ -4431,7 +4466,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
         <v>94</v>
@@ -4439,7 +4474,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>94</v>
@@ -4447,15 +4482,15 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>58</v>
+        <v>3</v>
       </c>
       <c r="B14" t="s">
         <v>93</v>
@@ -4463,15 +4498,15 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B16" t="s">
         <v>94</v>
@@ -4479,7 +4514,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B17" t="s">
         <v>94</v>
@@ -4487,7 +4522,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B18" t="s">
         <v>94</v>
@@ -4495,7 +4530,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B19" t="s">
         <v>94</v>
@@ -4503,7 +4538,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B20" t="s">
         <v>94</v>
@@ -4511,7 +4546,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B21" t="s">
         <v>94</v>
@@ -4519,7 +4554,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B22" t="s">
         <v>94</v>
@@ -4527,23 +4562,23 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B23" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>102</v>
+        <v>75</v>
       </c>
       <c r="B24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B25" t="s">
         <v>94</v>
@@ -4551,23 +4586,23 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B26" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B28" t="s">
         <v>94</v>
@@ -4575,7 +4610,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B29" t="s">
         <v>94</v>
@@ -4583,7 +4618,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B30" t="s">
         <v>94</v>
@@ -4591,7 +4626,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B31" t="s">
         <v>94</v>
@@ -4599,7 +4634,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B32" t="s">
         <v>94</v>
@@ -4607,7 +4642,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B33" t="s">
         <v>94</v>
@@ -4615,7 +4650,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="B34" t="s">
         <v>94</v>
@@ -4623,39 +4658,39 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B35" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>154</v>
+        <v>130</v>
       </c>
       <c r="B36" t="s">
-        <v>184</v>
+        <v>93</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>131</v>
+        <v>154</v>
       </c>
       <c r="B37" t="s">
-        <v>93</v>
+        <v>184</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="B38" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B39" t="s">
         <v>94</v>
@@ -4663,7 +4698,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B40" t="s">
         <v>94</v>
@@ -4671,7 +4706,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B41" t="s">
         <v>94</v>
@@ -4679,7 +4714,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B42" t="s">
         <v>94</v>
@@ -4687,7 +4722,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B43" t="s">
         <v>94</v>
@@ -4695,7 +4730,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B44" t="s">
         <v>94</v>
@@ -4703,23 +4738,23 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>185</v>
+        <v>152</v>
       </c>
       <c r="B45" t="s">
-        <v>251</v>
+        <v>94</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B46" t="s">
-        <v>94</v>
+        <v>251</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>213</v>
+        <v>188</v>
       </c>
       <c r="B47" t="s">
         <v>94</v>
@@ -4727,23 +4762,23 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>192</v>
+        <v>213</v>
       </c>
       <c r="B48" t="s">
-        <v>251</v>
+        <v>94</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>269</v>
+        <v>192</v>
       </c>
       <c r="B49" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>212</v>
+        <v>269</v>
       </c>
       <c r="B50" t="s">
         <v>252</v>
@@ -4751,7 +4786,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B51" t="s">
         <v>252</v>
@@ -4759,7 +4794,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B52" t="s">
         <v>252</v>
@@ -4767,7 +4802,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B53" t="s">
         <v>252</v>
@@ -4775,7 +4810,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B54" t="s">
         <v>252</v>
@@ -4783,7 +4818,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B55" t="s">
         <v>252</v>
@@ -4791,15 +4826,15 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="B56" t="s">
-        <v>93</v>
+        <v>252</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B57" t="s">
         <v>93</v>
@@ -4807,7 +4842,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B58" t="s">
         <v>93</v>
@@ -4815,7 +4850,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="B59" t="s">
         <v>93</v>
@@ -4823,23 +4858,23 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>31</v>
+        <v>244</v>
       </c>
       <c r="B60" t="s">
-        <v>257</v>
+        <v>93</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>258</v>
+        <v>31</v>
       </c>
       <c r="B61" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B62" t="s">
         <v>259</v>
@@ -4847,7 +4882,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="B63" t="s">
         <v>259</v>
@@ -4855,25 +4890,33 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>253</v>
+        <v>267</v>
       </c>
       <c r="B64" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>101</v>
+        <v>253</v>
       </c>
       <c r="B65" t="s">
-        <v>259</v>
+        <v>268</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>101</v>
+      </c>
+      <c r="B66" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>270</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B67" t="s">
         <v>252</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add new base registration rate to masterfiles
Add it to variable listing and FTT variables. Fix error with lifetime bikes in China too
</commit_message>
<xml_diff>
--- a/Inputs/_MasterFiles/FTT_variables.xlsx
+++ b/Inputs/_MasterFiles/FTT_variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rosiehayward/Documents/GitHub/FTT_StandAlone/Inputs/_MasterFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/f_j_m_m_nijsse_exeter_ac_uk/Documents/Documents/GitHub/FTT_StandAlone/Inputs/_MasterFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B21FCB0C-8A9E-F54D-8028-8000D713EF49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{B21FCB0C-8A9E-F54D-8028-8000D713EF49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB92C6E0-57DD-48CF-8B94-DE03344EFAE8}"/>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="1440" windowWidth="22940" windowHeight="12480" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FTT-P" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1494" uniqueCount="520">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1502" uniqueCount="522">
   <si>
     <t>Variable name</t>
   </si>
@@ -1607,6 +1607,12 @@
   </si>
   <si>
     <t xml:space="preserve">FTT-IH-OIS Fuel tax (2010 Euros/MWh) </t>
+  </si>
+  <si>
+    <t>Base registration rate</t>
+  </si>
+  <si>
+    <t>FTT-Tr registration rate as share of purchase price</t>
   </si>
 </sst>
 </file>
@@ -1957,16 +1963,16 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" customWidth="1"/>
-    <col min="7" max="7" width="14.5" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1995,7 +2001,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2024,7 +2030,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>58</v>
       </c>
@@ -2053,7 +2059,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>62</v>
       </c>
@@ -2082,7 +2088,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>63</v>
       </c>
@@ -2111,7 +2117,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>74</v>
       </c>
@@ -2140,7 +2146,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>84</v>
       </c>
@@ -2169,7 +2175,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -2198,7 +2204,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>79</v>
       </c>
@@ -2227,7 +2233,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>70</v>
       </c>
@@ -2256,7 +2262,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>72</v>
       </c>
@@ -2285,7 +2291,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -2314,7 +2320,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>81</v>
       </c>
@@ -2343,7 +2349,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>88</v>
       </c>
@@ -2372,7 +2378,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>90</v>
       </c>
@@ -2401,7 +2407,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>80</v>
       </c>
@@ -2430,7 +2436,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>82</v>
       </c>
@@ -2459,7 +2465,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>66</v>
       </c>
@@ -2488,7 +2494,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>76</v>
       </c>
@@ -2536,17 +2542,17 @@
       <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2581,7 +2587,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>186</v>
       </c>
@@ -2616,7 +2622,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>189</v>
       </c>
@@ -2651,7 +2657,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>220</v>
       </c>
@@ -2686,7 +2692,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>195</v>
       </c>
@@ -2721,7 +2727,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>198</v>
       </c>
@@ -2756,7 +2762,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>219</v>
       </c>
@@ -2791,7 +2797,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>221</v>
       </c>
@@ -2826,7 +2832,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>222</v>
       </c>
@@ -2861,7 +2867,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>223</v>
       </c>
@@ -2896,7 +2902,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>224</v>
       </c>
@@ -2931,7 +2937,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>225</v>
       </c>
@@ -2966,7 +2972,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>215</v>
       </c>
@@ -3001,7 +3007,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>229</v>
       </c>
@@ -3033,7 +3039,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>231</v>
       </c>
@@ -3065,7 +3071,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>238</v>
       </c>
@@ -3100,7 +3106,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>239</v>
       </c>
@@ -3135,7 +3141,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>242</v>
       </c>
@@ -3170,7 +3176,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>248</v>
       </c>
@@ -3205,7 +3211,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>250</v>
       </c>
@@ -3240,7 +3246,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>254</v>
       </c>
@@ -3275,7 +3281,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>258</v>
       </c>
@@ -3310,7 +3316,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>264</v>
       </c>
@@ -3345,7 +3351,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>270</v>
       </c>
@@ -3380,7 +3386,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>266</v>
       </c>
@@ -3415,7 +3421,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>276</v>
       </c>
@@ -3450,7 +3456,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>281</v>
       </c>
@@ -3492,15 +3498,15 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA629D80-511C-42AD-ACB3-22237E3BD282}">
-  <dimension ref="A1:B66"/>
+  <dimension ref="A1:B67"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="M77" sqref="M77"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3508,7 +3514,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -3516,7 +3522,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -3524,7 +3530,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -3532,7 +3538,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -3540,7 +3546,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -3548,7 +3554,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -3556,7 +3562,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -3564,7 +3570,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -3572,459 +3578,467 @@
         <v>95</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>520</v>
       </c>
       <c r="B10" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>3</v>
-      </c>
-      <c r="B13" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>58</v>
       </c>
       <c r="B14" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>62</v>
-      </c>
-      <c r="B15" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>63</v>
       </c>
       <c r="B16" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="B17" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B18" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="B19" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B20" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B21" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B22" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>76</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>103</v>
-      </c>
-      <c r="B24" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>104</v>
       </c>
       <c r="B25" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>104</v>
+      </c>
+      <c r="B26" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>105</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>106</v>
-      </c>
-      <c r="B27" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>107</v>
       </c>
       <c r="B28" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B29" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B30" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B31" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B32" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B33" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="B34" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>130</v>
+      </c>
+      <c r="B35" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>131</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>155</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>132</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>147</v>
-      </c>
-      <c r="B38" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>148</v>
       </c>
       <c r="B39" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B40" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B41" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B42" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B43" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B44" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>153</v>
+      </c>
+      <c r="B45" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>186</v>
-      </c>
-      <c r="B45" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>189</v>
       </c>
       <c r="B46" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>189</v>
+      </c>
+      <c r="B47" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>220</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>195</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>198</v>
-      </c>
-      <c r="B49" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>219</v>
       </c>
       <c r="B50" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B51" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B52" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B53" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B54" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B55" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>225</v>
+      </c>
+      <c r="B56" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>215</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B57" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>248</v>
-      </c>
-      <c r="B57" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>250</v>
       </c>
       <c r="B58" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B59" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="B60" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>270</v>
+      </c>
+      <c r="B61" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>31</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B62" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>286</v>
-      </c>
-      <c r="B62" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>290</v>
       </c>
       <c r="B63" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="B64" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>295</v>
+      </c>
+      <c r="B65" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>281</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B66" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>102</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B67" t="s">
         <v>287</v>
       </c>
     </row>
@@ -4036,20 +4050,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E04294AC-DBC1-4E51-84ED-2EC5066B9024}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.5" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4078,7 +4092,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -4107,7 +4121,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -4136,18 +4150,18 @@
         <v>293</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>520</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4">
-        <v>32030000</v>
+        <v>-99</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>521</v>
       </c>
       <c r="E4" t="s">
         <v>22</v>
@@ -4165,18 +4179,18 @@
         <v>293</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5">
-        <v>32040000</v>
+        <v>32030000</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E5" t="s">
         <v>22</v>
@@ -4194,18 +4208,18 @@
         <v>293</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6">
-        <v>32050000</v>
+        <v>32040000</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E6" t="s">
         <v>22</v>
@@ -4223,18 +4237,18 @@
         <v>293</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7">
-        <v>32060000</v>
+        <v>32050000</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E7" t="s">
         <v>22</v>
@@ -4249,50 +4263,50 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>32060000</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" t="s">
+        <v>54</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>26</v>
       </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
         <v>32130000</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>46</v>
-      </c>
-      <c r="E8" t="s">
-        <v>54</v>
-      </c>
-      <c r="F8" t="s">
-        <v>24</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>32140000</v>
-      </c>
-      <c r="D9" t="s">
-        <v>47</v>
       </c>
       <c r="E9" t="s">
         <v>54</v>
@@ -4310,18 +4324,18 @@
         <v>293</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10">
-        <v>32150000</v>
+        <v>32140000</v>
       </c>
       <c r="D10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E10" t="s">
         <v>54</v>
@@ -4339,47 +4353,47 @@
         <v>293</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>32150000</v>
+      </c>
+      <c r="D11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>29</v>
       </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11">
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
         <v>32160000</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" t="s">
         <v>49</v>
-      </c>
-      <c r="E11" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>32170000</v>
-      </c>
-      <c r="D12" t="s">
-        <v>50</v>
       </c>
       <c r="E12" t="s">
         <v>22</v>
@@ -4397,76 +4411,76 @@
         <v>292</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13">
-        <v>32180000</v>
+        <v>32170000</v>
       </c>
       <c r="D13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E13" t="s">
         <v>22</v>
       </c>
-      <c r="F13">
-        <v>0</v>
+      <c r="F13" t="s">
+        <v>22</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
-      <c r="H13" t="s">
-        <v>24</v>
+      <c r="H13">
+        <v>0</v>
       </c>
       <c r="I13" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>32180000</v>
+      </c>
+      <c r="D14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14" t="s">
+        <v>24</v>
+      </c>
+      <c r="I14" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>32</v>
       </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14">
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
         <v>32190000</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D15" t="s">
         <v>42</v>
-      </c>
-      <c r="E14" t="s">
-        <v>39</v>
-      </c>
-      <c r="F14" t="s">
-        <v>54</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15">
-        <v>32210000</v>
-      </c>
-      <c r="D15" t="s">
-        <v>43</v>
       </c>
       <c r="E15" t="s">
         <v>39</v>
@@ -4484,18 +4498,18 @@
         <v>292</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16">
-        <v>32220000</v>
+        <v>32210000</v>
       </c>
       <c r="D16" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="E16" t="s">
         <v>39</v>
@@ -4513,177 +4527,206 @@
         <v>292</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>32220000</v>
+      </c>
+      <c r="D17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" t="s">
+        <v>54</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>35</v>
       </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17">
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
         <v>32230000</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D18" t="s">
         <v>41</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E18" t="s">
         <v>22</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F18" t="s">
         <v>40</v>
       </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18">
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
         <v>32300000</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D19" t="s">
         <v>44</v>
       </c>
-      <c r="E18" t="s">
-        <v>54</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="E19" t="s">
+        <v>54</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>19</v>
       </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19">
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
         <v>32310000</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D20" t="s">
         <v>45</v>
       </c>
-      <c r="E19" t="s">
-        <v>54</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="E20" t="s">
+        <v>54</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>36</v>
       </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20">
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
         <v>32320000</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D21" t="s">
         <v>37</v>
       </c>
-      <c r="E20" t="s">
-        <v>54</v>
-      </c>
-      <c r="F20" t="s">
-        <v>24</v>
-      </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="E21" t="s">
+        <v>54</v>
+      </c>
+      <c r="F21" t="s">
+        <v>24</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>16</v>
       </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21">
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
         <v>32330000</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D22" t="s">
         <v>17</v>
       </c>
-      <c r="E21" t="s">
-        <v>54</v>
-      </c>
-      <c r="F21" t="s">
-        <v>24</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="E22" t="s">
+        <v>54</v>
+      </c>
+      <c r="F22" t="s">
+        <v>24</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>52</v>
       </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="C22">
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
         <v>32340000</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D23" t="s">
         <v>53</v>
       </c>
-      <c r="E22" t="s">
-        <v>54</v>
-      </c>
-      <c r="F22" t="s">
-        <v>24</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-      <c r="I22" t="s">
+      <c r="E23" t="s">
+        <v>54</v>
+      </c>
+      <c r="F23" t="s">
+        <v>24</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23" t="s">
         <v>292</v>
       </c>
     </row>
@@ -4700,13 +4743,13 @@
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.5" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4735,7 +4778,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>96</v>
       </c>
@@ -4764,7 +4807,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>99</v>
       </c>
@@ -4793,7 +4836,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>100</v>
       </c>
@@ -4822,7 +4865,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>101</v>
       </c>
@@ -4851,7 +4894,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>102</v>
       </c>
@@ -4880,7 +4923,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>103</v>
       </c>
@@ -4909,7 +4952,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>104</v>
       </c>
@@ -4938,7 +4981,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>105</v>
       </c>
@@ -4967,7 +5010,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>106</v>
       </c>
@@ -4996,7 +5039,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>107</v>
       </c>
@@ -5025,7 +5068,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>108</v>
       </c>
@@ -5054,7 +5097,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>109</v>
       </c>
@@ -5083,7 +5126,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>110</v>
       </c>
@@ -5112,7 +5155,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>111</v>
       </c>
@@ -5141,7 +5184,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>112</v>
       </c>
@@ -5170,7 +5213,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>113</v>
       </c>
@@ -5212,9 +5255,9 @@
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5243,7 +5286,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>297</v>
       </c>
@@ -5272,7 +5315,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>298</v>
       </c>
@@ -5301,7 +5344,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>299</v>
       </c>
@@ -5330,7 +5373,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>300</v>
       </c>
@@ -5359,7 +5402,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>301</v>
       </c>
@@ -5388,7 +5431,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>302</v>
       </c>
@@ -5417,7 +5460,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>303</v>
       </c>
@@ -5446,7 +5489,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>304</v>
       </c>
@@ -5475,7 +5518,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>305</v>
       </c>
@@ -5504,7 +5547,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>306</v>
       </c>
@@ -5533,7 +5576,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>307</v>
       </c>
@@ -5562,7 +5605,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>308</v>
       </c>
@@ -5591,7 +5634,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>309</v>
       </c>
@@ -5620,7 +5663,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>310</v>
       </c>
@@ -5649,7 +5692,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>311</v>
       </c>
@@ -5678,7 +5721,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>312</v>
       </c>
@@ -5707,7 +5750,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>313</v>
       </c>
@@ -5736,7 +5779,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>314</v>
       </c>
@@ -5765,7 +5808,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>315</v>
       </c>
@@ -5794,7 +5837,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>316</v>
       </c>
@@ -5823,7 +5866,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>317</v>
       </c>
@@ -5852,7 +5895,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>318</v>
       </c>
@@ -5891,13 +5934,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2593ADB1-2BA8-F64B-8388-EB1692F5297C}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5926,7 +5969,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>344</v>
       </c>
@@ -5955,7 +5998,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>345</v>
       </c>
@@ -5984,7 +6027,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>346</v>
       </c>
@@ -6013,7 +6056,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>347</v>
       </c>
@@ -6042,7 +6085,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>348</v>
       </c>
@@ -6071,7 +6114,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>349</v>
       </c>
@@ -6100,7 +6143,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>350</v>
       </c>
@@ -6129,7 +6172,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>351</v>
       </c>
@@ -6158,7 +6201,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>352</v>
       </c>
@@ -6187,7 +6230,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>353</v>
       </c>
@@ -6216,7 +6259,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>354</v>
       </c>
@@ -6245,7 +6288,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>355</v>
       </c>
@@ -6274,7 +6317,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>356</v>
       </c>
@@ -6303,7 +6346,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>357</v>
       </c>
@@ -6332,7 +6375,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>358</v>
       </c>
@@ -6361,7 +6404,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>359</v>
       </c>
@@ -6390,7 +6433,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>360</v>
       </c>
@@ -6419,7 +6462,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>361</v>
       </c>
@@ -6448,7 +6491,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>362</v>
       </c>
@@ -6477,7 +6520,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>363</v>
       </c>
@@ -6506,7 +6549,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>364</v>
       </c>
@@ -6535,7 +6578,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>365</v>
       </c>
@@ -6577,9 +6620,9 @@
       <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6608,7 +6651,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>388</v>
       </c>
@@ -6637,7 +6680,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>389</v>
       </c>
@@ -6666,7 +6709,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>390</v>
       </c>
@@ -6695,7 +6738,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>391</v>
       </c>
@@ -6724,7 +6767,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>392</v>
       </c>
@@ -6753,7 +6796,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>393</v>
       </c>
@@ -6782,7 +6825,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>394</v>
       </c>
@@ -6811,7 +6854,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>395</v>
       </c>
@@ -6840,7 +6883,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>396</v>
       </c>
@@ -6869,7 +6912,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>397</v>
       </c>
@@ -6898,7 +6941,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>398</v>
       </c>
@@ -6927,7 +6970,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>399</v>
       </c>
@@ -6956,7 +6999,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>400</v>
       </c>
@@ -6985,7 +7028,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>401</v>
       </c>
@@ -7014,7 +7057,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>402</v>
       </c>
@@ -7043,7 +7086,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>403</v>
       </c>
@@ -7072,7 +7115,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>404</v>
       </c>
@@ -7101,7 +7144,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>405</v>
       </c>
@@ -7130,7 +7173,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>406</v>
       </c>
@@ -7159,7 +7202,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>407</v>
       </c>
@@ -7188,7 +7231,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>408</v>
       </c>
@@ -7217,7 +7260,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>409</v>
       </c>
@@ -7259,9 +7302,9 @@
       <selection activeCell="D2" sqref="D2:D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7290,7 +7333,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>432</v>
       </c>
@@ -7319,7 +7362,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>433</v>
       </c>
@@ -7348,7 +7391,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>434</v>
       </c>
@@ -7377,7 +7420,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>435</v>
       </c>
@@ -7406,7 +7449,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>436</v>
       </c>
@@ -7435,7 +7478,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>437</v>
       </c>
@@ -7464,7 +7507,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>438</v>
       </c>
@@ -7493,7 +7536,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>439</v>
       </c>
@@ -7522,7 +7565,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>440</v>
       </c>
@@ -7551,7 +7594,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>441</v>
       </c>
@@ -7580,7 +7623,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>442</v>
       </c>
@@ -7609,7 +7652,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>443</v>
       </c>
@@ -7638,7 +7681,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>444</v>
       </c>
@@ -7667,7 +7710,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>445</v>
       </c>
@@ -7696,7 +7739,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>446</v>
       </c>
@@ -7725,7 +7768,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>447</v>
       </c>
@@ -7754,7 +7797,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>448</v>
       </c>
@@ -7783,7 +7826,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>449</v>
       </c>
@@ -7812,7 +7855,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>450</v>
       </c>
@@ -7841,7 +7884,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>451</v>
       </c>
@@ -7870,7 +7913,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>452</v>
       </c>
@@ -7899,7 +7942,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>453</v>
       </c>
@@ -7941,9 +7984,9 @@
       <selection activeCell="D2" sqref="D2:D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7972,7 +8015,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>476</v>
       </c>
@@ -8001,7 +8044,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>477</v>
       </c>
@@ -8030,7 +8073,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>478</v>
       </c>
@@ -8059,7 +8102,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>479</v>
       </c>
@@ -8088,7 +8131,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>480</v>
       </c>
@@ -8117,7 +8160,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>481</v>
       </c>
@@ -8146,7 +8189,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>482</v>
       </c>
@@ -8175,7 +8218,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>483</v>
       </c>
@@ -8204,7 +8247,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>484</v>
       </c>
@@ -8233,7 +8276,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>485</v>
       </c>
@@ -8262,7 +8305,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>486</v>
       </c>
@@ -8291,7 +8334,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>487</v>
       </c>
@@ -8320,7 +8363,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>488</v>
       </c>
@@ -8349,7 +8392,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>489</v>
       </c>
@@ -8378,7 +8421,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>490</v>
       </c>
@@ -8407,7 +8450,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>491</v>
       </c>
@@ -8436,7 +8479,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>492</v>
       </c>
@@ -8465,7 +8508,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>493</v>
       </c>
@@ -8494,7 +8537,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>494</v>
       </c>
@@ -8523,7 +8566,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>495</v>
       </c>
@@ -8552,7 +8595,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>496</v>
       </c>
@@ -8581,7 +8624,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>497</v>
       </c>
@@ -8623,14 +8666,14 @@
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="50.5" customWidth="1"/>
-    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.42578125" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8659,7 +8702,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>131</v>
       </c>
@@ -8688,7 +8731,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>155</v>
       </c>
@@ -8717,7 +8760,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>132</v>
       </c>
@@ -8746,7 +8789,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>133</v>
       </c>
@@ -8775,7 +8818,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>134</v>
       </c>
@@ -8804,7 +8847,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>135</v>
       </c>
@@ -8833,7 +8876,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>136</v>
       </c>
@@ -8862,7 +8905,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>137</v>
       </c>
@@ -8891,7 +8934,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>138</v>
       </c>
@@ -8920,7 +8963,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>139</v>
       </c>
@@ -8949,7 +8992,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>140</v>
       </c>
@@ -8978,7 +9021,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>141</v>
       </c>
@@ -9007,7 +9050,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>142</v>
       </c>
@@ -9036,7 +9079,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>143</v>
       </c>
@@ -9065,7 +9108,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>144</v>
       </c>
@@ -9094,7 +9137,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>145</v>
       </c>
@@ -9123,7 +9166,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>146</v>
       </c>
@@ -9152,7 +9195,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>147</v>
       </c>
@@ -9181,7 +9224,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>148</v>
       </c>
@@ -9210,7 +9253,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>149</v>
       </c>
@@ -9239,7 +9282,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>150</v>
       </c>
@@ -9268,7 +9311,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>151</v>
       </c>
@@ -9297,7 +9340,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>152</v>
       </c>
@@ -9326,7 +9369,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>153</v>
       </c>

</xml_diff>

<commit_message>
Add a 2D mandate variable + adjustment in the BHTC variable
Also put the full mandate code in the ftt_core functions, as it wasn't as DRY as could be
</commit_message>
<xml_diff>
--- a/Inputs/_MasterFiles/FTT_variables.xlsx
+++ b/Inputs/_MasterFiles/FTT_variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rosiehayward/Documents/GitHub/FTT_StandAlone/Inputs/_MasterFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/f_j_m_m_nijsse_exeter_ac_uk/Documents/Documents/GitHub/FTT_StandAlone/Inputs/_MasterFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B21FCB0C-8A9E-F54D-8028-8000D713EF49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{B21FCB0C-8A9E-F54D-8028-8000D713EF49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{79F5AD6D-13D2-4F21-8F0A-F9F57BB90DD8}"/>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="1440" windowWidth="22940" windowHeight="12480" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FTT-P" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1494" uniqueCount="520">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1501" uniqueCount="522">
   <si>
     <t>Variable name</t>
   </si>
@@ -1607,13 +1607,19 @@
   </si>
   <si>
     <t xml:space="preserve">FTT-IH-OIS Fuel tax (2010 Euros/MWh) </t>
+  </si>
+  <si>
+    <t>HMAN</t>
+  </si>
+  <si>
+    <t>FTT-Heat minimum sales mandate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1627,8 +1633,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1653,6 +1666,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1663,16 +1681,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1957,16 +1978,16 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" customWidth="1"/>
-    <col min="7" max="7" width="14.5" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1995,7 +2016,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2024,7 +2045,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>58</v>
       </c>
@@ -2053,7 +2074,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>62</v>
       </c>
@@ -2082,7 +2103,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>63</v>
       </c>
@@ -2111,7 +2132,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>74</v>
       </c>
@@ -2140,7 +2161,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>84</v>
       </c>
@@ -2169,7 +2190,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -2198,7 +2219,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>79</v>
       </c>
@@ -2227,7 +2248,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>70</v>
       </c>
@@ -2256,7 +2277,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>72</v>
       </c>
@@ -2285,7 +2306,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -2314,7 +2335,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>81</v>
       </c>
@@ -2343,7 +2364,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>88</v>
       </c>
@@ -2372,7 +2393,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>90</v>
       </c>
@@ -2401,7 +2422,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>80</v>
       </c>
@@ -2430,7 +2451,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>82</v>
       </c>
@@ -2459,7 +2480,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>66</v>
       </c>
@@ -2488,7 +2509,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>76</v>
       </c>
@@ -2536,17 +2557,17 @@
       <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2581,7 +2602,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>186</v>
       </c>
@@ -2616,7 +2637,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>189</v>
       </c>
@@ -2651,7 +2672,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>220</v>
       </c>
@@ -2686,7 +2707,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>195</v>
       </c>
@@ -2721,7 +2742,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>198</v>
       </c>
@@ -2756,7 +2777,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>219</v>
       </c>
@@ -2791,7 +2812,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>221</v>
       </c>
@@ -2826,7 +2847,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>222</v>
       </c>
@@ -2861,7 +2882,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>223</v>
       </c>
@@ -2896,7 +2917,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>224</v>
       </c>
@@ -2931,7 +2952,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>225</v>
       </c>
@@ -2966,7 +2987,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>215</v>
       </c>
@@ -3001,7 +3022,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>229</v>
       </c>
@@ -3033,7 +3054,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>231</v>
       </c>
@@ -3065,7 +3086,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>238</v>
       </c>
@@ -3100,7 +3121,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>239</v>
       </c>
@@ -3135,7 +3156,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>242</v>
       </c>
@@ -3170,7 +3191,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>248</v>
       </c>
@@ -3205,7 +3226,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>250</v>
       </c>
@@ -3240,7 +3261,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>254</v>
       </c>
@@ -3275,7 +3296,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>258</v>
       </c>
@@ -3310,7 +3331,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>264</v>
       </c>
@@ -3345,7 +3366,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>270</v>
       </c>
@@ -3380,7 +3401,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>266</v>
       </c>
@@ -3415,7 +3436,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>276</v>
       </c>
@@ -3450,7 +3471,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>281</v>
       </c>
@@ -3492,15 +3513,15 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA629D80-511C-42AD-ACB3-22237E3BD282}">
-  <dimension ref="A1:B66"/>
+  <dimension ref="A1:B67"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="M77" sqref="M77"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3508,7 +3529,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -3516,7 +3537,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -3524,7 +3545,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -3532,7 +3553,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -3540,7 +3561,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -3548,7 +3569,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -3556,7 +3577,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -3564,7 +3585,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -3572,7 +3593,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -3580,7 +3601,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -3588,7 +3609,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -3596,7 +3617,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -3604,7 +3625,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>58</v>
       </c>
@@ -3612,7 +3633,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>62</v>
       </c>
@@ -3620,7 +3641,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>63</v>
       </c>
@@ -3628,7 +3649,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>74</v>
       </c>
@@ -3636,7 +3657,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>79</v>
       </c>
@@ -3644,7 +3665,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>70</v>
       </c>
@@ -3652,7 +3673,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>72</v>
       </c>
@@ -3660,7 +3681,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>68</v>
       </c>
@@ -3668,7 +3689,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>66</v>
       </c>
@@ -3676,7 +3697,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>76</v>
       </c>
@@ -3684,7 +3705,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>103</v>
       </c>
@@ -3692,7 +3713,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>104</v>
       </c>
@@ -3700,7 +3721,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>105</v>
       </c>
@@ -3708,7 +3729,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>106</v>
       </c>
@@ -3716,7 +3737,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>107</v>
       </c>
@@ -3724,7 +3745,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>108</v>
       </c>
@@ -3732,7 +3753,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>109</v>
       </c>
@@ -3740,291 +3761,299 @@
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>110</v>
+        <v>520</v>
       </c>
       <c r="B31" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B32" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B33" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="B34" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>130</v>
+      </c>
+      <c r="B35" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>131</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>155</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>132</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>147</v>
-      </c>
-      <c r="B38" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>148</v>
       </c>
       <c r="B39" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B40" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B41" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B42" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B43" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B44" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>153</v>
+      </c>
+      <c r="B45" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>186</v>
-      </c>
-      <c r="B45" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>189</v>
       </c>
       <c r="B46" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>189</v>
+      </c>
+      <c r="B47" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>220</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>195</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>198</v>
-      </c>
-      <c r="B49" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>219</v>
       </c>
       <c r="B50" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B51" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B52" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B53" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B54" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B55" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>225</v>
+      </c>
+      <c r="B56" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>215</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B57" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>248</v>
-      </c>
-      <c r="B57" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>250</v>
       </c>
       <c r="B58" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B59" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="B60" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>270</v>
+      </c>
+      <c r="B61" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>31</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B62" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>286</v>
-      </c>
-      <c r="B62" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>290</v>
       </c>
       <c r="B63" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="B64" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>295</v>
+      </c>
+      <c r="B65" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>281</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B66" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>102</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B67" t="s">
         <v>287</v>
       </c>
     </row>
@@ -4042,14 +4071,14 @@
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.5" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4078,7 +4107,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -4107,7 +4136,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -4136,7 +4165,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -4165,7 +4194,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -4194,7 +4223,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -4223,7 +4252,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -4252,7 +4281,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -4281,7 +4310,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -4310,7 +4339,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -4339,7 +4368,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -4368,7 +4397,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -4397,7 +4426,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -4426,7 +4455,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -4455,7 +4484,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -4484,7 +4513,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -4513,7 +4542,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -4542,7 +4571,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -4571,7 +4600,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -4600,7 +4629,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -4629,7 +4658,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -4658,7 +4687,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>52</v>
       </c>
@@ -4694,19 +4723,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{893746F0-70F0-4C21-8E46-9B5DBA6E54BB}">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.5" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4735,7 +4764,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>96</v>
       </c>
@@ -4764,7 +4793,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>99</v>
       </c>
@@ -4793,7 +4822,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>100</v>
       </c>
@@ -4822,7 +4851,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>101</v>
       </c>
@@ -4851,7 +4880,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>102</v>
       </c>
@@ -4880,7 +4909,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>103</v>
       </c>
@@ -4909,7 +4938,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>104</v>
       </c>
@@ -4938,7 +4967,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>105</v>
       </c>
@@ -4967,7 +4996,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>106</v>
       </c>
@@ -4996,7 +5025,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>107</v>
       </c>
@@ -5025,7 +5054,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>108</v>
       </c>
@@ -5054,7 +5083,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>109</v>
       </c>
@@ -5083,7 +5112,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>110</v>
       </c>
@@ -5112,7 +5141,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>111</v>
       </c>
@@ -5141,27 +5170,27 @@
         <v>293</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>112</v>
+        <v>520</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
-      <c r="C16">
-        <v>33110000</v>
+      <c r="C16" s="4">
+        <v>33190000</v>
       </c>
       <c r="D16" t="s">
-        <v>128</v>
+        <v>521</v>
       </c>
       <c r="E16" t="s">
-        <v>98</v>
+        <v>54</v>
       </c>
       <c r="F16" t="s">
         <v>24</v>
       </c>
-      <c r="G16" t="s">
-        <v>54</v>
+      <c r="G16">
+        <v>0</v>
       </c>
       <c r="H16">
         <v>0</v>
@@ -5170,32 +5199,61 @@
         <v>293</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17">
-        <v>33010000</v>
+        <v>33110000</v>
       </c>
       <c r="D17" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="E17" t="s">
         <v>98</v>
       </c>
       <c r="F17" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17" t="s">
+        <v>54</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>113</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>33010000</v>
+      </c>
+      <c r="D18" t="s">
+        <v>114</v>
+      </c>
+      <c r="E18" t="s">
+        <v>98</v>
+      </c>
+      <c r="F18" t="s">
         <v>129</v>
       </c>
-      <c r="G17" t="s">
-        <v>54</v>
-      </c>
-      <c r="H17" t="s">
+      <c r="G18" t="s">
+        <v>54</v>
+      </c>
+      <c r="H18" t="s">
         <v>289</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I18" t="s">
         <v>292</v>
       </c>
     </row>
@@ -5212,9 +5270,9 @@
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5243,7 +5301,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>297</v>
       </c>
@@ -5272,7 +5330,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>298</v>
       </c>
@@ -5301,7 +5359,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>299</v>
       </c>
@@ -5330,7 +5388,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>300</v>
       </c>
@@ -5359,7 +5417,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>301</v>
       </c>
@@ -5388,7 +5446,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>302</v>
       </c>
@@ -5417,7 +5475,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>303</v>
       </c>
@@ -5446,7 +5504,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>304</v>
       </c>
@@ -5475,7 +5533,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>305</v>
       </c>
@@ -5504,7 +5562,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>306</v>
       </c>
@@ -5533,7 +5591,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>307</v>
       </c>
@@ -5562,7 +5620,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>308</v>
       </c>
@@ -5591,7 +5649,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>309</v>
       </c>
@@ -5620,7 +5678,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>310</v>
       </c>
@@ -5649,7 +5707,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>311</v>
       </c>
@@ -5678,7 +5736,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>312</v>
       </c>
@@ -5707,7 +5765,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>313</v>
       </c>
@@ -5736,7 +5794,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>314</v>
       </c>
@@ -5765,7 +5823,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>315</v>
       </c>
@@ -5794,7 +5852,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>316</v>
       </c>
@@ -5823,7 +5881,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>317</v>
       </c>
@@ -5852,7 +5910,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>318</v>
       </c>
@@ -5891,13 +5949,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2593ADB1-2BA8-F64B-8388-EB1692F5297C}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5926,7 +5984,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>344</v>
       </c>
@@ -5955,7 +6013,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>345</v>
       </c>
@@ -5984,7 +6042,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>346</v>
       </c>
@@ -6013,7 +6071,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>347</v>
       </c>
@@ -6042,7 +6100,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>348</v>
       </c>
@@ -6071,7 +6129,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>349</v>
       </c>
@@ -6100,7 +6158,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>350</v>
       </c>
@@ -6129,7 +6187,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>351</v>
       </c>
@@ -6158,7 +6216,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>352</v>
       </c>
@@ -6187,7 +6245,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>353</v>
       </c>
@@ -6216,7 +6274,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>354</v>
       </c>
@@ -6245,7 +6303,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>355</v>
       </c>
@@ -6274,7 +6332,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>356</v>
       </c>
@@ -6303,7 +6361,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>357</v>
       </c>
@@ -6332,7 +6390,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>358</v>
       </c>
@@ -6361,7 +6419,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>359</v>
       </c>
@@ -6390,7 +6448,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>360</v>
       </c>
@@ -6419,7 +6477,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>361</v>
       </c>
@@ -6448,7 +6506,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>362</v>
       </c>
@@ -6477,7 +6535,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>363</v>
       </c>
@@ -6506,7 +6564,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>364</v>
       </c>
@@ -6535,7 +6593,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>365</v>
       </c>
@@ -6577,9 +6635,9 @@
       <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6608,7 +6666,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>388</v>
       </c>
@@ -6637,7 +6695,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>389</v>
       </c>
@@ -6666,7 +6724,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>390</v>
       </c>
@@ -6695,7 +6753,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>391</v>
       </c>
@@ -6724,7 +6782,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>392</v>
       </c>
@@ -6753,7 +6811,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>393</v>
       </c>
@@ -6782,7 +6840,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>394</v>
       </c>
@@ -6811,7 +6869,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>395</v>
       </c>
@@ -6840,7 +6898,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>396</v>
       </c>
@@ -6869,7 +6927,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>397</v>
       </c>
@@ -6898,7 +6956,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>398</v>
       </c>
@@ -6927,7 +6985,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>399</v>
       </c>
@@ -6956,7 +7014,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>400</v>
       </c>
@@ -6985,7 +7043,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>401</v>
       </c>
@@ -7014,7 +7072,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>402</v>
       </c>
@@ -7043,7 +7101,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>403</v>
       </c>
@@ -7072,7 +7130,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>404</v>
       </c>
@@ -7101,7 +7159,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>405</v>
       </c>
@@ -7130,7 +7188,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>406</v>
       </c>
@@ -7159,7 +7217,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>407</v>
       </c>
@@ -7188,7 +7246,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>408</v>
       </c>
@@ -7217,7 +7275,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>409</v>
       </c>
@@ -7259,9 +7317,9 @@
       <selection activeCell="D2" sqref="D2:D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7290,7 +7348,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>432</v>
       </c>
@@ -7319,7 +7377,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>433</v>
       </c>
@@ -7348,7 +7406,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>434</v>
       </c>
@@ -7377,7 +7435,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>435</v>
       </c>
@@ -7406,7 +7464,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>436</v>
       </c>
@@ -7435,7 +7493,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>437</v>
       </c>
@@ -7464,7 +7522,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>438</v>
       </c>
@@ -7493,7 +7551,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>439</v>
       </c>
@@ -7522,7 +7580,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>440</v>
       </c>
@@ -7551,7 +7609,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>441</v>
       </c>
@@ -7580,7 +7638,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>442</v>
       </c>
@@ -7609,7 +7667,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>443</v>
       </c>
@@ -7638,7 +7696,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>444</v>
       </c>
@@ -7667,7 +7725,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>445</v>
       </c>
@@ -7696,7 +7754,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>446</v>
       </c>
@@ -7725,7 +7783,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>447</v>
       </c>
@@ -7754,7 +7812,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>448</v>
       </c>
@@ -7783,7 +7841,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>449</v>
       </c>
@@ -7812,7 +7870,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>450</v>
       </c>
@@ -7841,7 +7899,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>451</v>
       </c>
@@ -7870,7 +7928,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>452</v>
       </c>
@@ -7899,7 +7957,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>453</v>
       </c>
@@ -7941,9 +7999,9 @@
       <selection activeCell="D2" sqref="D2:D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7972,7 +8030,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>476</v>
       </c>
@@ -8001,7 +8059,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>477</v>
       </c>
@@ -8030,7 +8088,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>478</v>
       </c>
@@ -8059,7 +8117,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>479</v>
       </c>
@@ -8088,7 +8146,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>480</v>
       </c>
@@ -8117,7 +8175,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>481</v>
       </c>
@@ -8146,7 +8204,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>482</v>
       </c>
@@ -8175,7 +8233,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>483</v>
       </c>
@@ -8204,7 +8262,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>484</v>
       </c>
@@ -8233,7 +8291,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>485</v>
       </c>
@@ -8262,7 +8320,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>486</v>
       </c>
@@ -8291,7 +8349,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>487</v>
       </c>
@@ -8320,7 +8378,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>488</v>
       </c>
@@ -8349,7 +8407,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>489</v>
       </c>
@@ -8378,7 +8436,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>490</v>
       </c>
@@ -8407,7 +8465,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>491</v>
       </c>
@@ -8436,7 +8494,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>492</v>
       </c>
@@ -8465,7 +8523,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>493</v>
       </c>
@@ -8494,7 +8552,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>494</v>
       </c>
@@ -8523,7 +8581,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>495</v>
       </c>
@@ -8552,7 +8610,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>496</v>
       </c>
@@ -8581,7 +8639,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>497</v>
       </c>
@@ -8623,14 +8681,14 @@
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="50.5" customWidth="1"/>
-    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.42578125" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8659,7 +8717,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>131</v>
       </c>
@@ -8688,7 +8746,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>155</v>
       </c>
@@ -8717,7 +8775,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>132</v>
       </c>
@@ -8746,7 +8804,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>133</v>
       </c>
@@ -8775,7 +8833,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>134</v>
       </c>
@@ -8804,7 +8862,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>135</v>
       </c>
@@ -8833,7 +8891,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>136</v>
       </c>
@@ -8862,7 +8920,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>137</v>
       </c>
@@ -8891,7 +8949,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>138</v>
       </c>
@@ -8920,7 +8978,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>139</v>
       </c>
@@ -8949,7 +9007,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>140</v>
       </c>
@@ -8978,7 +9036,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>141</v>
       </c>
@@ -9007,7 +9065,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>142</v>
       </c>
@@ -9036,7 +9094,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>143</v>
       </c>
@@ -9065,7 +9123,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>144</v>
       </c>
@@ -9094,7 +9152,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>145</v>
       </c>
@@ -9123,7 +9181,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>146</v>
       </c>
@@ -9152,7 +9210,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>147</v>
       </c>
@@ -9181,7 +9239,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>148</v>
       </c>
@@ -9210,7 +9268,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>149</v>
       </c>
@@ -9239,7 +9297,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>150</v>
       </c>
@@ -9268,7 +9326,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>151</v>
       </c>
@@ -9297,7 +9355,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>152</v>
       </c>
@@ -9326,7 +9384,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>153</v>
       </c>

</xml_diff>

<commit_message>
Prevent creation MGAM files
Simplify convert_masterfile_to_csv to prevent creation of unnecessary MGAM files. Data now stored in BCET
</commit_message>
<xml_diff>
--- a/Inputs/_MasterFiles/FTT_variables.xlsx
+++ b/Inputs/_MasterFiles/FTT_variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/f_j_m_m_nijsse_exeter_ac_uk/Documents/Documents/GitHub/FTT_StandAlone/Inputs/_MasterFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{B21FCB0C-8A9E-F54D-8028-8000D713EF49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E6F0B048-1151-46B4-B033-2DF93B4C08AB}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{B21FCB0C-8A9E-F54D-8028-8000D713EF49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C900ADFB-7DD5-4FDD-9006-F74785241C29}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1496" uniqueCount="521">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1495" uniqueCount="521">
   <si>
     <t>Variable name</t>
   </si>
@@ -1972,7 +1972,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2209,8 +2209,8 @@
       <c r="G8" t="s">
         <v>54</v>
       </c>
-      <c r="H8" t="s">
-        <v>288</v>
+      <c r="H8">
+        <v>0</v>
       </c>
       <c r="I8" t="s">
         <v>291</v>

</xml_diff>

<commit_message>
Adding FTT-H2 to the master
Pull request to include FTT-H2 into the master version.

There are a few oddities to sort out:
- CSC approach works in selecting the right technologies, but it fails to produce sensible prices. So far, we have relied on domestic LCOH2 estimates.
- Universal core FTT functions have been developed in parallel and need to be pulled into this version.
- Techno-economic cost data and technology classification may also change.
</commit_message>
<xml_diff>
--- a/Inputs/_MasterFiles/FTT_variables.xlsx
+++ b/Inputs/_MasterFiles/FTT_variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\E3ME\EEIST2_FTT-H2_dev\In\FTTAssumptions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cambridgeeconometrics-my.sharepoint.com/personal/pv_camecon_com/Documents/Documents/GitHub/FTT_H2_dev_v2/Inputs/_MasterFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62A0F244-D621-4931-9BF9-28DFD2CA0B35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{62A0F244-D621-4931-9BF9-28DFD2CA0B35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{207E3376-0038-4C94-ABBD-94ACBE824D45}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="8745" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FTT-P" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1165" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1160" uniqueCount="408">
   <si>
     <t>Variable name</t>
   </si>
@@ -1238,12 +1238,6 @@
   </si>
   <si>
     <t>Solar OPEX</t>
-  </si>
-  <si>
-    <t>HYWA</t>
-  </si>
-  <si>
-    <t>Substitution frequency matrix</t>
   </si>
   <si>
     <t>NH3-fert</t>
@@ -1340,13 +1334,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5241,9 +5234,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05986654-6C49-4A34-BECD-4482E94CE084}">
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5281,7 +5276,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" t="s">
         <v>307</v>
       </c>
       <c r="B2">
@@ -5310,7 +5305,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" t="s">
         <v>308</v>
       </c>
       <c r="B3">
@@ -5339,7 +5334,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" t="s">
         <v>310</v>
       </c>
       <c r="B4">
@@ -5368,7 +5363,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" t="s">
         <v>311</v>
       </c>
       <c r="B5">
@@ -5397,7 +5392,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" t="s">
         <v>321</v>
       </c>
       <c r="B6">
@@ -5426,7 +5421,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" t="s">
         <v>309</v>
       </c>
       <c r="B7">
@@ -5436,7 +5431,7 @@
         <v>36060000</v>
       </c>
       <c r="D7" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="E7" t="s">
         <v>54</v>
@@ -5455,7 +5450,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" t="s">
         <v>324</v>
       </c>
       <c r="B8">
@@ -5484,7 +5479,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" t="s">
         <v>325</v>
       </c>
       <c r="B9">
@@ -5513,7 +5508,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" t="s">
         <v>326</v>
       </c>
       <c r="B10">
@@ -5542,7 +5537,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" t="s">
         <v>327</v>
       </c>
       <c r="B11">
@@ -5571,7 +5566,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" t="s">
         <v>328</v>
       </c>
       <c r="B12">
@@ -5600,7 +5595,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" t="s">
         <v>329</v>
       </c>
       <c r="B13">
@@ -5629,7 +5624,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="A14" t="s">
         <v>330</v>
       </c>
       <c r="B14">
@@ -5658,7 +5653,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="A15" t="s">
         <v>331</v>
       </c>
       <c r="B15">
@@ -5687,7 +5682,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="A16" t="s">
         <v>332</v>
       </c>
       <c r="B16">
@@ -5716,7 +5711,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="A17" t="s">
         <v>333</v>
       </c>
       <c r="B17">
@@ -5745,7 +5740,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="A18" t="s">
         <v>334</v>
       </c>
       <c r="B18">
@@ -5774,7 +5769,7 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+      <c r="A19" t="s">
         <v>335</v>
       </c>
       <c r="B19">
@@ -5803,7 +5798,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+      <c r="A20" t="s">
         <v>336</v>
       </c>
       <c r="B20">
@@ -5832,17 +5827,17 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>398</v>
+      <c r="A21" t="s">
+        <v>337</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21">
-        <v>36200000</v>
+        <v>36210000</v>
       </c>
       <c r="D21" t="s">
-        <v>399</v>
+        <v>352</v>
       </c>
       <c r="E21" t="s">
         <v>316</v>
@@ -5861,26 +5856,26 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>337</v>
+      <c r="A22" t="s">
+        <v>338</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22">
-        <v>36210000</v>
+        <v>36220000</v>
       </c>
       <c r="D22" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="E22" t="s">
         <v>316</v>
       </c>
       <c r="F22" t="s">
-        <v>316</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
+        <v>24</v>
+      </c>
+      <c r="G22" t="s">
+        <v>54</v>
       </c>
       <c r="H22">
         <v>0</v>
@@ -5890,17 +5885,17 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>338</v>
+      <c r="A23" t="s">
+        <v>354</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23">
-        <v>36220000</v>
+        <v>36230000</v>
       </c>
       <c r="D23" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="E23" t="s">
         <v>316</v>
@@ -5919,345 +5914,345 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>354</v>
+      <c r="A24" t="s">
+        <v>355</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
       <c r="C24">
-        <v>36230000</v>
+        <v>36240000</v>
       </c>
       <c r="D24" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="E24" t="s">
+        <v>54</v>
+      </c>
+      <c r="F24" t="s">
+        <v>24</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>356</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>36250000</v>
+      </c>
+      <c r="D25" t="s">
+        <v>359</v>
+      </c>
+      <c r="E25" t="s">
+        <v>54</v>
+      </c>
+      <c r="F25" t="s">
+        <v>24</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>361</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>36260000</v>
+      </c>
+      <c r="D26" t="s">
+        <v>366</v>
+      </c>
+      <c r="E26" t="s">
+        <v>54</v>
+      </c>
+      <c r="F26" t="s">
+        <v>24</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>362</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>36270000</v>
+      </c>
+      <c r="D27" t="s">
+        <v>367</v>
+      </c>
+      <c r="E27" t="s">
+        <v>54</v>
+      </c>
+      <c r="F27" t="s">
+        <v>24</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>363</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>36280000</v>
+      </c>
+      <c r="D28" t="s">
+        <v>368</v>
+      </c>
+      <c r="E28" t="s">
+        <v>54</v>
+      </c>
+      <c r="F28" t="s">
+        <v>24</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>364</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>36290000</v>
+      </c>
+      <c r="D29" t="s">
+        <v>369</v>
+      </c>
+      <c r="E29" t="s">
+        <v>54</v>
+      </c>
+      <c r="F29" t="s">
+        <v>24</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>365</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>36300000</v>
+      </c>
+      <c r="D30" t="s">
+        <v>370</v>
+      </c>
+      <c r="E30" t="s">
+        <v>54</v>
+      </c>
+      <c r="F30" t="s">
+        <v>24</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>371</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>36310000</v>
+      </c>
+      <c r="D31" t="s">
+        <v>315</v>
+      </c>
+      <c r="E31" t="s">
         <v>316</v>
       </c>
-      <c r="F24" t="s">
-        <v>24</v>
-      </c>
-      <c r="G24" t="s">
-        <v>54</v>
-      </c>
-      <c r="H24">
-        <v>0</v>
-      </c>
-      <c r="I24" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>355</v>
-      </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="C25">
-        <v>36240000</v>
-      </c>
-      <c r="D25" t="s">
-        <v>358</v>
-      </c>
-      <c r="E25" t="s">
-        <v>54</v>
-      </c>
-      <c r="F25" t="s">
-        <v>24</v>
-      </c>
-      <c r="G25">
-        <v>0</v>
-      </c>
-      <c r="H25">
-        <v>0</v>
-      </c>
-      <c r="I25" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26">
-        <v>36250000</v>
-      </c>
-      <c r="D26" t="s">
-        <v>359</v>
-      </c>
-      <c r="E26" t="s">
-        <v>54</v>
-      </c>
-      <c r="F26" t="s">
-        <v>24</v>
-      </c>
-      <c r="G26">
-        <v>0</v>
-      </c>
-      <c r="H26">
-        <v>0</v>
-      </c>
-      <c r="I26" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
-        <v>361</v>
-      </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="C27">
-        <v>36260000</v>
-      </c>
-      <c r="D27" t="s">
-        <v>366</v>
-      </c>
-      <c r="E27" t="s">
-        <v>54</v>
-      </c>
-      <c r="F27" t="s">
-        <v>24</v>
-      </c>
-      <c r="G27">
-        <v>0</v>
-      </c>
-      <c r="H27">
-        <v>0</v>
-      </c>
-      <c r="I27" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>362</v>
-      </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28">
-        <v>36270000</v>
-      </c>
-      <c r="D28" t="s">
-        <v>367</v>
-      </c>
-      <c r="E28" t="s">
-        <v>54</v>
-      </c>
-      <c r="F28" t="s">
-        <v>24</v>
-      </c>
-      <c r="G28">
-        <v>0</v>
-      </c>
-      <c r="H28">
-        <v>0</v>
-      </c>
-      <c r="I28" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>363</v>
-      </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-      <c r="C29">
-        <v>36280000</v>
-      </c>
-      <c r="D29" t="s">
-        <v>368</v>
-      </c>
-      <c r="E29" t="s">
-        <v>54</v>
-      </c>
-      <c r="F29" t="s">
-        <v>24</v>
-      </c>
-      <c r="G29">
-        <v>0</v>
-      </c>
-      <c r="H29">
-        <v>0</v>
-      </c>
-      <c r="I29" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
-        <v>364</v>
-      </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="C30">
-        <v>36290000</v>
-      </c>
-      <c r="D30" t="s">
-        <v>369</v>
-      </c>
-      <c r="E30" t="s">
-        <v>54</v>
-      </c>
-      <c r="F30" t="s">
-        <v>24</v>
-      </c>
-      <c r="G30">
-        <v>0</v>
-      </c>
-      <c r="H30">
-        <v>0</v>
-      </c>
-      <c r="I30" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
-        <v>365</v>
-      </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="C31">
-        <v>36300000</v>
-      </c>
-      <c r="D31" t="s">
-        <v>370</v>
-      </c>
-      <c r="E31" t="s">
-        <v>54</v>
-      </c>
-      <c r="F31" t="s">
-        <v>24</v>
+      <c r="F31">
+        <v>0</v>
       </c>
       <c r="G31">
         <v>0</v>
       </c>
-      <c r="H31">
-        <v>0</v>
+      <c r="H31" t="s">
+        <v>24</v>
       </c>
       <c r="I31" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
-        <v>371</v>
+      <c r="A32" t="s">
+        <v>372</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
       <c r="C32">
-        <v>36310000</v>
+        <v>36320000</v>
       </c>
       <c r="D32" t="s">
-        <v>315</v>
+        <v>375</v>
       </c>
       <c r="E32" t="s">
+        <v>54</v>
+      </c>
+      <c r="F32" t="s">
+        <v>24</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>373</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>36330000</v>
+      </c>
+      <c r="D33" t="s">
+        <v>376</v>
+      </c>
+      <c r="E33" t="s">
+        <v>54</v>
+      </c>
+      <c r="F33" t="s">
+        <v>24</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>374</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>36340000</v>
+      </c>
+      <c r="D34" t="s">
+        <v>377</v>
+      </c>
+      <c r="E34" t="s">
+        <v>54</v>
+      </c>
+      <c r="F34" t="s">
+        <v>24</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>378</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>36350000</v>
+      </c>
+      <c r="D35" t="s">
+        <v>379</v>
+      </c>
+      <c r="E35" t="s">
         <v>316</v>
       </c>
-      <c r="F32">
-        <v>0</v>
-      </c>
-      <c r="G32">
-        <v>0</v>
-      </c>
-      <c r="H32" t="s">
-        <v>24</v>
-      </c>
-      <c r="I32" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
-        <v>372</v>
-      </c>
-      <c r="B33">
-        <v>1</v>
-      </c>
-      <c r="C33">
-        <v>36320000</v>
-      </c>
-      <c r="D33" t="s">
-        <v>375</v>
-      </c>
-      <c r="E33" t="s">
-        <v>54</v>
-      </c>
-      <c r="F33" t="s">
-        <v>24</v>
-      </c>
-      <c r="G33">
-        <v>0</v>
-      </c>
-      <c r="H33">
-        <v>0</v>
-      </c>
-      <c r="I33" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
-        <v>373</v>
-      </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-      <c r="C34">
-        <v>36330000</v>
-      </c>
-      <c r="D34" t="s">
-        <v>376</v>
-      </c>
-      <c r="E34" t="s">
-        <v>54</v>
-      </c>
-      <c r="F34" t="s">
-        <v>24</v>
-      </c>
-      <c r="G34">
-        <v>0</v>
-      </c>
-      <c r="H34">
-        <v>0</v>
-      </c>
-      <c r="I34" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
-        <v>374</v>
-      </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-      <c r="C35">
-        <v>36340000</v>
-      </c>
-      <c r="D35" t="s">
-        <v>377</v>
-      </c>
-      <c r="E35" t="s">
-        <v>54</v>
-      </c>
       <c r="F35" t="s">
         <v>24</v>
       </c>
-      <c r="G35">
-        <v>0</v>
+      <c r="G35" t="s">
+        <v>54</v>
       </c>
       <c r="H35">
         <v>0</v>
@@ -6267,26 +6262,26 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
-        <v>378</v>
+      <c r="A36" s="4" t="s">
+        <v>380</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
       <c r="C36">
-        <v>36350000</v>
-      </c>
-      <c r="D36" t="s">
-        <v>379</v>
+        <v>36360000</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>392</v>
       </c>
       <c r="E36" t="s">
-        <v>316</v>
+        <v>54</v>
       </c>
       <c r="F36" t="s">
         <v>24</v>
       </c>
-      <c r="G36" t="s">
-        <v>54</v>
+      <c r="G36">
+        <v>0</v>
       </c>
       <c r="H36">
         <v>0</v>
@@ -6297,16 +6292,16 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B37">
         <v>1</v>
       </c>
       <c r="C37">
-        <v>36360000</v>
+        <v>36370000</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="E37" t="s">
         <v>54</v>
@@ -6326,16 +6321,16 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="B38">
         <v>1</v>
       </c>
       <c r="C38">
-        <v>36370000</v>
+        <v>36380000</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="E38" t="s">
         <v>54</v>
@@ -6355,16 +6350,16 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B39">
         <v>1</v>
       </c>
       <c r="C39">
-        <v>36380000</v>
+        <v>36390000</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="E39" t="s">
         <v>54</v>
@@ -6384,16 +6379,16 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="B40">
         <v>1</v>
       </c>
       <c r="C40">
-        <v>36390000</v>
+        <v>36400000</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="E40" t="s">
         <v>54</v>
@@ -6413,16 +6408,16 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B41">
         <v>1</v>
       </c>
       <c r="C41">
-        <v>36400000</v>
+        <v>36410000</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="E41" t="s">
         <v>54</v>
@@ -6442,16 +6437,16 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B42">
         <v>1</v>
       </c>
       <c r="C42">
-        <v>36410000</v>
+        <v>36420000</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="E42" t="s">
         <v>54</v>
@@ -6471,16 +6466,16 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B43">
         <v>1</v>
       </c>
       <c r="C43">
-        <v>36420000</v>
+        <v>36430000</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E43" t="s">
         <v>54</v>
@@ -6500,16 +6495,16 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B44">
         <v>1</v>
       </c>
       <c r="C44">
-        <v>36430000</v>
+        <v>36440000</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E44" t="s">
         <v>54</v>
@@ -6529,45 +6524,45 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>388</v>
+        <v>402</v>
       </c>
       <c r="B45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C45">
-        <v>36440000</v>
+        <v>36450000</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>389</v>
+        <v>405</v>
       </c>
       <c r="E45" t="s">
-        <v>54</v>
+        <v>316</v>
       </c>
       <c r="F45" t="s">
         <v>24</v>
       </c>
-      <c r="G45">
-        <v>0</v>
+      <c r="G45" t="s">
+        <v>54</v>
       </c>
       <c r="H45">
         <v>0</v>
       </c>
       <c r="I45" t="s">
-        <v>292</v>
+        <v>399</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B46">
         <v>0</v>
       </c>
       <c r="C46">
-        <v>36450000</v>
+        <v>36460000</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E46" t="s">
         <v>316</v>
@@ -6582,21 +6577,21 @@
         <v>0</v>
       </c>
       <c r="I46" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B47">
         <v>0</v>
       </c>
       <c r="C47">
-        <v>36460000</v>
+        <v>36470000</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E47" t="s">
         <v>316</v>
@@ -6611,36 +6606,7 @@
         <v>0</v>
       </c>
       <c r="I47" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
-        <v>406</v>
-      </c>
-      <c r="B48">
-        <v>0</v>
-      </c>
-      <c r="C48">
-        <v>36470000</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>409</v>
-      </c>
-      <c r="E48" t="s">
-        <v>316</v>
-      </c>
-      <c r="F48" t="s">
-        <v>24</v>
-      </c>
-      <c r="G48" t="s">
-        <v>54</v>
-      </c>
-      <c r="H48">
-        <v>0</v>
-      </c>
-      <c r="I48" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
   </sheetData>
@@ -6653,8 +6619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA629D80-511C-42AD-ACB3-22237E3BD282}">
   <dimension ref="A1:B109"/>
   <sheetViews>
-    <sheetView topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="B109" sqref="B109"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
market shares - rooftop solar
Updated the files to calculate the market shares for rooftop solar and utility electricity
</commit_message>
<xml_diff>
--- a/Inputs/_MasterFiles/FTT_variables.xlsx
+++ b/Inputs/_MasterFiles/FTT_variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/f_j_m_m_nijsse_exeter_ac_uk/Documents/Documents/GitHub/FTT_StandAlone/Inputs/_MasterFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uqcpaesd\Documents\GitHub\FTT_StandAlone\Inputs\_MasterFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="76" documentId="13_ncr:1_{96C6DCC7-F135-4F9F-BBD1-97530C10B60C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE8E03F7-4FBD-495E-92BD-7DCE410BAAB3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2348AAE0-4093-464C-805C-FEA1C24F411E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FTT-P" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="281">
   <si>
     <t>Variable name</t>
   </si>
@@ -870,6 +870,21 @@
   </si>
   <si>
     <t>FTT-Tr relative registration tax or subsidy</t>
+  </si>
+  <si>
+    <t>MEWDH</t>
+  </si>
+  <si>
+    <t>FTT-Power household demand</t>
+  </si>
+  <si>
+    <t>tl_2010</t>
+  </si>
+  <si>
+    <t>PRICH</t>
+  </si>
+  <si>
+    <t>FTT-Price of electricity use (incl taxes)</t>
   </si>
 </sst>
 </file>
@@ -1200,22 +1215,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.81640625" customWidth="1"/>
+    <col min="7" max="7" width="14.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1244,7 +1259,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1273,7 +1288,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>58</v>
       </c>
@@ -1302,7 +1317,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>62</v>
       </c>
@@ -1331,7 +1346,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>63</v>
       </c>
@@ -1360,7 +1375,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>73</v>
       </c>
@@ -1389,7 +1404,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>83</v>
       </c>
@@ -1418,7 +1433,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -1447,7 +1462,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>78</v>
       </c>
@@ -1476,7 +1491,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>69</v>
       </c>
@@ -1505,7 +1520,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>71</v>
       </c>
@@ -1534,7 +1549,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>67</v>
       </c>
@@ -1563,7 +1578,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>80</v>
       </c>
@@ -1592,7 +1607,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>87</v>
       </c>
@@ -1621,7 +1636,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>89</v>
       </c>
@@ -1650,7 +1665,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>79</v>
       </c>
@@ -1679,7 +1694,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>81</v>
       </c>
@@ -1708,7 +1723,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>75</v>
       </c>
@@ -1734,6 +1749,64 @@
         <v>0</v>
       </c>
       <c r="I18" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>276</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>33333333</v>
+      </c>
+      <c r="D19" t="s">
+        <v>277</v>
+      </c>
+      <c r="E19" t="s">
+        <v>54</v>
+      </c>
+      <c r="F19" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>279</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>33333334</v>
+      </c>
+      <c r="D20" t="s">
+        <v>280</v>
+      </c>
+      <c r="E20" t="s">
+        <v>54</v>
+      </c>
+      <c r="F20" t="s">
+        <v>24</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20" t="s">
         <v>265</v>
       </c>
     </row>
@@ -1753,17 +1826,17 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E11" sqref="E11:I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.7109375" customWidth="1"/>
+    <col min="2" max="2" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1792,7 +1865,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1821,7 +1894,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1850,7 +1923,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1879,7 +1952,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1908,7 +1981,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1937,7 +2010,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1966,7 +2039,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>274</v>
       </c>
@@ -1995,7 +2068,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -2024,7 +2097,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -2053,7 +2126,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -2082,7 +2155,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -2111,7 +2184,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -2140,7 +2213,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -2169,7 +2242,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -2198,7 +2271,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -2227,7 +2300,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -2256,7 +2329,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -2285,7 +2358,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -2314,7 +2387,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -2343,7 +2416,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -2372,7 +2445,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -2401,7 +2474,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>52</v>
       </c>
@@ -2443,13 +2516,13 @@
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.42578125" customWidth="1"/>
+    <col min="2" max="2" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2478,7 +2551,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>95</v>
       </c>
@@ -2507,7 +2580,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>98</v>
       </c>
@@ -2536,7 +2609,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>99</v>
       </c>
@@ -2565,7 +2638,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>100</v>
       </c>
@@ -2594,7 +2667,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>101</v>
       </c>
@@ -2623,7 +2696,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>102</v>
       </c>
@@ -2652,7 +2725,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>103</v>
       </c>
@@ -2681,7 +2754,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>104</v>
       </c>
@@ -2710,7 +2783,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>105</v>
       </c>
@@ -2739,7 +2812,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>106</v>
       </c>
@@ -2768,7 +2841,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>107</v>
       </c>
@@ -2797,7 +2870,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>108</v>
       </c>
@@ -2826,7 +2899,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>109</v>
       </c>
@@ -2855,7 +2928,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>110</v>
       </c>
@@ -2884,7 +2957,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>111</v>
       </c>
@@ -2913,7 +2986,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>112</v>
       </c>
@@ -2955,14 +3028,14 @@
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="50.5703125" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.54296875" customWidth="1"/>
+    <col min="5" max="5" width="9.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2991,7 +3064,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>130</v>
       </c>
@@ -3020,7 +3093,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>154</v>
       </c>
@@ -3049,7 +3122,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>131</v>
       </c>
@@ -3078,7 +3151,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>132</v>
       </c>
@@ -3107,7 +3180,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>133</v>
       </c>
@@ -3136,7 +3209,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>134</v>
       </c>
@@ -3165,7 +3238,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>135</v>
       </c>
@@ -3194,7 +3267,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>136</v>
       </c>
@@ -3223,7 +3296,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>137</v>
       </c>
@@ -3252,7 +3325,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>138</v>
       </c>
@@ -3281,7 +3354,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>139</v>
       </c>
@@ -3310,7 +3383,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>140</v>
       </c>
@@ -3339,7 +3412,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>141</v>
       </c>
@@ -3368,7 +3441,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>142</v>
       </c>
@@ -3397,7 +3470,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>143</v>
       </c>
@@ -3426,7 +3499,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>144</v>
       </c>
@@ -3455,7 +3528,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>145</v>
       </c>
@@ -3484,7 +3557,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>146</v>
       </c>
@@ -3513,7 +3586,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>147</v>
       </c>
@@ -3542,7 +3615,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>148</v>
       </c>
@@ -3571,7 +3644,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>149</v>
       </c>
@@ -3600,7 +3673,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>150</v>
       </c>
@@ -3629,7 +3702,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>151</v>
       </c>
@@ -3658,7 +3731,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>152</v>
       </c>
@@ -3700,17 +3773,17 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.54296875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3745,7 +3818,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>188</v>
       </c>
@@ -3780,7 +3853,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>213</v>
       </c>
@@ -3815,7 +3888,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>269</v>
       </c>
@@ -3850,7 +3923,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>212</v>
       </c>
@@ -3885,7 +3958,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>214</v>
       </c>
@@ -3920,7 +3993,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>215</v>
       </c>
@@ -3955,7 +4028,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>216</v>
       </c>
@@ -3990,7 +4063,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>217</v>
       </c>
@@ -4025,7 +4098,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>218</v>
       </c>
@@ -4060,7 +4133,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>226</v>
       </c>
@@ -4095,7 +4168,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>227</v>
       </c>
@@ -4130,7 +4203,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>231</v>
       </c>
@@ -4165,7 +4238,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>238</v>
       </c>
@@ -4200,7 +4273,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>244</v>
       </c>
@@ -4235,7 +4308,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>240</v>
       </c>
@@ -4270,7 +4343,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>273</v>
       </c>
@@ -4305,7 +4378,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>253</v>
       </c>
@@ -4340,7 +4413,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>270</v>
       </c>
@@ -4376,15 +4449,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA629D80-511C-42AD-ACB3-22237E3BD282}">
-  <dimension ref="A1:B67"/>
+  <dimension ref="A1:B69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4392,7 +4465,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -4400,7 +4473,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -4408,7 +4481,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -4416,7 +4489,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -4424,7 +4497,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -4432,7 +4505,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -4440,7 +4513,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -4448,7 +4521,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -4456,7 +4529,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>274</v>
       </c>
@@ -4464,7 +4537,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -4472,7 +4545,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -4480,7 +4553,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -4488,7 +4561,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -4496,7 +4569,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>58</v>
       </c>
@@ -4504,7 +4577,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>62</v>
       </c>
@@ -4512,7 +4585,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>63</v>
       </c>
@@ -4520,7 +4593,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>73</v>
       </c>
@@ -4528,7 +4601,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>78</v>
       </c>
@@ -4536,7 +4609,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>69</v>
       </c>
@@ -4544,7 +4617,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>71</v>
       </c>
@@ -4552,7 +4625,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>67</v>
       </c>
@@ -4560,7 +4633,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>66</v>
       </c>
@@ -4568,7 +4641,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>75</v>
       </c>
@@ -4576,7 +4649,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>102</v>
       </c>
@@ -4584,7 +4657,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>103</v>
       </c>
@@ -4592,7 +4665,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>104</v>
       </c>
@@ -4600,7 +4673,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>105</v>
       </c>
@@ -4608,7 +4681,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>106</v>
       </c>
@@ -4616,7 +4689,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>107</v>
       </c>
@@ -4624,7 +4697,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>108</v>
       </c>
@@ -4632,7 +4705,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>109</v>
       </c>
@@ -4640,7 +4713,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>110</v>
       </c>
@@ -4648,7 +4721,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>111</v>
       </c>
@@ -4656,7 +4729,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>129</v>
       </c>
@@ -4664,7 +4737,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>130</v>
       </c>
@@ -4672,7 +4745,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>154</v>
       </c>
@@ -4680,7 +4753,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>131</v>
       </c>
@@ -4688,7 +4761,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>146</v>
       </c>
@@ -4696,7 +4769,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>147</v>
       </c>
@@ -4704,7 +4777,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>148</v>
       </c>
@@ -4712,7 +4785,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>149</v>
       </c>
@@ -4720,7 +4793,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>150</v>
       </c>
@@ -4728,7 +4801,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>151</v>
       </c>
@@ -4736,7 +4809,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>152</v>
       </c>
@@ -4744,7 +4817,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>185</v>
       </c>
@@ -4752,7 +4825,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>188</v>
       </c>
@@ -4760,7 +4833,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>213</v>
       </c>
@@ -4768,7 +4841,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>192</v>
       </c>
@@ -4776,7 +4849,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>269</v>
       </c>
@@ -4784,7 +4857,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>212</v>
       </c>
@@ -4792,7 +4865,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>214</v>
       </c>
@@ -4800,7 +4873,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>215</v>
       </c>
@@ -4808,7 +4881,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>216</v>
       </c>
@@ -4816,7 +4889,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>217</v>
       </c>
@@ -4824,7 +4897,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>218</v>
       </c>
@@ -4832,7 +4905,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>230</v>
       </c>
@@ -4840,7 +4913,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>231</v>
       </c>
@@ -4848,7 +4921,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>235</v>
       </c>
@@ -4856,7 +4929,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>244</v>
       </c>
@@ -4864,7 +4937,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>31</v>
       </c>
@@ -4872,7 +4945,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>258</v>
       </c>
@@ -4880,7 +4953,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>262</v>
       </c>
@@ -4888,7 +4961,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>267</v>
       </c>
@@ -4896,7 +4969,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>253</v>
       </c>
@@ -4904,7 +4977,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>101</v>
       </c>
@@ -4912,12 +4985,28 @@
         <v>259</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>270</v>
       </c>
       <c r="B67" t="s">
         <v>252</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>276</v>
+      </c>
+      <c r="B68" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>279</v>
+      </c>
+      <c r="B69" t="s">
+        <v>278</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed accounting and changed assumptions
Fixed the transport emission taxation.

Changed assumptions on speed of uptake.

Added a switch to include indirect emissions to the CBAM or not.

Additional demand is now allocated based on export shares and delivery cost to the importing region.
</commit_message>
<xml_diff>
--- a/Inputs/_MasterFiles/FTT_variables.xlsx
+++ b/Inputs/_MasterFiles/FTT_variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cambridgeeconometrics-my.sharepoint.com/personal/pv_camecon_com/Documents/Documents/GitHub/NH3_Trade_Laptop/Inputs/_MasterFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cambridgeeconometrics-my.sharepoint.com/personal/pv_camecon_com/Documents/Documents/GitHub/NH3_trade/Inputs/_MasterFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{62A0F244-D621-4931-9BF9-28DFD2CA0B35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87886238-37D6-40ED-8049-54BEF71D0702}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{62A0F244-D621-4931-9BF9-28DFD2CA0B35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{321C108C-84E4-4E02-BAF9-D3CFB193AB47}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FTT-P" sheetId="1" r:id="rId1"/>
@@ -1620,19 +1620,19 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="12.81640625" customWidth="1"/>
-    <col min="7" max="7" width="14.453125" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1661,12 +1661,12 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <v>31010000</v>
@@ -1690,12 +1690,12 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>58</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>31020000</v>
@@ -1719,12 +1719,12 @@
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>62</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>31030000</v>
@@ -1748,12 +1748,12 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>63</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5">
         <v>31040000</v>
@@ -1777,12 +1777,12 @@
         <v>292</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>74</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6">
         <v>31050000</v>
@@ -1806,12 +1806,12 @@
         <v>293</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>84</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7">
         <v>31060000</v>
@@ -1835,7 +1835,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -1864,12 +1864,12 @@
         <v>292</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>79</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9">
         <v>31090000</v>
@@ -1893,12 +1893,12 @@
         <v>293</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>70</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10">
         <v>31100000</v>
@@ -1922,12 +1922,12 @@
         <v>293</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>72</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11">
         <v>31110000</v>
@@ -1951,12 +1951,12 @@
         <v>293</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>68</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12">
         <v>31120000</v>
@@ -1980,12 +1980,12 @@
         <v>293</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>81</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13">
         <v>31130000</v>
@@ -2009,12 +2009,12 @@
         <v>292</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>88</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14">
         <v>31140000</v>
@@ -2038,12 +2038,12 @@
         <v>292</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>90</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15">
         <v>31150000</v>
@@ -2067,12 +2067,12 @@
         <v>292</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>80</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16">
         <v>31180000</v>
@@ -2096,12 +2096,12 @@
         <v>292</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>82</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17">
         <v>31190000</v>
@@ -2125,12 +2125,12 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>66</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18">
         <v>31200000</v>
@@ -2154,12 +2154,12 @@
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>76</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19">
         <v>31210000</v>
@@ -2202,14 +2202,14 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.54296875" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2238,7 +2238,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2267,7 +2267,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2296,7 +2296,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -2325,7 +2325,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2354,7 +2354,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -2383,7 +2383,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -2412,7 +2412,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -2441,7 +2441,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -2470,7 +2470,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -2499,7 +2499,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -2528,7 +2528,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -2557,7 +2557,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -2586,7 +2586,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -2615,7 +2615,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -2644,7 +2644,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -2673,7 +2673,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -2702,7 +2702,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -2731,7 +2731,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -2760,7 +2760,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -2789,7 +2789,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -2818,7 +2818,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>52</v>
       </c>
@@ -2858,13 +2858,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.453125" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2893,7 +2893,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>96</v>
       </c>
@@ -2922,7 +2922,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>99</v>
       </c>
@@ -2951,7 +2951,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>100</v>
       </c>
@@ -2980,7 +2980,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>101</v>
       </c>
@@ -3009,7 +3009,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>102</v>
       </c>
@@ -3038,7 +3038,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>103</v>
       </c>
@@ -3067,7 +3067,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>104</v>
       </c>
@@ -3096,7 +3096,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>105</v>
       </c>
@@ -3125,7 +3125,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>106</v>
       </c>
@@ -3154,7 +3154,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>107</v>
       </c>
@@ -3183,7 +3183,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>108</v>
       </c>
@@ -3212,7 +3212,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>109</v>
       </c>
@@ -3241,7 +3241,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>110</v>
       </c>
@@ -3270,7 +3270,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>111</v>
       </c>
@@ -3299,7 +3299,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>112</v>
       </c>
@@ -3328,7 +3328,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>113</v>
       </c>
@@ -3370,14 +3370,14 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="50.54296875" customWidth="1"/>
-    <col min="5" max="5" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.5703125" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3406,7 +3406,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>131</v>
       </c>
@@ -3435,7 +3435,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>155</v>
       </c>
@@ -3464,7 +3464,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>132</v>
       </c>
@@ -3493,7 +3493,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>133</v>
       </c>
@@ -3522,7 +3522,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>134</v>
       </c>
@@ -3551,7 +3551,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>135</v>
       </c>
@@ -3580,7 +3580,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>136</v>
       </c>
@@ -3609,7 +3609,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>137</v>
       </c>
@@ -3638,7 +3638,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>138</v>
       </c>
@@ -3667,7 +3667,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>139</v>
       </c>
@@ -3696,7 +3696,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>140</v>
       </c>
@@ -3725,7 +3725,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>141</v>
       </c>
@@ -3754,7 +3754,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>142</v>
       </c>
@@ -3783,7 +3783,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>143</v>
       </c>
@@ -3812,7 +3812,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>144</v>
       </c>
@@ -3841,7 +3841,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>145</v>
       </c>
@@ -3870,7 +3870,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>146</v>
       </c>
@@ -3899,7 +3899,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>147</v>
       </c>
@@ -3928,7 +3928,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>148</v>
       </c>
@@ -3957,7 +3957,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>149</v>
       </c>
@@ -3986,7 +3986,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>150</v>
       </c>
@@ -4015,7 +4015,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>151</v>
       </c>
@@ -4044,7 +4044,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>152</v>
       </c>
@@ -4073,7 +4073,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>153</v>
       </c>
@@ -4115,17 +4115,17 @@
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4160,7 +4160,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>186</v>
       </c>
@@ -4195,7 +4195,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>189</v>
       </c>
@@ -4230,7 +4230,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>220</v>
       </c>
@@ -4265,7 +4265,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>195</v>
       </c>
@@ -4300,7 +4300,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>198</v>
       </c>
@@ -4335,7 +4335,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>219</v>
       </c>
@@ -4370,7 +4370,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>221</v>
       </c>
@@ -4405,7 +4405,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>222</v>
       </c>
@@ -4440,7 +4440,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>223</v>
       </c>
@@ -4475,7 +4475,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>224</v>
       </c>
@@ -4510,7 +4510,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>225</v>
       </c>
@@ -4545,7 +4545,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>215</v>
       </c>
@@ -4580,7 +4580,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>229</v>
       </c>
@@ -4612,7 +4612,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>231</v>
       </c>
@@ -4644,7 +4644,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>238</v>
       </c>
@@ -4679,7 +4679,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>239</v>
       </c>
@@ -4714,7 +4714,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>242</v>
       </c>
@@ -4749,7 +4749,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>248</v>
       </c>
@@ -4784,7 +4784,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>250</v>
       </c>
@@ -4819,7 +4819,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>254</v>
       </c>
@@ -4854,7 +4854,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>258</v>
       </c>
@@ -4889,7 +4889,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>264</v>
       </c>
@@ -4924,7 +4924,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>270</v>
       </c>
@@ -4959,7 +4959,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>266</v>
       </c>
@@ -4994,7 +4994,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>276</v>
       </c>
@@ -5029,7 +5029,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>281</v>
       </c>
@@ -5077,9 +5077,9 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5108,7 +5108,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>297</v>
       </c>
@@ -5137,7 +5137,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>319</v>
       </c>
@@ -5166,7 +5166,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>298</v>
       </c>
@@ -5195,7 +5195,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>304</v>
       </c>
@@ -5234,16 +5234,16 @@
   <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="19.26953125" customWidth="1"/>
-    <col min="4" max="4" width="39.54296875" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="39.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5272,7 +5272,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>307</v>
       </c>
@@ -5301,7 +5301,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>308</v>
       </c>
@@ -5330,7 +5330,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>310</v>
       </c>
@@ -5359,7 +5359,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>311</v>
       </c>
@@ -5388,7 +5388,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>321</v>
       </c>
@@ -5417,7 +5417,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>309</v>
       </c>
@@ -5446,7 +5446,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>324</v>
       </c>
@@ -5475,7 +5475,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>325</v>
       </c>
@@ -5504,7 +5504,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>326</v>
       </c>
@@ -5533,7 +5533,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>327</v>
       </c>
@@ -5562,7 +5562,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>328</v>
       </c>
@@ -5591,7 +5591,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>329</v>
       </c>
@@ -5620,7 +5620,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>330</v>
       </c>
@@ -5649,7 +5649,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>331</v>
       </c>
@@ -5678,7 +5678,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>332</v>
       </c>
@@ -5707,7 +5707,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>333</v>
       </c>
@@ -5736,7 +5736,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>334</v>
       </c>
@@ -5765,7 +5765,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>335</v>
       </c>
@@ -5794,7 +5794,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>336</v>
       </c>
@@ -5823,7 +5823,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>337</v>
       </c>
@@ -5852,7 +5852,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>338</v>
       </c>
@@ -5881,7 +5881,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>354</v>
       </c>
@@ -5910,7 +5910,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>355</v>
       </c>
@@ -5939,7 +5939,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>356</v>
       </c>
@@ -5968,7 +5968,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>361</v>
       </c>
@@ -5997,7 +5997,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>362</v>
       </c>
@@ -6026,7 +6026,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>363</v>
       </c>
@@ -6055,7 +6055,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>364</v>
       </c>
@@ -6084,7 +6084,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>365</v>
       </c>
@@ -6113,7 +6113,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>371</v>
       </c>
@@ -6142,7 +6142,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>372</v>
       </c>
@@ -6171,7 +6171,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>373</v>
       </c>
@@ -6200,7 +6200,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>374</v>
       </c>
@@ -6229,7 +6229,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>378</v>
       </c>
@@ -6258,7 +6258,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>380</v>
       </c>
@@ -6287,7 +6287,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>381</v>
       </c>
@@ -6316,7 +6316,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>382</v>
       </c>
@@ -6345,7 +6345,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>383</v>
       </c>
@@ -6374,7 +6374,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>384</v>
       </c>
@@ -6403,7 +6403,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>385</v>
       </c>
@@ -6432,7 +6432,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>386</v>
       </c>
@@ -6461,7 +6461,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>387</v>
       </c>
@@ -6490,7 +6490,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>388</v>
       </c>
@@ -6519,7 +6519,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>399</v>
       </c>
@@ -6548,7 +6548,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>400</v>
       </c>
@@ -6577,7 +6577,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>401</v>
       </c>
@@ -6620,9 +6620,9 @@
       <selection activeCell="B111" sqref="B111"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6630,7 +6630,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -6638,7 +6638,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -6646,7 +6646,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -6654,7 +6654,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -6662,7 +6662,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -6670,7 +6670,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -6678,7 +6678,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -6686,7 +6686,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -6694,7 +6694,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -6702,7 +6702,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -6710,7 +6710,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -6718,7 +6718,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -6726,7 +6726,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>58</v>
       </c>
@@ -6734,7 +6734,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>62</v>
       </c>
@@ -6742,7 +6742,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>63</v>
       </c>
@@ -6750,7 +6750,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>74</v>
       </c>
@@ -6758,7 +6758,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>79</v>
       </c>
@@ -6766,7 +6766,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>70</v>
       </c>
@@ -6774,7 +6774,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>72</v>
       </c>
@@ -6782,7 +6782,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>68</v>
       </c>
@@ -6790,7 +6790,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>66</v>
       </c>
@@ -6798,7 +6798,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>76</v>
       </c>
@@ -6806,7 +6806,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>103</v>
       </c>
@@ -6814,7 +6814,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>104</v>
       </c>
@@ -6822,7 +6822,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>105</v>
       </c>
@@ -6830,7 +6830,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>106</v>
       </c>
@@ -6838,7 +6838,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>107</v>
       </c>
@@ -6846,7 +6846,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>108</v>
       </c>
@@ -6854,7 +6854,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>109</v>
       </c>
@@ -6862,7 +6862,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>110</v>
       </c>
@@ -6870,7 +6870,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>111</v>
       </c>
@@ -6878,7 +6878,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>112</v>
       </c>
@@ -6886,7 +6886,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>130</v>
       </c>
@@ -6894,7 +6894,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>131</v>
       </c>
@@ -6902,7 +6902,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>155</v>
       </c>
@@ -6910,7 +6910,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>132</v>
       </c>
@@ -6918,7 +6918,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>147</v>
       </c>
@@ -6926,7 +6926,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>148</v>
       </c>
@@ -6934,7 +6934,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>149</v>
       </c>
@@ -6942,7 +6942,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>150</v>
       </c>
@@ -6950,7 +6950,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>151</v>
       </c>
@@ -6958,7 +6958,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>152</v>
       </c>
@@ -6966,7 +6966,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>153</v>
       </c>
@@ -6974,7 +6974,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>186</v>
       </c>
@@ -6982,7 +6982,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>189</v>
       </c>
@@ -6990,7 +6990,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>220</v>
       </c>
@@ -6998,7 +6998,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>195</v>
       </c>
@@ -7006,7 +7006,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>198</v>
       </c>
@@ -7014,7 +7014,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>219</v>
       </c>
@@ -7022,7 +7022,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>221</v>
       </c>
@@ -7030,7 +7030,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>222</v>
       </c>
@@ -7038,7 +7038,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>223</v>
       </c>
@@ -7046,7 +7046,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>224</v>
       </c>
@@ -7054,7 +7054,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>225</v>
       </c>
@@ -7062,7 +7062,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>215</v>
       </c>
@@ -7070,7 +7070,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>248</v>
       </c>
@@ -7078,7 +7078,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>250</v>
       </c>
@@ -7086,7 +7086,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>254</v>
       </c>
@@ -7094,7 +7094,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>270</v>
       </c>
@@ -7102,7 +7102,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>31</v>
       </c>
@@ -7110,7 +7110,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>286</v>
       </c>
@@ -7118,7 +7118,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>290</v>
       </c>
@@ -7126,7 +7126,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>295</v>
       </c>
@@ -7134,7 +7134,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>281</v>
       </c>
@@ -7142,7 +7142,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>102</v>
       </c>
@@ -7150,7 +7150,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>297</v>
       </c>
@@ -7158,7 +7158,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>319</v>
       </c>
@@ -7166,7 +7166,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>304</v>
       </c>
@@ -7174,7 +7174,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>308</v>
       </c>
@@ -7182,7 +7182,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>311</v>
       </c>
@@ -7190,7 +7190,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>321</v>
       </c>
@@ -7198,7 +7198,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>309</v>
       </c>
@@ -7206,7 +7206,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>324</v>
       </c>
@@ -7214,7 +7214,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>325</v>
       </c>
@@ -7222,7 +7222,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>326</v>
       </c>
@@ -7230,7 +7230,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>327</v>
       </c>
@@ -7238,7 +7238,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>328</v>
       </c>
@@ -7246,7 +7246,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>329</v>
       </c>
@@ -7254,7 +7254,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>330</v>
       </c>
@@ -7262,7 +7262,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>331</v>
       </c>
@@ -7270,7 +7270,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>332</v>
       </c>
@@ -7278,7 +7278,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>333</v>
       </c>
@@ -7286,7 +7286,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>334</v>
       </c>
@@ -7294,7 +7294,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>335</v>
       </c>
@@ -7302,7 +7302,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>336</v>
       </c>
@@ -7310,7 +7310,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>338</v>
       </c>
@@ -7318,7 +7318,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>354</v>
       </c>
@@ -7326,7 +7326,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>355</v>
       </c>
@@ -7334,7 +7334,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>356</v>
       </c>
@@ -7342,7 +7342,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>361</v>
       </c>
@@ -7350,7 +7350,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>362</v>
       </c>
@@ -7358,7 +7358,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>363</v>
       </c>
@@ -7366,7 +7366,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>364</v>
       </c>
@@ -7374,7 +7374,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>365</v>
       </c>
@@ -7382,7 +7382,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>371</v>
       </c>
@@ -7390,7 +7390,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>372</v>
       </c>
@@ -7398,7 +7398,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>373</v>
       </c>
@@ -7406,7 +7406,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>374</v>
       </c>
@@ -7414,7 +7414,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>378</v>
       </c>
@@ -7422,7 +7422,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>380</v>
       </c>
@@ -7430,7 +7430,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>381</v>
       </c>
@@ -7438,7 +7438,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>382</v>
       </c>
@@ -7446,7 +7446,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>383</v>
       </c>
@@ -7454,7 +7454,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>384</v>
       </c>
@@ -7462,7 +7462,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>385</v>
       </c>
@@ -7470,7 +7470,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>386</v>
       </c>
@@ -7478,7 +7478,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>387</v>
       </c>
@@ -7486,7 +7486,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>388</v>
       </c>
@@ -7494,7 +7494,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>399</v>
       </c>

</xml_diff>